<commit_message>
set cellstyle from column default
</commit_message>
<xml_diff>
--- a/X-Domestic Standard Upload.xlsx
+++ b/X-Domestic Standard Upload.xlsx
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="534">
   <si>
     <t>#</t>
   </si>
@@ -1156,114 +1156,6 @@
     <t>col:4</t>
   </si>
   <si>
-    <t>col:5</t>
-  </si>
-  <si>
-    <t>col:6</t>
-  </si>
-  <si>
-    <t>col:7</t>
-  </si>
-  <si>
-    <t>col:8</t>
-  </si>
-  <si>
-    <t>col:9</t>
-  </si>
-  <si>
-    <t>col:10</t>
-  </si>
-  <si>
-    <t>col:11</t>
-  </si>
-  <si>
-    <t>col:12</t>
-  </si>
-  <si>
-    <t>col:13</t>
-  </si>
-  <si>
-    <t>col:14</t>
-  </si>
-  <si>
-    <t>col:15</t>
-  </si>
-  <si>
-    <t>col:16</t>
-  </si>
-  <si>
-    <t>col:17</t>
-  </si>
-  <si>
-    <t>col:18</t>
-  </si>
-  <si>
-    <t>col:19</t>
-  </si>
-  <si>
-    <t>col:20</t>
-  </si>
-  <si>
-    <t>col:21</t>
-  </si>
-  <si>
-    <t>col:22</t>
-  </si>
-  <si>
-    <t>col:23</t>
-  </si>
-  <si>
-    <t>col:24</t>
-  </si>
-  <si>
-    <t>col:25</t>
-  </si>
-  <si>
-    <t>col:26</t>
-  </si>
-  <si>
-    <t>col:27</t>
-  </si>
-  <si>
-    <t>col:28</t>
-  </si>
-  <si>
-    <t>col:29</t>
-  </si>
-  <si>
-    <t>col:30</t>
-  </si>
-  <si>
-    <t>col:31</t>
-  </si>
-  <si>
-    <t>col:32</t>
-  </si>
-  <si>
-    <t>col:33</t>
-  </si>
-  <si>
-    <t>col:34</t>
-  </si>
-  <si>
-    <t>col:35</t>
-  </si>
-  <si>
-    <t>col:36</t>
-  </si>
-  <si>
-    <t>col:37</t>
-  </si>
-  <si>
-    <t>col:38</t>
-  </si>
-  <si>
-    <t>col:39</t>
-  </si>
-  <si>
-    <t>col:40</t>
-  </si>
-  <si>
     <t>dep:0</t>
   </si>
   <si>
@@ -1276,51 +1168,6 @@
     <t>dep:3</t>
   </si>
   <si>
-    <t>dep:4</t>
-  </si>
-  <si>
-    <t>dep:5</t>
-  </si>
-  <si>
-    <t>dep:6</t>
-  </si>
-  <si>
-    <t>dep:7</t>
-  </si>
-  <si>
-    <t>dep:8</t>
-  </si>
-  <si>
-    <t>dep:9</t>
-  </si>
-  <si>
-    <t>dep:10</t>
-  </si>
-  <si>
-    <t>dep:11</t>
-  </si>
-  <si>
-    <t>dep:12</t>
-  </si>
-  <si>
-    <t>dep:13</t>
-  </si>
-  <si>
-    <t>dep:14</t>
-  </si>
-  <si>
-    <t>dep:15</t>
-  </si>
-  <si>
-    <t>dep:16</t>
-  </si>
-  <si>
-    <t>dep:17</t>
-  </si>
-  <si>
-    <t>dep:18</t>
-  </si>
-  <si>
     <t>siz:0</t>
   </si>
   <si>
@@ -1351,30 +1198,153 @@
     <t>siz:9</t>
   </si>
   <si>
-    <t>siz:10</t>
-  </si>
-  <si>
-    <t>siz:11</t>
-  </si>
-  <si>
-    <t>siz:12</t>
-  </si>
-  <si>
-    <t>siz:13</t>
-  </si>
-  <si>
-    <t>siz:14</t>
-  </si>
-  <si>
-    <t>siz:15</t>
-  </si>
-  <si>
     <t>typ:0</t>
   </si>
   <si>
     <t>typ:1</t>
   </si>
   <si>
+    <t>typ:2</t>
+  </si>
+  <si>
+    <t>typ:3</t>
+  </si>
+  <si>
+    <t>typ:4</t>
+  </si>
+  <si>
+    <t>typ:5</t>
+  </si>
+  <si>
+    <t>typ:6</t>
+  </si>
+  <si>
+    <t>typ:7</t>
+  </si>
+  <si>
+    <t>typ:8</t>
+  </si>
+  <si>
+    <t>typ:9</t>
+  </si>
+  <si>
+    <t>typ:10</t>
+  </si>
+  <si>
+    <t>typ:11</t>
+  </si>
+  <si>
+    <t>typ:12</t>
+  </si>
+  <si>
+    <t>typ:13</t>
+  </si>
+  <si>
+    <t>typ:14</t>
+  </si>
+  <si>
+    <t>typ:15</t>
+  </si>
+  <si>
+    <t>typ:16</t>
+  </si>
+  <si>
+    <t>typ:17</t>
+  </si>
+  <si>
+    <t>typ:18</t>
+  </si>
+  <si>
+    <t>typ:19</t>
+  </si>
+  <si>
+    <t>typ:20</t>
+  </si>
+  <si>
+    <t>typ:21</t>
+  </si>
+  <si>
+    <t>typ:22</t>
+  </si>
+  <si>
+    <t>typ:23</t>
+  </si>
+  <si>
+    <t>typ:24</t>
+  </si>
+  <si>
+    <t>typ:25</t>
+  </si>
+  <si>
+    <t>typ:26</t>
+  </si>
+  <si>
+    <t>typ:27</t>
+  </si>
+  <si>
+    <t>typ:28</t>
+  </si>
+  <si>
+    <t>typ:29</t>
+  </si>
+  <si>
+    <t>typ:30</t>
+  </si>
+  <si>
+    <t>typ:31</t>
+  </si>
+  <si>
+    <t>typ:32</t>
+  </si>
+  <si>
+    <t>typ:33</t>
+  </si>
+  <si>
+    <t>typ:34</t>
+  </si>
+  <si>
+    <t>typ:35</t>
+  </si>
+  <si>
+    <t>typ:36</t>
+  </si>
+  <si>
+    <t>typ:37</t>
+  </si>
+  <si>
+    <t>typ:38</t>
+  </si>
+  <si>
+    <t>typ:39</t>
+  </si>
+  <si>
+    <t>typ:40</t>
+  </si>
+  <si>
+    <t>typ:41</t>
+  </si>
+  <si>
+    <t>typ:42</t>
+  </si>
+  <si>
+    <t>typ:43</t>
+  </si>
+  <si>
+    <t>typ:44</t>
+  </si>
+  <si>
+    <t>typ:45</t>
+  </si>
+  <si>
+    <t>typ:46</t>
+  </si>
+  <si>
+    <t>typ:47</t>
+  </si>
+  <si>
+    <t>typ:48</t>
+  </si>
+  <si>
     <t>mat:0</t>
   </si>
   <si>
@@ -1495,24 +1465,6 @@
     <t>mat:39</t>
   </si>
   <si>
-    <t>mat:40</t>
-  </si>
-  <si>
-    <t>mat:41</t>
-  </si>
-  <si>
-    <t>mat:42</t>
-  </si>
-  <si>
-    <t>mat:43</t>
-  </si>
-  <si>
-    <t>mat:44</t>
-  </si>
-  <si>
-    <t>mat:45</t>
-  </si>
-  <si>
     <t>vpn:0</t>
   </si>
   <si>
@@ -1624,36 +1576,6 @@
     <t>vpn:36</t>
   </si>
   <si>
-    <t>vpn:37</t>
-  </si>
-  <si>
-    <t>vpn:38</t>
-  </si>
-  <si>
-    <t>vpn:39</t>
-  </si>
-  <si>
-    <t>vpn:40</t>
-  </si>
-  <si>
-    <t>vpn:41</t>
-  </si>
-  <si>
-    <t>vpn:42</t>
-  </si>
-  <si>
-    <t>vpn:43</t>
-  </si>
-  <si>
-    <t>vpn:44</t>
-  </si>
-  <si>
-    <t>vpn:45</t>
-  </si>
-  <si>
-    <t>vpn:46</t>
-  </si>
-  <si>
     <t>sup:0</t>
   </si>
   <si>
@@ -1789,120 +1711,6 @@
     <t>cat:11</t>
   </si>
   <si>
-    <t>cat:12</t>
-  </si>
-  <si>
-    <t>cat:13</t>
-  </si>
-  <si>
-    <t>cat:14</t>
-  </si>
-  <si>
-    <t>cat:15</t>
-  </si>
-  <si>
-    <t>cat:16</t>
-  </si>
-  <si>
-    <t>cat:17</t>
-  </si>
-  <si>
-    <t>cat:18</t>
-  </si>
-  <si>
-    <t>cat:19</t>
-  </si>
-  <si>
-    <t>cat:20</t>
-  </si>
-  <si>
-    <t>cat:21</t>
-  </si>
-  <si>
-    <t>cat:22</t>
-  </si>
-  <si>
-    <t>cat:23</t>
-  </si>
-  <si>
-    <t>cat:24</t>
-  </si>
-  <si>
-    <t>cat:25</t>
-  </si>
-  <si>
-    <t>cat:26</t>
-  </si>
-  <si>
-    <t>cat:27</t>
-  </si>
-  <si>
-    <t>cat:28</t>
-  </si>
-  <si>
-    <t>cat:29</t>
-  </si>
-  <si>
-    <t>cat:30</t>
-  </si>
-  <si>
-    <t>cat:31</t>
-  </si>
-  <si>
-    <t>cat:32</t>
-  </si>
-  <si>
-    <t>cat:33</t>
-  </si>
-  <si>
-    <t>cat:34</t>
-  </si>
-  <si>
-    <t>cat:35</t>
-  </si>
-  <si>
-    <t>cat:36</t>
-  </si>
-  <si>
-    <t>cat:37</t>
-  </si>
-  <si>
-    <t>cat:38</t>
-  </si>
-  <si>
-    <t>cat:39</t>
-  </si>
-  <si>
-    <t>cat:40</t>
-  </si>
-  <si>
-    <t>cat:41</t>
-  </si>
-  <si>
-    <t>cat:42</t>
-  </si>
-  <si>
-    <t>cat:43</t>
-  </si>
-  <si>
-    <t>cat:44</t>
-  </si>
-  <si>
-    <t>cat:45</t>
-  </si>
-  <si>
-    <t>cat:46</t>
-  </si>
-  <si>
-    <t>cat:47</t>
-  </si>
-  <si>
-    <t>cat:48</t>
-  </si>
-  <si>
-    <t>cat:49</t>
-  </si>
-  <si>
     <t>ven:0</t>
   </si>
   <si>
@@ -2047,39 +1855,18 @@
     <t>ven:47</t>
   </si>
   <si>
+    <t>ven:48</t>
+  </si>
+  <si>
+    <t>ven:49</t>
+  </si>
+  <si>
     <t>lab:0</t>
   </si>
   <si>
     <t>lab:1</t>
   </si>
   <si>
-    <t>lab:2</t>
-  </si>
-  <si>
-    <t>lab:3</t>
-  </si>
-  <si>
-    <t>lab:4</t>
-  </si>
-  <si>
-    <t>lab:5</t>
-  </si>
-  <si>
-    <t>lab:6</t>
-  </si>
-  <si>
-    <t>lab:7</t>
-  </si>
-  <si>
-    <t>lab:8</t>
-  </si>
-  <si>
-    <t>lab:9</t>
-  </si>
-  <si>
-    <t>lab:10</t>
-  </si>
-  <si>
     <t>cla:0</t>
   </si>
   <si>
@@ -2113,39 +1900,6 @@
     <t>cla:10</t>
   </si>
   <si>
-    <t>cla:11</t>
-  </si>
-  <si>
-    <t>cla:12</t>
-  </si>
-  <si>
-    <t>cla:13</t>
-  </si>
-  <si>
-    <t>cla:14</t>
-  </si>
-  <si>
-    <t>cla:15</t>
-  </si>
-  <si>
-    <t>cla:16</t>
-  </si>
-  <si>
-    <t>cla:17</t>
-  </si>
-  <si>
-    <t>cla:18</t>
-  </si>
-  <si>
-    <t>cla:19</t>
-  </si>
-  <si>
-    <t>cla:20</t>
-  </si>
-  <si>
-    <t>cla:21</t>
-  </si>
-  <si>
     <t>pon:0</t>
   </si>
   <si>
@@ -2228,6 +1982,15 @@
   </si>
   <si>
     <t>pon:27</t>
+  </si>
+  <si>
+    <t>pon:28</t>
+  </si>
+  <si>
+    <t>pon:29</t>
+  </si>
+  <si>
+    <t>pon:30</t>
   </si>
 </sst>
 </file>
@@ -8063,1183 +7826,946 @@
       <c r="CV5" s="49"/>
     </row>
     <row r="6">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="36" t="s">
+        <v>358</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>440</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>490</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>503</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>395</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="K6" s="39" t="s">
+        <v>492</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>428</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="36" t="s">
+        <v>359</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>441</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>491</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>504</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>396</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="K7" s="39" t="s">
+        <v>493</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>429</v>
+      </c>
+      <c r="M7" s="39" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="36" t="s">
+        <v>360</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>442</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>505</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>397</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="K8" s="39" t="s">
+        <v>494</v>
+      </c>
+      <c r="L8" s="39" t="s">
+        <v>430</v>
+      </c>
+      <c r="M8" s="39" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="36" t="s">
+        <v>361</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>443</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>262</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>272</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>506</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>398</v>
+      </c>
+      <c r="J9" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="K9" s="39" t="s">
+        <v>495</v>
+      </c>
+      <c r="L9" s="39" t="s">
+        <v>431</v>
+      </c>
+      <c r="M9" s="39" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="36" t="s">
+        <v>362</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>444</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>263</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>507</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>399</v>
+      </c>
+      <c r="K10" s="39" t="s">
+        <v>496</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>432</v>
+      </c>
+      <c r="M10" s="39" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="36" t="s">
+        <v>363</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>445</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>264</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>508</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>400</v>
+      </c>
+      <c r="K11" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="L11" s="39" t="s">
+        <v>433</v>
+      </c>
+      <c r="M11" s="39" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>446</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>509</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="K12" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>434</v>
+      </c>
+      <c r="M12" s="39" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="36" t="s">
+        <v>365</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>447</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>510</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>402</v>
+      </c>
+      <c r="K13" s="39" t="s">
+        <v>499</v>
+      </c>
+      <c r="L13" s="39" t="s">
+        <v>435</v>
+      </c>
+      <c r="M13" s="39" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="36" t="s">
+        <v>366</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>448</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>267</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>511</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>403</v>
+      </c>
+      <c r="K14" s="39" t="s">
+        <v>500</v>
+      </c>
+      <c r="L14" s="39" t="s">
+        <v>436</v>
+      </c>
+      <c r="M14" s="39" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="36" t="s">
+        <v>367</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>449</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>278</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>512</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>404</v>
+      </c>
+      <c r="K15" s="39" t="s">
+        <v>501</v>
+      </c>
+      <c r="L15" s="39" t="s">
+        <v>437</v>
+      </c>
+      <c r="M15" s="39" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="36" t="s">
+        <v>368</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>450</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="H16" s="40" t="s">
+        <v>513</v>
+      </c>
+      <c r="I16" s="39" t="s">
+        <v>405</v>
+      </c>
+      <c r="K16" s="39" t="s">
+        <v>502</v>
+      </c>
+      <c r="L16" s="39" t="s">
+        <v>438</v>
+      </c>
+      <c r="M16" s="39" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="36" t="s">
+        <v>369</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>451</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="H17" s="40" t="s">
+        <v>514</v>
+      </c>
+      <c r="I17" s="39" t="s">
+        <v>406</v>
+      </c>
+      <c r="L17" s="39" t="s">
+        <v>439</v>
+      </c>
+      <c r="M17" s="39" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="36" t="s">
+        <v>370</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>452</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="H18" s="40" t="s">
+        <v>515</v>
+      </c>
+      <c r="I18" s="39" t="s">
+        <v>407</v>
+      </c>
+      <c r="M18" s="39" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="36" t="s">
+        <v>371</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>453</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>516</v>
+      </c>
+      <c r="I19" s="39" t="s">
+        <v>408</v>
+      </c>
+      <c r="M19" s="39" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="36" t="s">
+        <v>372</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>454</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="H20" s="40" t="s">
+        <v>517</v>
+      </c>
+      <c r="I20" s="39" t="s">
+        <v>409</v>
+      </c>
+      <c r="M20" s="39" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="36" t="s">
+        <v>373</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>455</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="H21" s="40" t="s">
+        <v>518</v>
+      </c>
+      <c r="I21" s="39" t="s">
+        <v>410</v>
+      </c>
+      <c r="M21" s="39" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="36" t="s">
         <v>374</v>
       </c>
-      <c r="C6" s="47" t="s">
-        <v>504</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>552</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>250</v>
-      </c>
-      <c r="F6" s="48" t="s">
+      <c r="C22" s="36" t="s">
+        <v>456</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>285</v>
+      </c>
+      <c r="H22" s="40" t="s">
+        <v>519</v>
+      </c>
+      <c r="I22" s="39" t="s">
+        <v>411</v>
+      </c>
+      <c r="M22" s="39" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>457</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>286</v>
+      </c>
+      <c r="H23" s="40" t="s">
+        <v>520</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>412</v>
+      </c>
+      <c r="M23" s="39" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="36" t="s">
+        <v>376</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>458</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>287</v>
+      </c>
+      <c r="H24" s="40" t="s">
+        <v>521</v>
+      </c>
+      <c r="I24" s="39" t="s">
+        <v>413</v>
+      </c>
+      <c r="M24" s="39" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>459</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>288</v>
+      </c>
+      <c r="H25" s="40" t="s">
+        <v>522</v>
+      </c>
+      <c r="I25" s="39" t="s">
+        <v>414</v>
+      </c>
+      <c r="M25" s="39" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="36" t="s">
+        <v>378</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>460</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>289</v>
+      </c>
+      <c r="H26" s="40" t="s">
+        <v>523</v>
+      </c>
+      <c r="I26" s="39" t="s">
+        <v>415</v>
+      </c>
+      <c r="M26" s="39" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="36" t="s">
+        <v>379</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>461</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>290</v>
+      </c>
+      <c r="H27" s="40" t="s">
+        <v>524</v>
+      </c>
+      <c r="I27" s="39" t="s">
+        <v>416</v>
+      </c>
+      <c r="M27" s="39" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="36" t="s">
+        <v>380</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>462</v>
+      </c>
+      <c r="G28" s="38" t="s">
+        <v>291</v>
+      </c>
+      <c r="H28" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="I28" s="39" t="s">
+        <v>417</v>
+      </c>
+      <c r="M28" s="39" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="36" t="s">
+        <v>381</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>463</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="H29" s="40" t="s">
+        <v>526</v>
+      </c>
+      <c r="I29" s="39" t="s">
+        <v>418</v>
+      </c>
+      <c r="M29" s="39" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" s="36" t="s">
+        <v>382</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>464</v>
+      </c>
+      <c r="G30" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="H30" s="40" t="s">
+        <v>527</v>
+      </c>
+      <c r="I30" s="39" t="s">
+        <v>419</v>
+      </c>
+      <c r="M30" s="39" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" s="36" t="s">
+        <v>383</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>465</v>
+      </c>
+      <c r="G31" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>528</v>
+      </c>
+      <c r="I31" s="39" t="s">
+        <v>420</v>
+      </c>
+      <c r="M31" s="39" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" s="36" t="s">
+        <v>384</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>466</v>
+      </c>
+      <c r="G32" s="38" t="s">
+        <v>295</v>
+      </c>
+      <c r="H32" s="40" t="s">
+        <v>529</v>
+      </c>
+      <c r="I32" s="39" t="s">
+        <v>421</v>
+      </c>
+      <c r="M32" s="39" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" s="36" t="s">
+        <v>385</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>467</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="H33" s="40" t="s">
+        <v>530</v>
+      </c>
+      <c r="I33" s="39" t="s">
+        <v>422</v>
+      </c>
+      <c r="M33" s="39" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" s="36" t="s">
+        <v>386</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>468</v>
+      </c>
+      <c r="G34" s="38" t="s">
+        <v>297</v>
+      </c>
+      <c r="H34" s="40" t="s">
+        <v>531</v>
+      </c>
+      <c r="I34" s="39" t="s">
+        <v>423</v>
+      </c>
+      <c r="M34" s="39" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" s="36" t="s">
+        <v>387</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>469</v>
+      </c>
+      <c r="G35" s="38" t="s">
+        <v>298</v>
+      </c>
+      <c r="H35" s="40" t="s">
+        <v>532</v>
+      </c>
+      <c r="I35" s="39" t="s">
+        <v>424</v>
+      </c>
+      <c r="M35" s="39" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" s="36" t="s">
+        <v>388</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>470</v>
+      </c>
+      <c r="G36" s="38" t="s">
+        <v>299</v>
+      </c>
+      <c r="H36" s="40" t="s">
+        <v>533</v>
+      </c>
+      <c r="I36" s="39" t="s">
+        <v>425</v>
+      </c>
+      <c r="M36" s="39" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="36" t="s">
+        <v>389</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>471</v>
+      </c>
+      <c r="G37" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="I37" s="39" t="s">
+        <v>426</v>
+      </c>
+      <c r="M37" s="39" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="C38" s="36" t="s">
+        <v>472</v>
+      </c>
+      <c r="G38" s="38" t="s">
+        <v>301</v>
+      </c>
+      <c r="I38" s="39" t="s">
+        <v>427</v>
+      </c>
+      <c r="M38" s="39" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>473</v>
+      </c>
+      <c r="G39" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="M39" s="39" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" s="36" t="s">
+        <v>392</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>474</v>
+      </c>
+      <c r="G40" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="M40" s="39" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" s="36" t="s">
+        <v>393</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>475</v>
+      </c>
+      <c r="G41" s="38" t="s">
+        <v>304</v>
+      </c>
+      <c r="M41" s="39" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" s="36" t="s">
+        <v>394</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>476</v>
+      </c>
+      <c r="G42" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="M42" s="39" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" s="36" t="s">
+        <v>477</v>
+      </c>
+      <c r="G43" s="38" t="s">
+        <v>306</v>
+      </c>
+      <c r="M43" s="39" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" s="36" t="s">
+        <v>478</v>
+      </c>
+      <c r="G44" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="M44" s="39" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="C45" s="36" t="s">
+        <v>479</v>
+      </c>
+      <c r="G45" s="38" t="s">
+        <v>308</v>
+      </c>
+      <c r="M45" s="39" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" s="36" t="s">
+        <v>480</v>
+      </c>
+      <c r="G46" s="38" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="C47" s="36" t="s">
+        <v>481</v>
+      </c>
+      <c r="G47" s="38" t="s">
         <v>310</v>
       </c>
-      <c r="G6" s="49" t="s">
-        <v>326</v>
-      </c>
-      <c r="H6" s="51" t="s">
-        <v>585</v>
-      </c>
-      <c r="I6" s="50" t="s">
-        <v>421</v>
-      </c>
-      <c r="J6" s="50" t="s">
-        <v>291</v>
-      </c>
-      <c r="K6" s="50" t="s">
-        <v>563</v>
-      </c>
-      <c r="L6" s="50" t="s">
-        <v>454</v>
-      </c>
-      <c r="M6" s="50" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="47" t="s">
-        <v>375</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>505</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>553</v>
-      </c>
-      <c r="E7" s="48" t="s">
-        <v>251</v>
-      </c>
-      <c r="F7" s="48" t="s">
+    </row>
+    <row r="48">
+      <c r="C48" s="36" t="s">
+        <v>482</v>
+      </c>
+      <c r="G48" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="G7" s="49" t="s">
-        <v>327</v>
-      </c>
-      <c r="H7" s="51" t="s">
-        <v>586</v>
-      </c>
-      <c r="I7" s="50" t="s">
-        <v>422</v>
-      </c>
-      <c r="J7" s="50" t="s">
-        <v>292</v>
-      </c>
-      <c r="K7" s="50" t="s">
-        <v>564</v>
-      </c>
-      <c r="L7" s="50" t="s">
-        <v>455</v>
-      </c>
-      <c r="M7" s="50" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="47" t="s">
-        <v>376</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>506</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>554</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>252</v>
-      </c>
-      <c r="F8" s="48" t="s">
+    </row>
+    <row r="49">
+      <c r="C49" s="36" t="s">
+        <v>483</v>
+      </c>
+      <c r="G49" s="38" t="s">
         <v>312</v>
       </c>
-      <c r="H8" s="51" t="s">
-        <v>587</v>
-      </c>
-      <c r="I8" s="50" t="s">
-        <v>423</v>
-      </c>
-      <c r="J8" s="50" t="s">
-        <v>293</v>
-      </c>
-      <c r="K8" s="50" t="s">
-        <v>565</v>
-      </c>
-      <c r="L8" s="50" t="s">
-        <v>456</v>
-      </c>
-      <c r="M8" s="50" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="47" t="s">
-        <v>377</v>
-      </c>
-      <c r="C9" s="47" t="s">
-        <v>507</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>555</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>253</v>
-      </c>
-      <c r="F9" s="48" t="s">
+    </row>
+    <row r="50">
+      <c r="C50" s="36" t="s">
+        <v>484</v>
+      </c>
+      <c r="G50" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="H9" s="51" t="s">
-        <v>588</v>
-      </c>
-      <c r="I9" s="50" t="s">
-        <v>424</v>
-      </c>
-      <c r="J9" s="50" t="s">
-        <v>294</v>
-      </c>
-      <c r="K9" s="50" t="s">
-        <v>566</v>
-      </c>
-      <c r="L9" s="50" t="s">
-        <v>457</v>
-      </c>
-      <c r="M9" s="50" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="47" t="s">
-        <v>378</v>
-      </c>
-      <c r="C10" s="47" t="s">
-        <v>508</v>
-      </c>
-      <c r="D10" s="47" t="s">
-        <v>556</v>
-      </c>
-      <c r="E10" s="48" t="s">
-        <v>254</v>
-      </c>
-      <c r="F10" s="48" t="s">
+    </row>
+    <row r="51">
+      <c r="C51" s="36" t="s">
+        <v>485</v>
+      </c>
+      <c r="G51" s="38" t="s">
         <v>314</v>
       </c>
-      <c r="H10" s="51" t="s">
-        <v>589</v>
-      </c>
-      <c r="I10" s="50" t="s">
-        <v>425</v>
-      </c>
-      <c r="J10" s="50" t="s">
-        <v>295</v>
-      </c>
-      <c r="K10" s="50" t="s">
-        <v>567</v>
-      </c>
-      <c r="L10" s="50" t="s">
-        <v>458</v>
-      </c>
-      <c r="M10" s="50" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="47" t="s">
-        <v>379</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>509</v>
-      </c>
-      <c r="D11" s="47" t="s">
-        <v>557</v>
-      </c>
-      <c r="E11" s="48" t="s">
-        <v>255</v>
-      </c>
-      <c r="F11" s="48" t="s">
+    </row>
+    <row r="52">
+      <c r="C52" s="36" t="s">
+        <v>486</v>
+      </c>
+      <c r="G52" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="H11" s="51" t="s">
-        <v>590</v>
-      </c>
-      <c r="I11" s="50" t="s">
-        <v>426</v>
-      </c>
-      <c r="J11" s="50" t="s">
-        <v>296</v>
-      </c>
-      <c r="K11" s="50" t="s">
-        <v>568</v>
-      </c>
-      <c r="L11" s="50" t="s">
-        <v>459</v>
-      </c>
-      <c r="M11" s="50" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="47" t="s">
-        <v>380</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>510</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>558</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>256</v>
-      </c>
-      <c r="F12" s="48" t="s">
+    </row>
+    <row r="53">
+      <c r="C53" s="36" t="s">
+        <v>487</v>
+      </c>
+      <c r="G53" s="38" t="s">
         <v>316</v>
       </c>
-      <c r="H12" s="51" t="s">
-        <v>591</v>
-      </c>
-      <c r="I12" s="50" t="s">
-        <v>427</v>
-      </c>
-      <c r="J12" s="50" t="s">
-        <v>297</v>
-      </c>
-      <c r="K12" s="50" t="s">
-        <v>569</v>
-      </c>
-      <c r="L12" s="50" t="s">
-        <v>460</v>
-      </c>
-      <c r="M12" s="50" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="47" t="s">
-        <v>381</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>511</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>559</v>
-      </c>
-      <c r="E13" s="48" t="s">
-        <v>257</v>
-      </c>
-      <c r="F13" s="48" t="s">
-        <v>317</v>
-      </c>
-      <c r="H13" s="51" t="s">
-        <v>592</v>
-      </c>
-      <c r="I13" s="50" t="s">
-        <v>428</v>
-      </c>
-      <c r="J13" s="50" t="s">
-        <v>298</v>
-      </c>
-      <c r="K13" s="50" t="s">
-        <v>570</v>
-      </c>
-      <c r="L13" s="50" t="s">
-        <v>461</v>
-      </c>
-      <c r="M13" s="50" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="47" t="s">
-        <v>382</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>512</v>
-      </c>
-      <c r="D14" s="47" t="s">
-        <v>560</v>
-      </c>
-      <c r="E14" s="48" t="s">
-        <v>258</v>
-      </c>
-      <c r="F14" s="48" t="s">
-        <v>318</v>
-      </c>
-      <c r="H14" s="51" t="s">
-        <v>593</v>
-      </c>
-      <c r="I14" s="50" t="s">
-        <v>429</v>
-      </c>
-      <c r="J14" s="50" t="s">
-        <v>299</v>
-      </c>
-      <c r="K14" s="50" t="s">
-        <v>571</v>
-      </c>
-      <c r="L14" s="50" t="s">
-        <v>462</v>
-      </c>
-      <c r="M14" s="50" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="47" t="s">
-        <v>383</v>
-      </c>
-      <c r="C15" s="47" t="s">
-        <v>513</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>561</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>259</v>
-      </c>
-      <c r="F15" s="48" t="s">
-        <v>319</v>
-      </c>
-      <c r="H15" s="51" t="s">
-        <v>594</v>
-      </c>
-      <c r="I15" s="50" t="s">
-        <v>430</v>
-      </c>
-      <c r="J15" s="50" t="s">
-        <v>300</v>
-      </c>
-      <c r="K15" s="50" t="s">
-        <v>572</v>
-      </c>
-      <c r="L15" s="50" t="s">
-        <v>463</v>
-      </c>
-      <c r="M15" s="50" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="47" t="s">
-        <v>384</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>514</v>
-      </c>
-      <c r="D16" s="47" t="s">
-        <v>562</v>
-      </c>
-      <c r="E16" s="48" t="s">
-        <v>260</v>
-      </c>
-      <c r="F16" s="48" t="s">
-        <v>320</v>
-      </c>
-      <c r="H16" s="51" t="s">
-        <v>595</v>
-      </c>
-      <c r="I16" s="50" t="s">
-        <v>431</v>
-      </c>
-      <c r="J16" s="50" t="s">
-        <v>301</v>
-      </c>
-      <c r="K16" s="50" t="s">
-        <v>573</v>
-      </c>
-      <c r="L16" s="50" t="s">
-        <v>464</v>
-      </c>
-      <c r="M16" s="50" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="47" t="s">
-        <v>385</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>515</v>
-      </c>
-      <c r="E17" s="48" t="s">
-        <v>261</v>
-      </c>
-      <c r="F17" s="48" t="s">
-        <v>321</v>
-      </c>
-      <c r="H17" s="51" t="s">
-        <v>596</v>
-      </c>
-      <c r="I17" s="50" t="s">
-        <v>432</v>
-      </c>
-      <c r="J17" s="50" t="s">
-        <v>302</v>
-      </c>
-      <c r="K17" s="50" t="s">
-        <v>574</v>
-      </c>
-      <c r="L17" s="50" t="s">
-        <v>465</v>
-      </c>
-      <c r="M17" s="50" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="47" t="s">
-        <v>386</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>516</v>
-      </c>
-      <c r="E18" s="48" t="s">
-        <v>262</v>
-      </c>
-      <c r="F18" s="48" t="s">
-        <v>322</v>
-      </c>
-      <c r="H18" s="51" t="s">
-        <v>597</v>
-      </c>
-      <c r="I18" s="50" t="s">
-        <v>433</v>
-      </c>
-      <c r="J18" s="50" t="s">
-        <v>303</v>
-      </c>
-      <c r="K18" s="50" t="s">
-        <v>575</v>
-      </c>
-      <c r="L18" s="50" t="s">
-        <v>466</v>
-      </c>
-      <c r="M18" s="50" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="47" t="s">
-        <v>387</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>517</v>
-      </c>
-      <c r="E19" s="48" t="s">
-        <v>263</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>323</v>
-      </c>
-      <c r="H19" s="51" t="s">
-        <v>598</v>
-      </c>
-      <c r="I19" s="50" t="s">
-        <v>434</v>
-      </c>
-      <c r="J19" s="50" t="s">
-        <v>304</v>
-      </c>
-      <c r="K19" s="50" t="s">
-        <v>576</v>
-      </c>
-      <c r="L19" s="50" t="s">
-        <v>467</v>
-      </c>
-      <c r="M19" s="50" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="47" t="s">
-        <v>388</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>518</v>
-      </c>
-      <c r="E20" s="48" t="s">
-        <v>264</v>
-      </c>
-      <c r="F20" s="48" t="s">
-        <v>324</v>
-      </c>
-      <c r="H20" s="51" t="s">
-        <v>599</v>
-      </c>
-      <c r="I20" s="50" t="s">
-        <v>435</v>
-      </c>
-      <c r="J20" s="50" t="s">
-        <v>305</v>
-      </c>
-      <c r="K20" s="50" t="s">
-        <v>577</v>
-      </c>
-      <c r="L20" s="50" t="s">
-        <v>468</v>
-      </c>
-      <c r="M20" s="50" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" s="47" t="s">
-        <v>389</v>
-      </c>
-      <c r="C21" s="47" t="s">
-        <v>519</v>
-      </c>
-      <c r="E21" s="48" t="s">
-        <v>265</v>
-      </c>
-      <c r="F21" s="48" t="s">
-        <v>325</v>
-      </c>
-      <c r="H21" s="51" t="s">
-        <v>600</v>
-      </c>
-      <c r="I21" s="50" t="s">
-        <v>436</v>
-      </c>
-      <c r="J21" s="50" t="s">
-        <v>306</v>
-      </c>
-      <c r="K21" s="50" t="s">
-        <v>578</v>
-      </c>
-      <c r="L21" s="50" t="s">
-        <v>469</v>
-      </c>
-      <c r="M21" s="50" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" s="47" t="s">
-        <v>390</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>520</v>
-      </c>
-      <c r="E22" s="48" t="s">
-        <v>266</v>
-      </c>
-      <c r="H22" s="51" t="s">
-        <v>601</v>
-      </c>
-      <c r="I22" s="50" t="s">
-        <v>437</v>
-      </c>
-      <c r="J22" s="50" t="s">
-        <v>307</v>
-      </c>
-      <c r="K22" s="50" t="s">
-        <v>579</v>
-      </c>
-      <c r="L22" s="50" t="s">
-        <v>470</v>
-      </c>
-      <c r="M22" s="50" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" s="47" t="s">
-        <v>391</v>
-      </c>
-      <c r="C23" s="47" t="s">
-        <v>521</v>
-      </c>
-      <c r="E23" s="48" t="s">
-        <v>267</v>
-      </c>
-      <c r="H23" s="51" t="s">
-        <v>602</v>
-      </c>
-      <c r="I23" s="50" t="s">
-        <v>438</v>
-      </c>
-      <c r="J23" s="50" t="s">
-        <v>308</v>
-      </c>
-      <c r="K23" s="50" t="s">
-        <v>580</v>
-      </c>
-      <c r="L23" s="50" t="s">
-        <v>471</v>
-      </c>
-      <c r="M23" s="50" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" s="47" t="s">
-        <v>392</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>522</v>
-      </c>
-      <c r="E24" s="48" t="s">
-        <v>268</v>
-      </c>
-      <c r="H24" s="51" t="s">
-        <v>603</v>
-      </c>
-      <c r="I24" s="50" t="s">
-        <v>439</v>
-      </c>
-      <c r="J24" s="50" t="s">
-        <v>309</v>
-      </c>
-      <c r="K24" s="50" t="s">
-        <v>581</v>
-      </c>
-      <c r="L24" s="50" t="s">
-        <v>472</v>
-      </c>
-      <c r="M24" s="50" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="47" t="s">
-        <v>393</v>
-      </c>
-      <c r="C25" s="47" t="s">
-        <v>523</v>
-      </c>
-      <c r="E25" s="48" t="s">
-        <v>269</v>
-      </c>
-      <c r="H25" s="51" t="s">
-        <v>604</v>
-      </c>
-      <c r="I25" s="50" t="s">
-        <v>440</v>
-      </c>
-      <c r="K25" s="50" t="s">
-        <v>582</v>
-      </c>
-      <c r="L25" s="50" t="s">
-        <v>473</v>
-      </c>
-      <c r="M25" s="50" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="47" t="s">
-        <v>394</v>
-      </c>
-      <c r="C26" s="47" t="s">
-        <v>524</v>
-      </c>
-      <c r="E26" s="48" t="s">
-        <v>270</v>
-      </c>
-      <c r="H26" s="51" t="s">
-        <v>605</v>
-      </c>
-      <c r="I26" s="50" t="s">
-        <v>441</v>
-      </c>
-      <c r="K26" s="50" t="s">
-        <v>583</v>
-      </c>
-      <c r="L26" s="50" t="s">
-        <v>474</v>
-      </c>
-      <c r="M26" s="50" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="47" t="s">
-        <v>395</v>
-      </c>
-      <c r="C27" s="47" t="s">
-        <v>525</v>
-      </c>
-      <c r="E27" s="48" t="s">
-        <v>271</v>
-      </c>
-      <c r="H27" s="51" t="s">
-        <v>606</v>
-      </c>
-      <c r="I27" s="50" t="s">
-        <v>442</v>
-      </c>
-      <c r="K27" s="50" t="s">
-        <v>584</v>
-      </c>
-      <c r="L27" s="50" t="s">
-        <v>475</v>
-      </c>
-      <c r="M27" s="50" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="47" t="s">
-        <v>396</v>
-      </c>
-      <c r="C28" s="47" t="s">
-        <v>526</v>
-      </c>
-      <c r="E28" s="48" t="s">
-        <v>272</v>
-      </c>
-      <c r="H28" s="51" t="s">
-        <v>607</v>
-      </c>
-      <c r="I28" s="50" t="s">
-        <v>443</v>
-      </c>
-      <c r="L28" s="50" t="s">
-        <v>476</v>
-      </c>
-      <c r="M28" s="50" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="47" t="s">
-        <v>397</v>
-      </c>
-      <c r="C29" s="47" t="s">
-        <v>527</v>
-      </c>
-      <c r="E29" s="48" t="s">
-        <v>273</v>
-      </c>
-      <c r="H29" s="51" t="s">
-        <v>608</v>
-      </c>
-      <c r="I29" s="50" t="s">
-        <v>444</v>
-      </c>
-      <c r="L29" s="50" t="s">
-        <v>477</v>
-      </c>
-      <c r="M29" s="50" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" s="47" t="s">
-        <v>398</v>
-      </c>
-      <c r="C30" s="47" t="s">
-        <v>528</v>
-      </c>
-      <c r="E30" s="48" t="s">
-        <v>274</v>
-      </c>
-      <c r="H30" s="51" t="s">
-        <v>609</v>
-      </c>
-      <c r="I30" s="50" t="s">
-        <v>445</v>
-      </c>
-      <c r="L30" s="50" t="s">
-        <v>478</v>
-      </c>
-      <c r="M30" s="50" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="47" t="s">
-        <v>399</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>529</v>
-      </c>
-      <c r="E31" s="48" t="s">
-        <v>275</v>
-      </c>
-      <c r="H31" s="51" t="s">
-        <v>610</v>
-      </c>
-      <c r="I31" s="50" t="s">
-        <v>446</v>
-      </c>
-      <c r="L31" s="50" t="s">
-        <v>479</v>
-      </c>
-      <c r="M31" s="50" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" s="47" t="s">
-        <v>400</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>530</v>
-      </c>
-      <c r="E32" s="48" t="s">
-        <v>276</v>
-      </c>
-      <c r="H32" s="51" t="s">
-        <v>611</v>
-      </c>
-      <c r="I32" s="50" t="s">
-        <v>447</v>
-      </c>
-      <c r="L32" s="50" t="s">
-        <v>480</v>
-      </c>
-      <c r="M32" s="50" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" s="47" t="s">
-        <v>401</v>
-      </c>
-      <c r="C33" s="47" t="s">
-        <v>531</v>
-      </c>
-      <c r="E33" s="48" t="s">
-        <v>277</v>
-      </c>
-      <c r="H33" s="51" t="s">
-        <v>612</v>
-      </c>
-      <c r="I33" s="50" t="s">
-        <v>448</v>
-      </c>
-      <c r="L33" s="50" t="s">
-        <v>481</v>
-      </c>
-      <c r="M33" s="50" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" s="47" t="s">
-        <v>402</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>532</v>
-      </c>
-      <c r="E34" s="48" t="s">
-        <v>278</v>
-      </c>
-      <c r="I34" s="50" t="s">
-        <v>449</v>
-      </c>
-      <c r="L34" s="50" t="s">
-        <v>482</v>
-      </c>
-      <c r="M34" s="50" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" s="47" t="s">
-        <v>403</v>
-      </c>
-      <c r="C35" s="47" t="s">
-        <v>533</v>
-      </c>
-      <c r="E35" s="48" t="s">
-        <v>279</v>
-      </c>
-      <c r="I35" s="50" t="s">
-        <v>450</v>
-      </c>
-      <c r="L35" s="50" t="s">
-        <v>483</v>
-      </c>
-      <c r="M35" s="50" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" s="47" t="s">
-        <v>404</v>
-      </c>
-      <c r="C36" s="47" t="s">
-        <v>534</v>
-      </c>
-      <c r="E36" s="48" t="s">
-        <v>280</v>
-      </c>
-      <c r="I36" s="50" t="s">
-        <v>451</v>
-      </c>
-      <c r="L36" s="50" t="s">
-        <v>484</v>
-      </c>
-      <c r="M36" s="50" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" s="47" t="s">
-        <v>405</v>
-      </c>
-      <c r="C37" s="47" t="s">
-        <v>535</v>
-      </c>
-      <c r="E37" s="48" t="s">
-        <v>281</v>
-      </c>
-      <c r="I37" s="50" t="s">
-        <v>452</v>
-      </c>
-      <c r="L37" s="50" t="s">
-        <v>485</v>
-      </c>
-      <c r="M37" s="50" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="B38" s="47" t="s">
-        <v>406</v>
-      </c>
-      <c r="C38" s="47" t="s">
-        <v>536</v>
-      </c>
-      <c r="E38" s="48" t="s">
-        <v>282</v>
-      </c>
-      <c r="I38" s="50" t="s">
-        <v>453</v>
-      </c>
-      <c r="L38" s="50" t="s">
-        <v>486</v>
-      </c>
-      <c r="M38" s="50" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" s="47" t="s">
-        <v>407</v>
-      </c>
-      <c r="C39" s="47" t="s">
-        <v>537</v>
-      </c>
-      <c r="E39" s="48" t="s">
-        <v>283</v>
-      </c>
-      <c r="L39" s="50" t="s">
-        <v>487</v>
-      </c>
-      <c r="M39" s="50" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" s="47" t="s">
-        <v>408</v>
-      </c>
-      <c r="C40" s="47" t="s">
-        <v>538</v>
-      </c>
-      <c r="E40" s="48" t="s">
-        <v>284</v>
-      </c>
-      <c r="L40" s="50" t="s">
+    </row>
+    <row r="54">
+      <c r="C54" s="36" t="s">
         <v>488</v>
       </c>
-      <c r="M40" s="50" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="B41" s="47" t="s">
-        <v>409</v>
-      </c>
-      <c r="C41" s="47" t="s">
-        <v>539</v>
-      </c>
-      <c r="E41" s="48" t="s">
-        <v>285</v>
-      </c>
-      <c r="L41" s="50" t="s">
+    </row>
+    <row r="55">
+      <c r="C55" s="36" t="s">
         <v>489</v>
-      </c>
-      <c r="M41" s="50" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" s="47" t="s">
-        <v>410</v>
-      </c>
-      <c r="C42" s="47" t="s">
-        <v>540</v>
-      </c>
-      <c r="E42" s="48" t="s">
-        <v>286</v>
-      </c>
-      <c r="L42" s="50" t="s">
-        <v>490</v>
-      </c>
-      <c r="M42" s="50" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" s="47" t="s">
-        <v>411</v>
-      </c>
-      <c r="C43" s="47" t="s">
-        <v>541</v>
-      </c>
-      <c r="E43" s="48" t="s">
-        <v>287</v>
-      </c>
-      <c r="L43" s="50" t="s">
-        <v>491</v>
-      </c>
-      <c r="M43" s="50" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" s="47" t="s">
-        <v>412</v>
-      </c>
-      <c r="C44" s="47" t="s">
-        <v>542</v>
-      </c>
-      <c r="E44" s="48" t="s">
-        <v>288</v>
-      </c>
-      <c r="L44" s="50" t="s">
-        <v>492</v>
-      </c>
-      <c r="M44" s="50" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" s="47" t="s">
-        <v>413</v>
-      </c>
-      <c r="C45" s="47" t="s">
-        <v>543</v>
-      </c>
-      <c r="E45" s="48" t="s">
-        <v>289</v>
-      </c>
-      <c r="L45" s="50" t="s">
-        <v>493</v>
-      </c>
-      <c r="M45" s="50" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" s="47" t="s">
-        <v>414</v>
-      </c>
-      <c r="C46" s="47" t="s">
-        <v>544</v>
-      </c>
-      <c r="L46" s="50" t="s">
-        <v>494</v>
-      </c>
-      <c r="M46" s="50" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" s="47" t="s">
-        <v>415</v>
-      </c>
-      <c r="C47" s="47" t="s">
-        <v>545</v>
-      </c>
-      <c r="L47" s="50" t="s">
-        <v>495</v>
-      </c>
-      <c r="M47" s="50" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" s="47" t="s">
-        <v>416</v>
-      </c>
-      <c r="C48" s="47" t="s">
-        <v>546</v>
-      </c>
-      <c r="L48" s="50" t="s">
-        <v>496</v>
-      </c>
-      <c r="M48" s="50" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" s="47" t="s">
-        <v>417</v>
-      </c>
-      <c r="C49" s="47" t="s">
-        <v>547</v>
-      </c>
-      <c r="L49" s="50" t="s">
-        <v>497</v>
-      </c>
-      <c r="M49" s="50" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" s="47" t="s">
-        <v>418</v>
-      </c>
-      <c r="C50" s="47" t="s">
-        <v>548</v>
-      </c>
-      <c r="L50" s="50" t="s">
-        <v>498</v>
-      </c>
-      <c r="M50" s="50" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" s="47" t="s">
-        <v>419</v>
-      </c>
-      <c r="C51" s="47" t="s">
-        <v>549</v>
-      </c>
-      <c r="L51" s="50" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="C52" s="47" t="s">
-        <v>550</v>
-      </c>
-      <c r="L52" s="50" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="C53" s="47" t="s">
-        <v>551</v>
-      </c>
-      <c r="L53" s="50" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="L54" s="50" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="L55" s="50" t="s">
-        <v>503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed range method name
</commit_message>
<xml_diff>
--- a/X-Domestic Standard Upload.xlsx
+++ b/X-Domestic Standard Upload.xlsx
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="623">
   <si>
     <t>#</t>
   </si>
@@ -1201,6 +1201,48 @@
     <t>col:19</t>
   </si>
   <si>
+    <t>col:20</t>
+  </si>
+  <si>
+    <t>col:21</t>
+  </si>
+  <si>
+    <t>col:22</t>
+  </si>
+  <si>
+    <t>col:23</t>
+  </si>
+  <si>
+    <t>col:24</t>
+  </si>
+  <si>
+    <t>col:25</t>
+  </si>
+  <si>
+    <t>col:26</t>
+  </si>
+  <si>
+    <t>col:27</t>
+  </si>
+  <si>
+    <t>col:28</t>
+  </si>
+  <si>
+    <t>col:29</t>
+  </si>
+  <si>
+    <t>col:30</t>
+  </si>
+  <si>
+    <t>col:31</t>
+  </si>
+  <si>
+    <t>col:32</t>
+  </si>
+  <si>
+    <t>col:33</t>
+  </si>
+  <si>
     <t>dep:0</t>
   </si>
   <si>
@@ -1273,6 +1315,78 @@
     <t>dep:23</t>
   </si>
   <si>
+    <t>dep:24</t>
+  </si>
+  <si>
+    <t>dep:25</t>
+  </si>
+  <si>
+    <t>dep:26</t>
+  </si>
+  <si>
+    <t>dep:27</t>
+  </si>
+  <si>
+    <t>dep:28</t>
+  </si>
+  <si>
+    <t>dep:29</t>
+  </si>
+  <si>
+    <t>dep:30</t>
+  </si>
+  <si>
+    <t>dep:31</t>
+  </si>
+  <si>
+    <t>dep:32</t>
+  </si>
+  <si>
+    <t>dep:33</t>
+  </si>
+  <si>
+    <t>dep:34</t>
+  </si>
+  <si>
+    <t>dep:35</t>
+  </si>
+  <si>
+    <t>dep:36</t>
+  </si>
+  <si>
+    <t>dep:37</t>
+  </si>
+  <si>
+    <t>dep:38</t>
+  </si>
+  <si>
+    <t>dep:39</t>
+  </si>
+  <si>
+    <t>dep:40</t>
+  </si>
+  <si>
+    <t>dep:41</t>
+  </si>
+  <si>
+    <t>dep:42</t>
+  </si>
+  <si>
+    <t>dep:43</t>
+  </si>
+  <si>
+    <t>dep:44</t>
+  </si>
+  <si>
+    <t>dep:45</t>
+  </si>
+  <si>
+    <t>dep:46</t>
+  </si>
+  <si>
+    <t>dep:47</t>
+  </si>
+  <si>
     <t>siz:0</t>
   </si>
   <si>
@@ -1294,6 +1408,135 @@
     <t>siz:6</t>
   </si>
   <si>
+    <t>siz:7</t>
+  </si>
+  <si>
+    <t>siz:8</t>
+  </si>
+  <si>
+    <t>siz:9</t>
+  </si>
+  <si>
+    <t>siz:10</t>
+  </si>
+  <si>
+    <t>siz:11</t>
+  </si>
+  <si>
+    <t>siz:12</t>
+  </si>
+  <si>
+    <t>siz:13</t>
+  </si>
+  <si>
+    <t>siz:14</t>
+  </si>
+  <si>
+    <t>siz:15</t>
+  </si>
+  <si>
+    <t>siz:16</t>
+  </si>
+  <si>
+    <t>siz:17</t>
+  </si>
+  <si>
+    <t>siz:18</t>
+  </si>
+  <si>
+    <t>siz:19</t>
+  </si>
+  <si>
+    <t>siz:20</t>
+  </si>
+  <si>
+    <t>siz:21</t>
+  </si>
+  <si>
+    <t>siz:22</t>
+  </si>
+  <si>
+    <t>siz:23</t>
+  </si>
+  <si>
+    <t>siz:24</t>
+  </si>
+  <si>
+    <t>siz:25</t>
+  </si>
+  <si>
+    <t>siz:26</t>
+  </si>
+  <si>
+    <t>siz:27</t>
+  </si>
+  <si>
+    <t>siz:28</t>
+  </si>
+  <si>
+    <t>siz:29</t>
+  </si>
+  <si>
+    <t>siz:30</t>
+  </si>
+  <si>
+    <t>siz:31</t>
+  </si>
+  <si>
+    <t>siz:32</t>
+  </si>
+  <si>
+    <t>siz:33</t>
+  </si>
+  <si>
+    <t>siz:34</t>
+  </si>
+  <si>
+    <t>siz:35</t>
+  </si>
+  <si>
+    <t>siz:36</t>
+  </si>
+  <si>
+    <t>siz:37</t>
+  </si>
+  <si>
+    <t>siz:38</t>
+  </si>
+  <si>
+    <t>siz:39</t>
+  </si>
+  <si>
+    <t>siz:40</t>
+  </si>
+  <si>
+    <t>siz:41</t>
+  </si>
+  <si>
+    <t>siz:42</t>
+  </si>
+  <si>
+    <t>siz:43</t>
+  </si>
+  <si>
+    <t>siz:44</t>
+  </si>
+  <si>
+    <t>siz:45</t>
+  </si>
+  <si>
+    <t>siz:46</t>
+  </si>
+  <si>
+    <t>siz:47</t>
+  </si>
+  <si>
+    <t>siz:48</t>
+  </si>
+  <si>
+    <t>siz:49</t>
+  </si>
+  <si>
     <t>typ:0</t>
   </si>
   <si>
@@ -1384,6 +1627,39 @@
     <t>typ:29</t>
   </si>
   <si>
+    <t>typ:30</t>
+  </si>
+  <si>
+    <t>typ:31</t>
+  </si>
+  <si>
+    <t>typ:32</t>
+  </si>
+  <si>
+    <t>typ:33</t>
+  </si>
+  <si>
+    <t>typ:34</t>
+  </si>
+  <si>
+    <t>typ:35</t>
+  </si>
+  <si>
+    <t>typ:36</t>
+  </si>
+  <si>
+    <t>typ:37</t>
+  </si>
+  <si>
+    <t>typ:38</t>
+  </si>
+  <si>
+    <t>typ:39</t>
+  </si>
+  <si>
+    <t>typ:40</t>
+  </si>
+  <si>
     <t>mat:0</t>
   </si>
   <si>
@@ -1432,51 +1708,6 @@
     <t>mat:15</t>
   </si>
   <si>
-    <t>mat:16</t>
-  </si>
-  <si>
-    <t>mat:17</t>
-  </si>
-  <si>
-    <t>mat:18</t>
-  </si>
-  <si>
-    <t>mat:19</t>
-  </si>
-  <si>
-    <t>mat:20</t>
-  </si>
-  <si>
-    <t>mat:21</t>
-  </si>
-  <si>
-    <t>mat:22</t>
-  </si>
-  <si>
-    <t>mat:23</t>
-  </si>
-  <si>
-    <t>mat:24</t>
-  </si>
-  <si>
-    <t>mat:25</t>
-  </si>
-  <si>
-    <t>mat:26</t>
-  </si>
-  <si>
-    <t>mat:27</t>
-  </si>
-  <si>
-    <t>mat:28</t>
-  </si>
-  <si>
-    <t>mat:29</t>
-  </si>
-  <si>
-    <t>mat:30</t>
-  </si>
-  <si>
     <t>vpn:0</t>
   </si>
   <si>
@@ -1492,75 +1723,6 @@
     <t>vpn:4</t>
   </si>
   <si>
-    <t>vpn:5</t>
-  </si>
-  <si>
-    <t>vpn:6</t>
-  </si>
-  <si>
-    <t>vpn:7</t>
-  </si>
-  <si>
-    <t>vpn:8</t>
-  </si>
-  <si>
-    <t>vpn:9</t>
-  </si>
-  <si>
-    <t>vpn:10</t>
-  </si>
-  <si>
-    <t>vpn:11</t>
-  </si>
-  <si>
-    <t>vpn:12</t>
-  </si>
-  <si>
-    <t>vpn:13</t>
-  </si>
-  <si>
-    <t>vpn:14</t>
-  </si>
-  <si>
-    <t>vpn:15</t>
-  </si>
-  <si>
-    <t>vpn:16</t>
-  </si>
-  <si>
-    <t>vpn:17</t>
-  </si>
-  <si>
-    <t>vpn:18</t>
-  </si>
-  <si>
-    <t>vpn:19</t>
-  </si>
-  <si>
-    <t>vpn:20</t>
-  </si>
-  <si>
-    <t>vpn:21</t>
-  </si>
-  <si>
-    <t>vpn:22</t>
-  </si>
-  <si>
-    <t>vpn:23</t>
-  </si>
-  <si>
-    <t>vpn:24</t>
-  </si>
-  <si>
-    <t>vpn:25</t>
-  </si>
-  <si>
-    <t>vpn:26</t>
-  </si>
-  <si>
-    <t>vpn:27</t>
-  </si>
-  <si>
     <t>sup:0</t>
   </si>
   <si>
@@ -1612,51 +1774,6 @@
     <t>sup:16</t>
   </si>
   <si>
-    <t>sup:17</t>
-  </si>
-  <si>
-    <t>sup:18</t>
-  </si>
-  <si>
-    <t>sup:19</t>
-  </si>
-  <si>
-    <t>sup:20</t>
-  </si>
-  <si>
-    <t>sup:21</t>
-  </si>
-  <si>
-    <t>sup:22</t>
-  </si>
-  <si>
-    <t>sup:23</t>
-  </si>
-  <si>
-    <t>sup:24</t>
-  </si>
-  <si>
-    <t>sup:25</t>
-  </si>
-  <si>
-    <t>sup:26</t>
-  </si>
-  <si>
-    <t>sup:27</t>
-  </si>
-  <si>
-    <t>sup:28</t>
-  </si>
-  <si>
-    <t>sup:29</t>
-  </si>
-  <si>
-    <t>sup:30</t>
-  </si>
-  <si>
-    <t>sup:31</t>
-  </si>
-  <si>
     <t>cat:0</t>
   </si>
   <si>
@@ -1678,6 +1795,135 @@
     <t>cat:6</t>
   </si>
   <si>
+    <t>cat:7</t>
+  </si>
+  <si>
+    <t>cat:8</t>
+  </si>
+  <si>
+    <t>cat:9</t>
+  </si>
+  <si>
+    <t>cat:10</t>
+  </si>
+  <si>
+    <t>cat:11</t>
+  </si>
+  <si>
+    <t>cat:12</t>
+  </si>
+  <si>
+    <t>cat:13</t>
+  </si>
+  <si>
+    <t>cat:14</t>
+  </si>
+  <si>
+    <t>cat:15</t>
+  </si>
+  <si>
+    <t>cat:16</t>
+  </si>
+  <si>
+    <t>cat:17</t>
+  </si>
+  <si>
+    <t>cat:18</t>
+  </si>
+  <si>
+    <t>cat:19</t>
+  </si>
+  <si>
+    <t>cat:20</t>
+  </si>
+  <si>
+    <t>cat:21</t>
+  </si>
+  <si>
+    <t>cat:22</t>
+  </si>
+  <si>
+    <t>cat:23</t>
+  </si>
+  <si>
+    <t>cat:24</t>
+  </si>
+  <si>
+    <t>cat:25</t>
+  </si>
+  <si>
+    <t>cat:26</t>
+  </si>
+  <si>
+    <t>cat:27</t>
+  </si>
+  <si>
+    <t>cat:28</t>
+  </si>
+  <si>
+    <t>cat:29</t>
+  </si>
+  <si>
+    <t>cat:30</t>
+  </si>
+  <si>
+    <t>cat:31</t>
+  </si>
+  <si>
+    <t>cat:32</t>
+  </si>
+  <si>
+    <t>cat:33</t>
+  </si>
+  <si>
+    <t>cat:34</t>
+  </si>
+  <si>
+    <t>cat:35</t>
+  </si>
+  <si>
+    <t>cat:36</t>
+  </si>
+  <si>
+    <t>cat:37</t>
+  </si>
+  <si>
+    <t>cat:38</t>
+  </si>
+  <si>
+    <t>cat:39</t>
+  </si>
+  <si>
+    <t>cat:40</t>
+  </si>
+  <si>
+    <t>cat:41</t>
+  </si>
+  <si>
+    <t>cat:42</t>
+  </si>
+  <si>
+    <t>cat:43</t>
+  </si>
+  <si>
+    <t>cat:44</t>
+  </si>
+  <si>
+    <t>cat:45</t>
+  </si>
+  <si>
+    <t>cat:46</t>
+  </si>
+  <si>
+    <t>cat:47</t>
+  </si>
+  <si>
+    <t>cat:48</t>
+  </si>
+  <si>
+    <t>cat:49</t>
+  </si>
+  <si>
     <t>ven:0</t>
   </si>
   <si>
@@ -1744,6 +1990,24 @@
     <t>ven:21</t>
   </si>
   <si>
+    <t>ven:22</t>
+  </si>
+  <si>
+    <t>ven:23</t>
+  </si>
+  <si>
+    <t>ven:24</t>
+  </si>
+  <si>
+    <t>ven:25</t>
+  </si>
+  <si>
+    <t>ven:26</t>
+  </si>
+  <si>
+    <t>ven:27</t>
+  </si>
+  <si>
     <t>lab:0</t>
   </si>
   <si>
@@ -1825,30 +2089,6 @@
     <t>lab:26</t>
   </si>
   <si>
-    <t>lab:27</t>
-  </si>
-  <si>
-    <t>lab:28</t>
-  </si>
-  <si>
-    <t>lab:29</t>
-  </si>
-  <si>
-    <t>lab:30</t>
-  </si>
-  <si>
-    <t>lab:31</t>
-  </si>
-  <si>
-    <t>lab:32</t>
-  </si>
-  <si>
-    <t>lab:33</t>
-  </si>
-  <si>
-    <t>lab:34</t>
-  </si>
-  <si>
     <t>cla:0</t>
   </si>
   <si>
@@ -1939,6 +2179,45 @@
     <t>cla:29</t>
   </si>
   <si>
+    <t>cla:30</t>
+  </si>
+  <si>
+    <t>cla:31</t>
+  </si>
+  <si>
+    <t>cla:32</t>
+  </si>
+  <si>
+    <t>cla:33</t>
+  </si>
+  <si>
+    <t>cla:34</t>
+  </si>
+  <si>
+    <t>cla:35</t>
+  </si>
+  <si>
+    <t>cla:36</t>
+  </si>
+  <si>
+    <t>cla:37</t>
+  </si>
+  <si>
+    <t>cla:38</t>
+  </si>
+  <si>
+    <t>cla:39</t>
+  </si>
+  <si>
+    <t>cla:40</t>
+  </si>
+  <si>
+    <t>cla:41</t>
+  </si>
+  <si>
+    <t>cla:42</t>
+  </si>
+  <si>
     <t>pon:0</t>
   </si>
   <si>
@@ -1979,108 +2258,6 @@
   </si>
   <si>
     <t>pon:13</t>
-  </si>
-  <si>
-    <t>pon:14</t>
-  </si>
-  <si>
-    <t>pon:15</t>
-  </si>
-  <si>
-    <t>pon:16</t>
-  </si>
-  <si>
-    <t>pon:17</t>
-  </si>
-  <si>
-    <t>pon:18</t>
-  </si>
-  <si>
-    <t>pon:19</t>
-  </si>
-  <si>
-    <t>pon:20</t>
-  </si>
-  <si>
-    <t>pon:21</t>
-  </si>
-  <si>
-    <t>pon:22</t>
-  </si>
-  <si>
-    <t>pon:23</t>
-  </si>
-  <si>
-    <t>pon:24</t>
-  </si>
-  <si>
-    <t>pon:25</t>
-  </si>
-  <si>
-    <t>pon:26</t>
-  </si>
-  <si>
-    <t>pon:27</t>
-  </si>
-  <si>
-    <t>pon:28</t>
-  </si>
-  <si>
-    <t>pon:29</t>
-  </si>
-  <si>
-    <t>pon:30</t>
-  </si>
-  <si>
-    <t>pon:31</t>
-  </si>
-  <si>
-    <t>pon:32</t>
-  </si>
-  <si>
-    <t>pon:33</t>
-  </si>
-  <si>
-    <t>pon:34</t>
-  </si>
-  <si>
-    <t>pon:35</t>
-  </si>
-  <si>
-    <t>pon:36</t>
-  </si>
-  <si>
-    <t>pon:37</t>
-  </si>
-  <si>
-    <t>pon:38</t>
-  </si>
-  <si>
-    <t>pon:39</t>
-  </si>
-  <si>
-    <t>pon:40</t>
-  </si>
-  <si>
-    <t>pon:41</t>
-  </si>
-  <si>
-    <t>pon:42</t>
-  </si>
-  <si>
-    <t>pon:43</t>
-  </si>
-  <si>
-    <t>pon:44</t>
-  </si>
-  <si>
-    <t>pon:45</t>
-  </si>
-  <si>
-    <t>pon:46</t>
-  </si>
-  <si>
-    <t>pon:47</t>
   </si>
 </sst>
 </file>
@@ -6537,7 +6714,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A17F3EB-F212-417F-BA00-A3FB97B2BF77}">
-  <dimension ref="A1:CV53"/>
+  <dimension ref="A1:CV55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
@@ -7917,1022 +8094,1212 @@
     </row>
     <row r="6">
       <c r="B6" s="36" t="s">
-        <v>362</v>
+        <v>439</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>429</v>
+        <v>511</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>451</v>
+        <v>539</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>250</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>294</v>
+        <v>332</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>301</v>
+        <v>382</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>516</v>
+        <v>609</v>
       </c>
       <c r="I6" s="39" t="s">
-        <v>390</v>
+        <v>444</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="K6" s="39" t="s">
-        <v>486</v>
+        <v>566</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>422</v>
+        <v>461</v>
       </c>
       <c r="M6" s="39" t="s">
-        <v>331</v>
+        <v>423</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="36" t="s">
-        <v>363</v>
+        <v>440</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>430</v>
+        <v>512</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>452</v>
+        <v>540</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>251</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>295</v>
+        <v>333</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>302</v>
+        <v>383</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>517</v>
+        <v>610</v>
       </c>
       <c r="I7" s="39" t="s">
-        <v>391</v>
+        <v>445</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>487</v>
+        <v>567</v>
       </c>
       <c r="L7" s="39" t="s">
-        <v>423</v>
+        <v>462</v>
       </c>
       <c r="M7" s="39" t="s">
-        <v>332</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="36" t="s">
-        <v>364</v>
+        <v>441</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>431</v>
+        <v>513</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>453</v>
+        <v>541</v>
       </c>
       <c r="E8" s="37" t="s">
         <v>252</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>296</v>
+        <v>334</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>303</v>
+        <v>384</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>518</v>
+        <v>611</v>
       </c>
       <c r="I8" s="39" t="s">
-        <v>392</v>
+        <v>446</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>488</v>
+        <v>568</v>
       </c>
       <c r="L8" s="39" t="s">
-        <v>424</v>
+        <v>463</v>
       </c>
       <c r="M8" s="39" t="s">
-        <v>333</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="36" t="s">
-        <v>365</v>
+        <v>442</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>432</v>
+        <v>514</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>454</v>
+        <v>542</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>253</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>297</v>
+        <v>335</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>304</v>
+        <v>385</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>519</v>
+        <v>612</v>
       </c>
       <c r="I9" s="39" t="s">
-        <v>393</v>
+        <v>447</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="K9" s="39" t="s">
-        <v>489</v>
+        <v>569</v>
       </c>
       <c r="L9" s="39" t="s">
-        <v>425</v>
+        <v>464</v>
       </c>
       <c r="M9" s="39" t="s">
-        <v>334</v>
+        <v>426</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="36" t="s">
-        <v>366</v>
+        <v>443</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>433</v>
+        <v>515</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>455</v>
+        <v>543</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>254</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>298</v>
+        <v>336</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>305</v>
+        <v>386</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>520</v>
+        <v>613</v>
       </c>
       <c r="I10" s="39" t="s">
-        <v>394</v>
+        <v>448</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>490</v>
+        <v>570</v>
       </c>
       <c r="L10" s="39" t="s">
-        <v>426</v>
+        <v>465</v>
       </c>
       <c r="M10" s="39" t="s">
-        <v>335</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="36" t="s">
-        <v>367</v>
-      </c>
       <c r="C11" s="36" t="s">
-        <v>434</v>
+        <v>516</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>456</v>
+        <v>544</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>255</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>299</v>
+        <v>337</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>306</v>
+        <v>387</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>521</v>
+        <v>614</v>
       </c>
       <c r="I11" s="39" t="s">
-        <v>395</v>
+        <v>449</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>491</v>
+        <v>571</v>
       </c>
       <c r="L11" s="39" t="s">
-        <v>427</v>
+        <v>466</v>
       </c>
       <c r="M11" s="39" t="s">
-        <v>336</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="36" t="s">
-        <v>368</v>
-      </c>
       <c r="C12" s="36" t="s">
-        <v>435</v>
+        <v>517</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>457</v>
+        <v>545</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>256</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>300</v>
+        <v>338</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>307</v>
+        <v>388</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>522</v>
+        <v>615</v>
       </c>
       <c r="I12" s="39" t="s">
-        <v>396</v>
+        <v>450</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="K12" s="39" t="s">
-        <v>492</v>
+        <v>572</v>
       </c>
       <c r="L12" s="39" t="s">
-        <v>428</v>
+        <v>467</v>
       </c>
       <c r="M12" s="39" t="s">
-        <v>337</v>
+        <v>429</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="36" t="s">
-        <v>369</v>
-      </c>
       <c r="C13" s="36" t="s">
-        <v>436</v>
+        <v>518</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>458</v>
+        <v>546</v>
       </c>
       <c r="E13" s="37" t="s">
         <v>257</v>
       </c>
+      <c r="F13" s="37" t="s">
+        <v>339</v>
+      </c>
       <c r="G13" s="38" t="s">
-        <v>308</v>
+        <v>389</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>523</v>
+        <v>616</v>
       </c>
       <c r="I13" s="39" t="s">
-        <v>397</v>
+        <v>451</v>
       </c>
       <c r="J13" s="39" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="K13" s="39" t="s">
-        <v>493</v>
+        <v>573</v>
+      </c>
+      <c r="L13" s="39" t="s">
+        <v>468</v>
       </c>
       <c r="M13" s="39" t="s">
-        <v>338</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="36" t="s">
-        <v>370</v>
-      </c>
       <c r="C14" s="36" t="s">
-        <v>437</v>
+        <v>519</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>459</v>
+        <v>547</v>
       </c>
       <c r="E14" s="37" t="s">
         <v>258</v>
       </c>
+      <c r="F14" s="37" t="s">
+        <v>340</v>
+      </c>
       <c r="G14" s="38" t="s">
-        <v>309</v>
+        <v>390</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>524</v>
+        <v>617</v>
       </c>
       <c r="I14" s="39" t="s">
-        <v>398</v>
+        <v>452</v>
       </c>
       <c r="J14" s="39" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="K14" s="39" t="s">
-        <v>494</v>
+        <v>574</v>
+      </c>
+      <c r="L14" s="39" t="s">
+        <v>469</v>
       </c>
       <c r="M14" s="39" t="s">
-        <v>339</v>
+        <v>431</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="36" t="s">
-        <v>371</v>
-      </c>
       <c r="C15" s="36" t="s">
-        <v>438</v>
+        <v>520</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>460</v>
+        <v>548</v>
       </c>
       <c r="E15" s="37" t="s">
         <v>259</v>
       </c>
+      <c r="F15" s="37" t="s">
+        <v>341</v>
+      </c>
       <c r="G15" s="38" t="s">
-        <v>310</v>
+        <v>391</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>525</v>
+        <v>618</v>
       </c>
       <c r="I15" s="39" t="s">
-        <v>399</v>
+        <v>453</v>
       </c>
       <c r="J15" s="39" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="K15" s="39" t="s">
-        <v>495</v>
+        <v>575</v>
+      </c>
+      <c r="L15" s="39" t="s">
+        <v>470</v>
       </c>
       <c r="M15" s="39" t="s">
-        <v>340</v>
+        <v>432</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="36" t="s">
-        <v>372</v>
-      </c>
       <c r="C16" s="36" t="s">
-        <v>439</v>
+        <v>521</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>461</v>
+        <v>549</v>
       </c>
       <c r="E16" s="37" t="s">
         <v>260</v>
       </c>
+      <c r="F16" s="37" t="s">
+        <v>342</v>
+      </c>
       <c r="G16" s="38" t="s">
-        <v>311</v>
+        <v>392</v>
       </c>
       <c r="H16" s="40" t="s">
-        <v>526</v>
+        <v>619</v>
       </c>
       <c r="I16" s="39" t="s">
-        <v>400</v>
+        <v>454</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="K16" s="39" t="s">
-        <v>496</v>
+        <v>576</v>
+      </c>
+      <c r="L16" s="39" t="s">
+        <v>471</v>
       </c>
       <c r="M16" s="39" t="s">
-        <v>341</v>
+        <v>433</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="36" t="s">
-        <v>373</v>
-      </c>
       <c r="C17" s="36" t="s">
-        <v>440</v>
+        <v>522</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>462</v>
+        <v>550</v>
       </c>
       <c r="E17" s="37" t="s">
         <v>261</v>
       </c>
+      <c r="F17" s="37" t="s">
+        <v>343</v>
+      </c>
       <c r="G17" s="38" t="s">
-        <v>312</v>
+        <v>393</v>
       </c>
       <c r="H17" s="40" t="s">
-        <v>527</v>
+        <v>620</v>
       </c>
       <c r="I17" s="39" t="s">
-        <v>401</v>
+        <v>455</v>
       </c>
       <c r="J17" s="39" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="K17" s="39" t="s">
-        <v>497</v>
+        <v>577</v>
+      </c>
+      <c r="L17" s="39" t="s">
+        <v>472</v>
       </c>
       <c r="M17" s="39" t="s">
-        <v>342</v>
+        <v>434</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="36" t="s">
-        <v>374</v>
-      </c>
       <c r="C18" s="36" t="s">
-        <v>441</v>
+        <v>523</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>463</v>
+        <v>551</v>
       </c>
       <c r="E18" s="37" t="s">
         <v>262</v>
       </c>
+      <c r="F18" s="37" t="s">
+        <v>344</v>
+      </c>
       <c r="G18" s="38" t="s">
-        <v>313</v>
+        <v>394</v>
       </c>
       <c r="H18" s="40" t="s">
-        <v>528</v>
+        <v>621</v>
       </c>
       <c r="I18" s="39" t="s">
-        <v>402</v>
+        <v>456</v>
       </c>
       <c r="J18" s="39" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="K18" s="39" t="s">
-        <v>498</v>
+        <v>578</v>
+      </c>
+      <c r="L18" s="39" t="s">
+        <v>473</v>
       </c>
       <c r="M18" s="39" t="s">
-        <v>343</v>
+        <v>435</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="36" t="s">
-        <v>375</v>
-      </c>
       <c r="C19" s="36" t="s">
-        <v>442</v>
+        <v>524</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>464</v>
+        <v>552</v>
       </c>
       <c r="E19" s="37" t="s">
         <v>263</v>
       </c>
+      <c r="F19" s="37" t="s">
+        <v>345</v>
+      </c>
       <c r="G19" s="38" t="s">
-        <v>314</v>
+        <v>395</v>
       </c>
       <c r="H19" s="40" t="s">
-        <v>529</v>
+        <v>622</v>
       </c>
       <c r="I19" s="39" t="s">
-        <v>403</v>
+        <v>457</v>
       </c>
       <c r="J19" s="39" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="K19" s="39" t="s">
-        <v>499</v>
+        <v>579</v>
+      </c>
+      <c r="L19" s="39" t="s">
+        <v>474</v>
       </c>
       <c r="M19" s="39" t="s">
-        <v>344</v>
+        <v>436</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="36" t="s">
-        <v>376</v>
-      </c>
       <c r="C20" s="36" t="s">
-        <v>443</v>
+        <v>525</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>465</v>
+        <v>553</v>
       </c>
       <c r="E20" s="37" t="s">
         <v>264</v>
       </c>
+      <c r="F20" s="37" t="s">
+        <v>346</v>
+      </c>
       <c r="G20" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="H20" s="40" t="s">
-        <v>530</v>
+        <v>396</v>
       </c>
       <c r="I20" s="39" t="s">
-        <v>404</v>
+        <v>458</v>
       </c>
       <c r="J20" s="39" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>500</v>
+        <v>580</v>
+      </c>
+      <c r="L20" s="39" t="s">
+        <v>475</v>
       </c>
       <c r="M20" s="39" t="s">
-        <v>345</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="36" t="s">
-        <v>377</v>
-      </c>
       <c r="C21" s="36" t="s">
-        <v>444</v>
+        <v>526</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>466</v>
+        <v>554</v>
       </c>
       <c r="E21" s="37" t="s">
         <v>265</v>
       </c>
+      <c r="F21" s="37" t="s">
+        <v>347</v>
+      </c>
       <c r="G21" s="38" t="s">
-        <v>316</v>
-      </c>
-      <c r="H21" s="40" t="s">
-        <v>531</v>
+        <v>397</v>
       </c>
       <c r="I21" s="39" t="s">
-        <v>405</v>
+        <v>459</v>
       </c>
       <c r="J21" s="39" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="K21" s="39" t="s">
-        <v>501</v>
+        <v>581</v>
+      </c>
+      <c r="L21" s="39" t="s">
+        <v>476</v>
       </c>
       <c r="M21" s="39" t="s">
-        <v>346</v>
+        <v>438</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="36" t="s">
-        <v>378</v>
-      </c>
       <c r="C22" s="36" t="s">
-        <v>445</v>
+        <v>527</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>467</v>
+        <v>555</v>
       </c>
       <c r="E22" s="37" t="s">
         <v>266</v>
       </c>
+      <c r="F22" s="37" t="s">
+        <v>348</v>
+      </c>
       <c r="G22" s="38" t="s">
-        <v>317</v>
-      </c>
-      <c r="H22" s="40" t="s">
-        <v>532</v>
+        <v>398</v>
       </c>
       <c r="I22" s="39" t="s">
-        <v>406</v>
+        <v>460</v>
       </c>
       <c r="J22" s="39" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="K22" s="39" t="s">
-        <v>502</v>
-      </c>
-      <c r="M22" s="39" t="s">
-        <v>347</v>
+        <v>582</v>
+      </c>
+      <c r="L22" s="39" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="36" t="s">
-        <v>379</v>
-      </c>
       <c r="C23" s="36" t="s">
-        <v>446</v>
+        <v>528</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>468</v>
+        <v>556</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>267</v>
       </c>
+      <c r="F23" s="37" t="s">
+        <v>349</v>
+      </c>
       <c r="G23" s="38" t="s">
-        <v>318</v>
-      </c>
-      <c r="H23" s="40" t="s">
-        <v>533</v>
-      </c>
-      <c r="I23" s="39" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="J23" s="39" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="K23" s="39" t="s">
-        <v>503</v>
-      </c>
-      <c r="M23" s="39" t="s">
-        <v>348</v>
+        <v>583</v>
+      </c>
+      <c r="L23" s="39" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="36" t="s">
-        <v>380</v>
-      </c>
       <c r="C24" s="36" t="s">
-        <v>447</v>
+        <v>529</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>469</v>
+        <v>557</v>
       </c>
       <c r="E24" s="37" t="s">
         <v>268</v>
       </c>
+      <c r="F24" s="37" t="s">
+        <v>350</v>
+      </c>
       <c r="G24" s="38" t="s">
+        <v>400</v>
+      </c>
+      <c r="J24" s="39" t="s">
+        <v>302</v>
+      </c>
+      <c r="K24" s="39" t="s">
+        <v>584</v>
+      </c>
+      <c r="L24" s="39" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="36" t="s">
+        <v>530</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>558</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>351</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>401</v>
+      </c>
+      <c r="J25" s="39" t="s">
+        <v>303</v>
+      </c>
+      <c r="K25" s="39" t="s">
+        <v>585</v>
+      </c>
+      <c r="L25" s="39" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" s="36" t="s">
+        <v>531</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>559</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>352</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>402</v>
+      </c>
+      <c r="J26" s="39" t="s">
+        <v>304</v>
+      </c>
+      <c r="K26" s="39" t="s">
+        <v>586</v>
+      </c>
+      <c r="L26" s="39" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" s="36" t="s">
+        <v>532</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>560</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>353</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>403</v>
+      </c>
+      <c r="J27" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="K27" s="39" t="s">
+        <v>587</v>
+      </c>
+      <c r="L27" s="39" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" s="36" t="s">
+        <v>533</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>561</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>354</v>
+      </c>
+      <c r="G28" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="J28" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="K28" s="39" t="s">
+        <v>588</v>
+      </c>
+      <c r="L28" s="39" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="36" t="s">
+        <v>534</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>562</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>355</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>405</v>
+      </c>
+      <c r="J29" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="K29" s="39" t="s">
+        <v>589</v>
+      </c>
+      <c r="L29" s="39" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" s="36" t="s">
+        <v>535</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>563</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>356</v>
+      </c>
+      <c r="G30" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="J30" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="K30" s="39" t="s">
+        <v>590</v>
+      </c>
+      <c r="L30" s="39" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="36" t="s">
+        <v>536</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>564</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="F31" s="37" t="s">
+        <v>357</v>
+      </c>
+      <c r="G31" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="J31" s="39" t="s">
+        <v>309</v>
+      </c>
+      <c r="K31" s="39" t="s">
+        <v>591</v>
+      </c>
+      <c r="L31" s="39" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" s="36" t="s">
+        <v>537</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>565</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>276</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>358</v>
+      </c>
+      <c r="G32" s="38" t="s">
+        <v>408</v>
+      </c>
+      <c r="J32" s="39" t="s">
+        <v>310</v>
+      </c>
+      <c r="K32" s="39" t="s">
+        <v>592</v>
+      </c>
+      <c r="L32" s="39" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" s="36" t="s">
+        <v>538</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="F33" s="37" t="s">
+        <v>359</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="J33" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="K33" s="39" t="s">
+        <v>593</v>
+      </c>
+      <c r="L33" s="39" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" s="37" t="s">
+        <v>278</v>
+      </c>
+      <c r="F34" s="37" t="s">
+        <v>360</v>
+      </c>
+      <c r="G34" s="38" t="s">
+        <v>410</v>
+      </c>
+      <c r="J34" s="39" t="s">
+        <v>312</v>
+      </c>
+      <c r="K34" s="39" t="s">
+        <v>594</v>
+      </c>
+      <c r="L34" s="39" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="E35" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>361</v>
+      </c>
+      <c r="G35" s="38" t="s">
+        <v>411</v>
+      </c>
+      <c r="J35" s="39" t="s">
+        <v>313</v>
+      </c>
+      <c r="K35" s="39" t="s">
+        <v>595</v>
+      </c>
+      <c r="L35" s="39" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="E36" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="F36" s="37" t="s">
+        <v>362</v>
+      </c>
+      <c r="G36" s="38" t="s">
+        <v>412</v>
+      </c>
+      <c r="J36" s="39" t="s">
+        <v>314</v>
+      </c>
+      <c r="K36" s="39" t="s">
+        <v>596</v>
+      </c>
+      <c r="L36" s="39" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="E37" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="F37" s="37" t="s">
+        <v>363</v>
+      </c>
+      <c r="G37" s="38" t="s">
+        <v>413</v>
+      </c>
+      <c r="J37" s="39" t="s">
+        <v>315</v>
+      </c>
+      <c r="K37" s="39" t="s">
+        <v>597</v>
+      </c>
+      <c r="L37" s="39" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="E38" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="F38" s="37" t="s">
+        <v>364</v>
+      </c>
+      <c r="G38" s="38" t="s">
+        <v>414</v>
+      </c>
+      <c r="J38" s="39" t="s">
+        <v>316</v>
+      </c>
+      <c r="K38" s="39" t="s">
+        <v>598</v>
+      </c>
+      <c r="L38" s="39" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="F39" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="G39" s="38" t="s">
+        <v>415</v>
+      </c>
+      <c r="J39" s="39" t="s">
+        <v>317</v>
+      </c>
+      <c r="K39" s="39" t="s">
+        <v>599</v>
+      </c>
+      <c r="L39" s="39" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="F40" s="37" t="s">
+        <v>366</v>
+      </c>
+      <c r="G40" s="38" t="s">
+        <v>416</v>
+      </c>
+      <c r="J40" s="39" t="s">
+        <v>318</v>
+      </c>
+      <c r="K40" s="39" t="s">
+        <v>600</v>
+      </c>
+      <c r="L40" s="39" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="F41" s="37" t="s">
+        <v>367</v>
+      </c>
+      <c r="G41" s="38" t="s">
+        <v>417</v>
+      </c>
+      <c r="J41" s="39" t="s">
         <v>319</v>
       </c>
-      <c r="H24" s="40" t="s">
-        <v>534</v>
-      </c>
-      <c r="I24" s="39" t="s">
-        <v>408</v>
-      </c>
-      <c r="J24" s="39" t="s">
-        <v>288</v>
-      </c>
-      <c r="K24" s="39" t="s">
+      <c r="K41" s="39" t="s">
+        <v>601</v>
+      </c>
+      <c r="L41" s="39" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="F42" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="G42" s="38" t="s">
+        <v>418</v>
+      </c>
+      <c r="J42" s="39" t="s">
+        <v>320</v>
+      </c>
+      <c r="K42" s="39" t="s">
+        <v>602</v>
+      </c>
+      <c r="L42" s="39" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="F43" s="37" t="s">
+        <v>369</v>
+      </c>
+      <c r="G43" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="J43" s="39" t="s">
+        <v>321</v>
+      </c>
+      <c r="K43" s="39" t="s">
+        <v>603</v>
+      </c>
+      <c r="L43" s="39" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="F44" s="37" t="s">
+        <v>370</v>
+      </c>
+      <c r="G44" s="38" t="s">
+        <v>420</v>
+      </c>
+      <c r="J44" s="39" t="s">
+        <v>322</v>
+      </c>
+      <c r="K44" s="39" t="s">
+        <v>604</v>
+      </c>
+      <c r="L44" s="39" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="F45" s="37" t="s">
+        <v>371</v>
+      </c>
+      <c r="G45" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="J45" s="39" t="s">
+        <v>323</v>
+      </c>
+      <c r="K45" s="39" t="s">
+        <v>605</v>
+      </c>
+      <c r="L45" s="39" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="F46" s="37" t="s">
+        <v>372</v>
+      </c>
+      <c r="G46" s="38" t="s">
+        <v>422</v>
+      </c>
+      <c r="J46" s="39" t="s">
+        <v>324</v>
+      </c>
+      <c r="K46" s="39" t="s">
+        <v>606</v>
+      </c>
+      <c r="L46" s="39" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="F47" s="37" t="s">
+        <v>373</v>
+      </c>
+      <c r="J47" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="K47" s="39" t="s">
+        <v>607</v>
+      </c>
+      <c r="L47" s="39" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="F48" s="37" t="s">
+        <v>374</v>
+      </c>
+      <c r="J48" s="39" t="s">
+        <v>326</v>
+      </c>
+      <c r="K48" s="39" t="s">
+        <v>608</v>
+      </c>
+      <c r="L48" s="39" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="F49" s="37" t="s">
+        <v>375</v>
+      </c>
+      <c r="J49" s="39" t="s">
+        <v>327</v>
+      </c>
+      <c r="L49" s="39" t="s">
         <v>504</v>
       </c>
-      <c r="M24" s="39" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="36" t="s">
-        <v>381</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>448</v>
-      </c>
-      <c r="D25" s="36" t="s">
-        <v>470</v>
-      </c>
-      <c r="G25" s="38" t="s">
-        <v>320</v>
-      </c>
-      <c r="H25" s="40" t="s">
-        <v>535</v>
-      </c>
-      <c r="I25" s="39" t="s">
-        <v>409</v>
-      </c>
-      <c r="J25" s="39" t="s">
-        <v>289</v>
-      </c>
-      <c r="K25" s="39" t="s">
+    </row>
+    <row r="50">
+      <c r="F50" s="37" t="s">
+        <v>376</v>
+      </c>
+      <c r="J50" s="39" t="s">
+        <v>328</v>
+      </c>
+      <c r="L50" s="39" t="s">
         <v>505</v>
       </c>
-      <c r="M25" s="39" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="36" t="s">
-        <v>382</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>449</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>471</v>
-      </c>
-      <c r="G26" s="38" t="s">
-        <v>321</v>
-      </c>
-      <c r="H26" s="40" t="s">
-        <v>536</v>
-      </c>
-      <c r="I26" s="39" t="s">
-        <v>410</v>
-      </c>
-      <c r="J26" s="39" t="s">
-        <v>290</v>
-      </c>
-      <c r="K26" s="39" t="s">
+    </row>
+    <row r="51">
+      <c r="F51" s="37" t="s">
+        <v>377</v>
+      </c>
+      <c r="J51" s="39" t="s">
+        <v>329</v>
+      </c>
+      <c r="L51" s="39" t="s">
         <v>506</v>
       </c>
-      <c r="M26" s="39" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="36" t="s">
-        <v>383</v>
-      </c>
-      <c r="C27" s="36" t="s">
-        <v>450</v>
-      </c>
-      <c r="D27" s="36" t="s">
-        <v>472</v>
-      </c>
-      <c r="G27" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="H27" s="40" t="s">
-        <v>537</v>
-      </c>
-      <c r="I27" s="39" t="s">
-        <v>411</v>
-      </c>
-      <c r="J27" s="39" t="s">
-        <v>291</v>
-      </c>
-      <c r="K27" s="39" t="s">
+    </row>
+    <row r="52">
+      <c r="F52" s="37" t="s">
+        <v>378</v>
+      </c>
+      <c r="J52" s="39" t="s">
+        <v>330</v>
+      </c>
+      <c r="L52" s="39" t="s">
         <v>507</v>
       </c>
-      <c r="M27" s="39" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="36" t="s">
-        <v>384</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>473</v>
-      </c>
-      <c r="G28" s="38" t="s">
-        <v>323</v>
-      </c>
-      <c r="H28" s="40" t="s">
-        <v>538</v>
-      </c>
-      <c r="I28" s="39" t="s">
-        <v>412</v>
-      </c>
-      <c r="J28" s="39" t="s">
-        <v>292</v>
-      </c>
-      <c r="K28" s="39" t="s">
+    </row>
+    <row r="53">
+      <c r="F53" s="37" t="s">
+        <v>379</v>
+      </c>
+      <c r="L53" s="39" t="s">
         <v>508</v>
       </c>
-      <c r="M28" s="39" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="36" t="s">
-        <v>385</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>474</v>
-      </c>
-      <c r="G29" s="38" t="s">
-        <v>324</v>
-      </c>
-      <c r="H29" s="40" t="s">
-        <v>539</v>
-      </c>
-      <c r="I29" s="39" t="s">
-        <v>413</v>
-      </c>
-      <c r="K29" s="39" t="s">
+    </row>
+    <row r="54">
+      <c r="F54" s="37" t="s">
+        <v>380</v>
+      </c>
+      <c r="L54" s="39" t="s">
         <v>509</v>
       </c>
-      <c r="M29" s="39" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" s="36" t="s">
-        <v>386</v>
-      </c>
-      <c r="D30" s="36" t="s">
-        <v>475</v>
-      </c>
-      <c r="G30" s="38" t="s">
-        <v>325</v>
-      </c>
-      <c r="H30" s="40" t="s">
-        <v>540</v>
-      </c>
-      <c r="I30" s="39" t="s">
-        <v>414</v>
-      </c>
-      <c r="K30" s="39" t="s">
+    </row>
+    <row r="55">
+      <c r="L55" s="39" t="s">
         <v>510</v>
-      </c>
-      <c r="M30" s="39" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="36" t="s">
-        <v>387</v>
-      </c>
-      <c r="D31" s="36" t="s">
-        <v>476</v>
-      </c>
-      <c r="G31" s="38" t="s">
-        <v>326</v>
-      </c>
-      <c r="H31" s="40" t="s">
-        <v>541</v>
-      </c>
-      <c r="I31" s="39" t="s">
-        <v>415</v>
-      </c>
-      <c r="K31" s="39" t="s">
-        <v>511</v>
-      </c>
-      <c r="M31" s="39" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" s="36" t="s">
-        <v>388</v>
-      </c>
-      <c r="D32" s="36" t="s">
-        <v>477</v>
-      </c>
-      <c r="G32" s="38" t="s">
-        <v>327</v>
-      </c>
-      <c r="H32" s="40" t="s">
-        <v>542</v>
-      </c>
-      <c r="I32" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="K32" s="39" t="s">
-        <v>512</v>
-      </c>
-      <c r="M32" s="39" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" s="36" t="s">
-        <v>389</v>
-      </c>
-      <c r="D33" s="36" t="s">
-        <v>478</v>
-      </c>
-      <c r="G33" s="38" t="s">
-        <v>328</v>
-      </c>
-      <c r="H33" s="40" t="s">
-        <v>543</v>
-      </c>
-      <c r="I33" s="39" t="s">
-        <v>417</v>
-      </c>
-      <c r="K33" s="39" t="s">
-        <v>513</v>
-      </c>
-      <c r="M33" s="39" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" s="36" t="s">
-        <v>479</v>
-      </c>
-      <c r="G34" s="38" t="s">
-        <v>329</v>
-      </c>
-      <c r="H34" s="40" t="s">
-        <v>544</v>
-      </c>
-      <c r="I34" s="39" t="s">
-        <v>418</v>
-      </c>
-      <c r="K34" s="39" t="s">
-        <v>514</v>
-      </c>
-      <c r="M34" s="39" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" s="36" t="s">
-        <v>480</v>
-      </c>
-      <c r="H35" s="40" t="s">
-        <v>545</v>
-      </c>
-      <c r="I35" s="39" t="s">
-        <v>419</v>
-      </c>
-      <c r="K35" s="39" t="s">
-        <v>515</v>
-      </c>
-      <c r="M35" s="39" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="D36" s="36" t="s">
-        <v>481</v>
-      </c>
-      <c r="H36" s="40" t="s">
-        <v>546</v>
-      </c>
-      <c r="I36" s="39" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="D37" s="36" t="s">
-        <v>482</v>
-      </c>
-      <c r="H37" s="40" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="D38" s="36" t="s">
-        <v>483</v>
-      </c>
-      <c r="H38" s="40" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="D39" s="36" t="s">
-        <v>484</v>
-      </c>
-      <c r="H39" s="40" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="H40" s="40" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="H41" s="40" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="H42" s="40" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="H43" s="40" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="H44" s="40" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="H45" s="40" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="H46" s="40" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="H47" s="40" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="H48" s="40" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="H49" s="40" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="H50" s="40" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="H51" s="40" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="H52" s="40" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="H53" s="40" t="s">
-        <v>563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check read / write of range ref
</commit_message>
<xml_diff>
--- a/X-Domestic Standard Upload.xlsx
+++ b/X-Domestic Standard Upload.xlsx
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="514">
   <si>
     <t>#</t>
   </si>
@@ -1144,105 +1144,6 @@
     <t>col:0</t>
   </si>
   <si>
-    <t>col:1</t>
-  </si>
-  <si>
-    <t>col:2</t>
-  </si>
-  <si>
-    <t>col:3</t>
-  </si>
-  <si>
-    <t>col:4</t>
-  </si>
-  <si>
-    <t>col:5</t>
-  </si>
-  <si>
-    <t>col:6</t>
-  </si>
-  <si>
-    <t>col:7</t>
-  </si>
-  <si>
-    <t>col:8</t>
-  </si>
-  <si>
-    <t>col:9</t>
-  </si>
-  <si>
-    <t>col:10</t>
-  </si>
-  <si>
-    <t>col:11</t>
-  </si>
-  <si>
-    <t>col:12</t>
-  </si>
-  <si>
-    <t>col:13</t>
-  </si>
-  <si>
-    <t>col:14</t>
-  </si>
-  <si>
-    <t>col:15</t>
-  </si>
-  <si>
-    <t>col:16</t>
-  </si>
-  <si>
-    <t>col:17</t>
-  </si>
-  <si>
-    <t>col:18</t>
-  </si>
-  <si>
-    <t>col:19</t>
-  </si>
-  <si>
-    <t>col:20</t>
-  </si>
-  <si>
-    <t>col:21</t>
-  </si>
-  <si>
-    <t>col:22</t>
-  </si>
-  <si>
-    <t>col:23</t>
-  </si>
-  <si>
-    <t>col:24</t>
-  </si>
-  <si>
-    <t>col:25</t>
-  </si>
-  <si>
-    <t>col:26</t>
-  </si>
-  <si>
-    <t>col:27</t>
-  </si>
-  <si>
-    <t>col:28</t>
-  </si>
-  <si>
-    <t>col:29</t>
-  </si>
-  <si>
-    <t>col:30</t>
-  </si>
-  <si>
-    <t>col:31</t>
-  </si>
-  <si>
-    <t>col:32</t>
-  </si>
-  <si>
-    <t>col:33</t>
-  </si>
-  <si>
     <t>dep:0</t>
   </si>
   <si>
@@ -1351,42 +1252,6 @@
     <t>dep:35</t>
   </si>
   <si>
-    <t>dep:36</t>
-  </si>
-  <si>
-    <t>dep:37</t>
-  </si>
-  <si>
-    <t>dep:38</t>
-  </si>
-  <si>
-    <t>dep:39</t>
-  </si>
-  <si>
-    <t>dep:40</t>
-  </si>
-  <si>
-    <t>dep:41</t>
-  </si>
-  <si>
-    <t>dep:42</t>
-  </si>
-  <si>
-    <t>dep:43</t>
-  </si>
-  <si>
-    <t>dep:44</t>
-  </si>
-  <si>
-    <t>dep:45</t>
-  </si>
-  <si>
-    <t>dep:46</t>
-  </si>
-  <si>
-    <t>dep:47</t>
-  </si>
-  <si>
     <t>siz:0</t>
   </si>
   <si>
@@ -1456,87 +1321,6 @@
     <t>siz:22</t>
   </si>
   <si>
-    <t>siz:23</t>
-  </si>
-  <si>
-    <t>siz:24</t>
-  </si>
-  <si>
-    <t>siz:25</t>
-  </si>
-  <si>
-    <t>siz:26</t>
-  </si>
-  <si>
-    <t>siz:27</t>
-  </si>
-  <si>
-    <t>siz:28</t>
-  </si>
-  <si>
-    <t>siz:29</t>
-  </si>
-  <si>
-    <t>siz:30</t>
-  </si>
-  <si>
-    <t>siz:31</t>
-  </si>
-  <si>
-    <t>siz:32</t>
-  </si>
-  <si>
-    <t>siz:33</t>
-  </si>
-  <si>
-    <t>siz:34</t>
-  </si>
-  <si>
-    <t>siz:35</t>
-  </si>
-  <si>
-    <t>siz:36</t>
-  </si>
-  <si>
-    <t>siz:37</t>
-  </si>
-  <si>
-    <t>siz:38</t>
-  </si>
-  <si>
-    <t>siz:39</t>
-  </si>
-  <si>
-    <t>siz:40</t>
-  </si>
-  <si>
-    <t>siz:41</t>
-  </si>
-  <si>
-    <t>siz:42</t>
-  </si>
-  <si>
-    <t>siz:43</t>
-  </si>
-  <si>
-    <t>siz:44</t>
-  </si>
-  <si>
-    <t>siz:45</t>
-  </si>
-  <si>
-    <t>siz:46</t>
-  </si>
-  <si>
-    <t>siz:47</t>
-  </si>
-  <si>
-    <t>siz:48</t>
-  </si>
-  <si>
-    <t>siz:49</t>
-  </si>
-  <si>
     <t>typ:0</t>
   </si>
   <si>
@@ -1597,69 +1381,6 @@
     <t>typ:19</t>
   </si>
   <si>
-    <t>typ:20</t>
-  </si>
-  <si>
-    <t>typ:21</t>
-  </si>
-  <si>
-    <t>typ:22</t>
-  </si>
-  <si>
-    <t>typ:23</t>
-  </si>
-  <si>
-    <t>typ:24</t>
-  </si>
-  <si>
-    <t>typ:25</t>
-  </si>
-  <si>
-    <t>typ:26</t>
-  </si>
-  <si>
-    <t>typ:27</t>
-  </si>
-  <si>
-    <t>typ:28</t>
-  </si>
-  <si>
-    <t>typ:29</t>
-  </si>
-  <si>
-    <t>typ:30</t>
-  </si>
-  <si>
-    <t>typ:31</t>
-  </si>
-  <si>
-    <t>typ:32</t>
-  </si>
-  <si>
-    <t>typ:33</t>
-  </si>
-  <si>
-    <t>typ:34</t>
-  </si>
-  <si>
-    <t>typ:35</t>
-  </si>
-  <si>
-    <t>typ:36</t>
-  </si>
-  <si>
-    <t>typ:37</t>
-  </si>
-  <si>
-    <t>typ:38</t>
-  </si>
-  <si>
-    <t>typ:39</t>
-  </si>
-  <si>
-    <t>typ:40</t>
-  </si>
-  <si>
     <t>mat:0</t>
   </si>
   <si>
@@ -1708,6 +1429,156 @@
     <t>mat:15</t>
   </si>
   <si>
+    <t>mat:16</t>
+  </si>
+  <si>
+    <t>mat:17</t>
+  </si>
+  <si>
+    <t>mat:18</t>
+  </si>
+  <si>
+    <t>mat:19</t>
+  </si>
+  <si>
+    <t>mat:20</t>
+  </si>
+  <si>
+    <t>mat:21</t>
+  </si>
+  <si>
+    <t>mat:22</t>
+  </si>
+  <si>
+    <t>mat:23</t>
+  </si>
+  <si>
+    <t>mat:24</t>
+  </si>
+  <si>
+    <t>mat:25</t>
+  </si>
+  <si>
+    <t>mat:26</t>
+  </si>
+  <si>
+    <t>mat:27</t>
+  </si>
+  <si>
+    <t>mat:28</t>
+  </si>
+  <si>
+    <t>mat:29</t>
+  </si>
+  <si>
+    <t>mat:30</t>
+  </si>
+  <si>
+    <t>mat:31</t>
+  </si>
+  <si>
+    <t>mat:32</t>
+  </si>
+  <si>
+    <t>mat:33</t>
+  </si>
+  <si>
+    <t>mat:34</t>
+  </si>
+  <si>
+    <t>mat:35</t>
+  </si>
+  <si>
+    <t>wei:0</t>
+  </si>
+  <si>
+    <t>wei:1</t>
+  </si>
+  <si>
+    <t>wei:2</t>
+  </si>
+  <si>
+    <t>wei:3</t>
+  </si>
+  <si>
+    <t>wei:4</t>
+  </si>
+  <si>
+    <t>wei:5</t>
+  </si>
+  <si>
+    <t>wei:6</t>
+  </si>
+  <si>
+    <t>wei:7</t>
+  </si>
+  <si>
+    <t>wei:8</t>
+  </si>
+  <si>
+    <t>wei:9</t>
+  </si>
+  <si>
+    <t>wei:10</t>
+  </si>
+  <si>
+    <t>wei:11</t>
+  </si>
+  <si>
+    <t>wei:12</t>
+  </si>
+  <si>
+    <t>wei:13</t>
+  </si>
+  <si>
+    <t>wei:14</t>
+  </si>
+  <si>
+    <t>wei:15</t>
+  </si>
+  <si>
+    <t>wei:16</t>
+  </si>
+  <si>
+    <t>wei:17</t>
+  </si>
+  <si>
+    <t>wei:18</t>
+  </si>
+  <si>
+    <t>wei:19</t>
+  </si>
+  <si>
+    <t>wei:20</t>
+  </si>
+  <si>
+    <t>wei:21</t>
+  </si>
+  <si>
+    <t>wei:22</t>
+  </si>
+  <si>
+    <t>wei:23</t>
+  </si>
+  <si>
+    <t>wei:24</t>
+  </si>
+  <si>
+    <t>wei:25</t>
+  </si>
+  <si>
+    <t>wei:26</t>
+  </si>
+  <si>
+    <t>wei:27</t>
+  </si>
+  <si>
+    <t>wei:28</t>
+  </si>
+  <si>
+    <t>wei:29</t>
+  </si>
+  <si>
     <t>vpn:0</t>
   </si>
   <si>
@@ -1720,9 +1591,6 @@
     <t>vpn:3</t>
   </si>
   <si>
-    <t>vpn:4</t>
-  </si>
-  <si>
     <t>sup:0</t>
   </si>
   <si>
@@ -1774,6 +1642,33 @@
     <t>sup:16</t>
   </si>
   <si>
+    <t>sup:17</t>
+  </si>
+  <si>
+    <t>sup:18</t>
+  </si>
+  <si>
+    <t>sup:19</t>
+  </si>
+  <si>
+    <t>sup:20</t>
+  </si>
+  <si>
+    <t>sup:21</t>
+  </si>
+  <si>
+    <t>sup:22</t>
+  </si>
+  <si>
+    <t>sup:23</t>
+  </si>
+  <si>
+    <t>sup:24</t>
+  </si>
+  <si>
+    <t>sup:25</t>
+  </si>
+  <si>
     <t>cat:0</t>
   </si>
   <si>
@@ -1822,108 +1717,6 @@
     <t>cat:15</t>
   </si>
   <si>
-    <t>cat:16</t>
-  </si>
-  <si>
-    <t>cat:17</t>
-  </si>
-  <si>
-    <t>cat:18</t>
-  </si>
-  <si>
-    <t>cat:19</t>
-  </si>
-  <si>
-    <t>cat:20</t>
-  </si>
-  <si>
-    <t>cat:21</t>
-  </si>
-  <si>
-    <t>cat:22</t>
-  </si>
-  <si>
-    <t>cat:23</t>
-  </si>
-  <si>
-    <t>cat:24</t>
-  </si>
-  <si>
-    <t>cat:25</t>
-  </si>
-  <si>
-    <t>cat:26</t>
-  </si>
-  <si>
-    <t>cat:27</t>
-  </si>
-  <si>
-    <t>cat:28</t>
-  </si>
-  <si>
-    <t>cat:29</t>
-  </si>
-  <si>
-    <t>cat:30</t>
-  </si>
-  <si>
-    <t>cat:31</t>
-  </si>
-  <si>
-    <t>cat:32</t>
-  </si>
-  <si>
-    <t>cat:33</t>
-  </si>
-  <si>
-    <t>cat:34</t>
-  </si>
-  <si>
-    <t>cat:35</t>
-  </si>
-  <si>
-    <t>cat:36</t>
-  </si>
-  <si>
-    <t>cat:37</t>
-  </si>
-  <si>
-    <t>cat:38</t>
-  </si>
-  <si>
-    <t>cat:39</t>
-  </si>
-  <si>
-    <t>cat:40</t>
-  </si>
-  <si>
-    <t>cat:41</t>
-  </si>
-  <si>
-    <t>cat:42</t>
-  </si>
-  <si>
-    <t>cat:43</t>
-  </si>
-  <si>
-    <t>cat:44</t>
-  </si>
-  <si>
-    <t>cat:45</t>
-  </si>
-  <si>
-    <t>cat:46</t>
-  </si>
-  <si>
-    <t>cat:47</t>
-  </si>
-  <si>
-    <t>cat:48</t>
-  </si>
-  <si>
-    <t>cat:49</t>
-  </si>
-  <si>
     <t>ven:0</t>
   </si>
   <si>
@@ -1978,36 +1771,6 @@
     <t>ven:17</t>
   </si>
   <si>
-    <t>ven:18</t>
-  </si>
-  <si>
-    <t>ven:19</t>
-  </si>
-  <si>
-    <t>ven:20</t>
-  </si>
-  <si>
-    <t>ven:21</t>
-  </si>
-  <si>
-    <t>ven:22</t>
-  </si>
-  <si>
-    <t>ven:23</t>
-  </si>
-  <si>
-    <t>ven:24</t>
-  </si>
-  <si>
-    <t>ven:25</t>
-  </si>
-  <si>
-    <t>ven:26</t>
-  </si>
-  <si>
-    <t>ven:27</t>
-  </si>
-  <si>
     <t>lab:0</t>
   </si>
   <si>
@@ -2074,21 +1837,6 @@
     <t>lab:21</t>
   </si>
   <si>
-    <t>lab:22</t>
-  </si>
-  <si>
-    <t>lab:23</t>
-  </si>
-  <si>
-    <t>lab:24</t>
-  </si>
-  <si>
-    <t>lab:25</t>
-  </si>
-  <si>
-    <t>lab:26</t>
-  </si>
-  <si>
     <t>cla:0</t>
   </si>
   <si>
@@ -2161,63 +1909,6 @@
     <t>cla:23</t>
   </si>
   <si>
-    <t>cla:24</t>
-  </si>
-  <si>
-    <t>cla:25</t>
-  </si>
-  <si>
-    <t>cla:26</t>
-  </si>
-  <si>
-    <t>cla:27</t>
-  </si>
-  <si>
-    <t>cla:28</t>
-  </si>
-  <si>
-    <t>cla:29</t>
-  </si>
-  <si>
-    <t>cla:30</t>
-  </si>
-  <si>
-    <t>cla:31</t>
-  </si>
-  <si>
-    <t>cla:32</t>
-  </si>
-  <si>
-    <t>cla:33</t>
-  </si>
-  <si>
-    <t>cla:34</t>
-  </si>
-  <si>
-    <t>cla:35</t>
-  </si>
-  <si>
-    <t>cla:36</t>
-  </si>
-  <si>
-    <t>cla:37</t>
-  </si>
-  <si>
-    <t>cla:38</t>
-  </si>
-  <si>
-    <t>cla:39</t>
-  </si>
-  <si>
-    <t>cla:40</t>
-  </si>
-  <si>
-    <t>cla:41</t>
-  </si>
-  <si>
-    <t>cla:42</t>
-  </si>
-  <si>
     <t>pon:0</t>
   </si>
   <si>
@@ -2240,24 +1931,6 @@
   </si>
   <si>
     <t>pon:7</t>
-  </si>
-  <si>
-    <t>pon:8</t>
-  </si>
-  <si>
-    <t>pon:9</t>
-  </si>
-  <si>
-    <t>pon:10</t>
-  </si>
-  <si>
-    <t>pon:11</t>
-  </si>
-  <si>
-    <t>pon:12</t>
-  </si>
-  <si>
-    <t>pon:13</t>
   </si>
 </sst>
 </file>
@@ -6714,7 +6387,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A17F3EB-F212-417F-BA00-A3FB97B2BF77}">
-  <dimension ref="A1:CV55"/>
+  <dimension ref="A1:CV41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
@@ -8019,7 +7692,9 @@
       <c r="Z5" s="50"/>
       <c r="AA5" s="50"/>
       <c r="AB5" s="50"/>
-      <c r="AC5" s="50"/>
+      <c r="AC5" s="39" t="s">
+        <v>366</v>
+      </c>
       <c r="AD5" s="50"/>
       <c r="AE5" s="50"/>
       <c r="AF5" s="50"/>
@@ -8094,1212 +7769,857 @@
     </row>
     <row r="6">
       <c r="B6" s="36" t="s">
-        <v>439</v>
+        <v>396</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>511</v>
+        <v>442</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>539</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>250</v>
+        <v>460</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>332</v>
+        <v>287</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>382</v>
+        <v>310</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>609</v>
+        <v>506</v>
       </c>
       <c r="I6" s="39" t="s">
-        <v>444</v>
+        <v>400</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="K6" s="39" t="s">
-        <v>566</v>
+        <v>482</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>461</v>
+        <v>426</v>
       </c>
       <c r="M6" s="39" t="s">
-        <v>423</v>
+        <v>330</v>
+      </c>
+      <c r="AC6" s="39" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="36" t="s">
-        <v>440</v>
+        <v>397</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>512</v>
+        <v>443</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>540</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>251</v>
+        <v>461</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>333</v>
+        <v>288</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>383</v>
+        <v>311</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>610</v>
+        <v>507</v>
       </c>
       <c r="I7" s="39" t="s">
-        <v>445</v>
+        <v>401</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>285</v>
+        <v>252</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>567</v>
+        <v>483</v>
       </c>
       <c r="L7" s="39" t="s">
-        <v>462</v>
+        <v>427</v>
       </c>
       <c r="M7" s="39" t="s">
-        <v>424</v>
+        <v>331</v>
+      </c>
+      <c r="AC7" s="39" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="36" t="s">
-        <v>441</v>
+        <v>398</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>513</v>
+        <v>444</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>541</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>252</v>
+        <v>462</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>334</v>
+        <v>289</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>384</v>
+        <v>312</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>611</v>
+        <v>508</v>
       </c>
       <c r="I8" s="39" t="s">
-        <v>446</v>
+        <v>402</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>286</v>
+        <v>253</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>568</v>
+        <v>484</v>
       </c>
       <c r="L8" s="39" t="s">
-        <v>463</v>
+        <v>428</v>
       </c>
       <c r="M8" s="39" t="s">
-        <v>425</v>
+        <v>332</v>
+      </c>
+      <c r="AC8" s="39" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="36" t="s">
-        <v>442</v>
+        <v>399</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>514</v>
+        <v>445</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>542</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>253</v>
+        <v>463</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>335</v>
+        <v>290</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>385</v>
+        <v>313</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>612</v>
+        <v>509</v>
       </c>
       <c r="I9" s="39" t="s">
-        <v>447</v>
+        <v>403</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="K9" s="39" t="s">
-        <v>569</v>
+        <v>485</v>
       </c>
       <c r="L9" s="39" t="s">
+        <v>429</v>
+      </c>
+      <c r="M9" s="39" t="s">
+        <v>333</v>
+      </c>
+      <c r="AC9" s="39" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="36" t="s">
+        <v>446</v>
+      </c>
+      <c r="D10" s="36" t="s">
         <v>464</v>
       </c>
-      <c r="M9" s="39" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="36" t="s">
-        <v>443</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>515</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>543</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>254</v>
-      </c>
       <c r="F10" s="37" t="s">
-        <v>336</v>
+        <v>291</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>386</v>
+        <v>314</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>613</v>
+        <v>510</v>
       </c>
       <c r="I10" s="39" t="s">
-        <v>448</v>
+        <v>404</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>288</v>
+        <v>255</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>570</v>
+        <v>486</v>
       </c>
       <c r="L10" s="39" t="s">
-        <v>465</v>
+        <v>430</v>
       </c>
       <c r="M10" s="39" t="s">
-        <v>427</v>
+        <v>334</v>
+      </c>
+      <c r="AC10" s="39" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="11">
       <c r="C11" s="36" t="s">
-        <v>516</v>
+        <v>447</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>544</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>255</v>
+        <v>465</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>337</v>
+        <v>292</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>387</v>
+        <v>315</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>614</v>
+        <v>511</v>
       </c>
       <c r="I11" s="39" t="s">
-        <v>449</v>
+        <v>405</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>289</v>
+        <v>256</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>571</v>
+        <v>487</v>
       </c>
       <c r="L11" s="39" t="s">
-        <v>466</v>
+        <v>431</v>
       </c>
       <c r="M11" s="39" t="s">
-        <v>428</v>
+        <v>335</v>
+      </c>
+      <c r="AC11" s="39" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="12">
       <c r="C12" s="36" t="s">
-        <v>517</v>
+        <v>448</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>545</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>256</v>
+        <v>466</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>338</v>
+        <v>293</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>388</v>
+        <v>316</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>615</v>
+        <v>512</v>
       </c>
       <c r="I12" s="39" t="s">
-        <v>450</v>
+        <v>406</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>290</v>
+        <v>257</v>
       </c>
       <c r="K12" s="39" t="s">
-        <v>572</v>
+        <v>488</v>
       </c>
       <c r="L12" s="39" t="s">
-        <v>467</v>
+        <v>432</v>
       </c>
       <c r="M12" s="39" t="s">
-        <v>429</v>
+        <v>336</v>
+      </c>
+      <c r="AC12" s="39" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="36" t="s">
-        <v>518</v>
+        <v>449</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>546</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>257</v>
+        <v>467</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>339</v>
+        <v>294</v>
       </c>
       <c r="G13" s="38" t="s">
-        <v>389</v>
+        <v>317</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>616</v>
+        <v>513</v>
       </c>
       <c r="I13" s="39" t="s">
-        <v>451</v>
+        <v>407</v>
       </c>
       <c r="J13" s="39" t="s">
-        <v>291</v>
+        <v>258</v>
       </c>
       <c r="K13" s="39" t="s">
-        <v>573</v>
+        <v>489</v>
       </c>
       <c r="L13" s="39" t="s">
-        <v>468</v>
+        <v>433</v>
       </c>
       <c r="M13" s="39" t="s">
-        <v>430</v>
+        <v>337</v>
+      </c>
+      <c r="AC13" s="39" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="14">
       <c r="C14" s="36" t="s">
-        <v>519</v>
+        <v>450</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>547</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>258</v>
+        <v>468</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>340</v>
+        <v>295</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>390</v>
-      </c>
-      <c r="H14" s="40" t="s">
-        <v>617</v>
+        <v>318</v>
       </c>
       <c r="I14" s="39" t="s">
-        <v>452</v>
+        <v>408</v>
       </c>
       <c r="J14" s="39" t="s">
-        <v>292</v>
+        <v>259</v>
       </c>
       <c r="K14" s="39" t="s">
-        <v>574</v>
+        <v>490</v>
       </c>
       <c r="L14" s="39" t="s">
-        <v>469</v>
+        <v>434</v>
       </c>
       <c r="M14" s="39" t="s">
-        <v>431</v>
+        <v>338</v>
+      </c>
+      <c r="AC14" s="39" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="36" t="s">
-        <v>520</v>
+        <v>451</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>548</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>259</v>
+        <v>469</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>341</v>
+        <v>296</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>391</v>
-      </c>
-      <c r="H15" s="40" t="s">
-        <v>618</v>
+        <v>319</v>
       </c>
       <c r="I15" s="39" t="s">
-        <v>453</v>
+        <v>409</v>
       </c>
       <c r="J15" s="39" t="s">
-        <v>293</v>
+        <v>260</v>
       </c>
       <c r="K15" s="39" t="s">
-        <v>575</v>
+        <v>491</v>
       </c>
       <c r="L15" s="39" t="s">
-        <v>470</v>
+        <v>435</v>
       </c>
       <c r="M15" s="39" t="s">
-        <v>432</v>
+        <v>339</v>
+      </c>
+      <c r="AC15" s="39" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="36" t="s">
-        <v>521</v>
+        <v>452</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>549</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>260</v>
+        <v>470</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>342</v>
+        <v>297</v>
       </c>
       <c r="G16" s="38" t="s">
-        <v>392</v>
-      </c>
-      <c r="H16" s="40" t="s">
-        <v>619</v>
+        <v>320</v>
       </c>
       <c r="I16" s="39" t="s">
-        <v>454</v>
+        <v>410</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>294</v>
+        <v>261</v>
       </c>
       <c r="K16" s="39" t="s">
-        <v>576</v>
+        <v>492</v>
       </c>
       <c r="L16" s="39" t="s">
-        <v>471</v>
+        <v>436</v>
       </c>
       <c r="M16" s="39" t="s">
-        <v>433</v>
+        <v>340</v>
+      </c>
+      <c r="AC16" s="39" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="17">
       <c r="C17" s="36" t="s">
-        <v>522</v>
+        <v>453</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>550</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>261</v>
+        <v>471</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>343</v>
+        <v>298</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>393</v>
-      </c>
-      <c r="H17" s="40" t="s">
-        <v>620</v>
+        <v>321</v>
       </c>
       <c r="I17" s="39" t="s">
-        <v>455</v>
+        <v>411</v>
       </c>
       <c r="J17" s="39" t="s">
-        <v>295</v>
+        <v>262</v>
       </c>
       <c r="K17" s="39" t="s">
-        <v>577</v>
+        <v>493</v>
       </c>
       <c r="L17" s="39" t="s">
-        <v>472</v>
+        <v>437</v>
       </c>
       <c r="M17" s="39" t="s">
-        <v>434</v>
+        <v>341</v>
+      </c>
+      <c r="AC17" s="39" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" s="36" t="s">
-        <v>523</v>
+        <v>454</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>551</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>262</v>
+        <v>472</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>344</v>
+        <v>299</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>394</v>
-      </c>
-      <c r="H18" s="40" t="s">
-        <v>621</v>
+        <v>322</v>
       </c>
       <c r="I18" s="39" t="s">
-        <v>456</v>
+        <v>412</v>
       </c>
       <c r="J18" s="39" t="s">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="K18" s="39" t="s">
-        <v>578</v>
+        <v>494</v>
       </c>
       <c r="L18" s="39" t="s">
-        <v>473</v>
+        <v>438</v>
       </c>
       <c r="M18" s="39" t="s">
-        <v>435</v>
+        <v>342</v>
+      </c>
+      <c r="AC18" s="39" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" s="36" t="s">
-        <v>524</v>
+        <v>455</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>552</v>
-      </c>
-      <c r="E19" s="37" t="s">
-        <v>263</v>
+        <v>473</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>345</v>
+        <v>300</v>
       </c>
       <c r="G19" s="38" t="s">
-        <v>395</v>
-      </c>
-      <c r="H19" s="40" t="s">
-        <v>622</v>
+        <v>323</v>
       </c>
       <c r="I19" s="39" t="s">
-        <v>457</v>
+        <v>413</v>
       </c>
       <c r="J19" s="39" t="s">
-        <v>297</v>
+        <v>264</v>
       </c>
       <c r="K19" s="39" t="s">
-        <v>579</v>
+        <v>495</v>
       </c>
       <c r="L19" s="39" t="s">
-        <v>474</v>
+        <v>439</v>
       </c>
       <c r="M19" s="39" t="s">
-        <v>436</v>
+        <v>343</v>
+      </c>
+      <c r="AC19" s="39" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" s="36" t="s">
-        <v>525</v>
+        <v>456</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>553</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>264</v>
+        <v>474</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>346</v>
+        <v>301</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>396</v>
+        <v>324</v>
       </c>
       <c r="I20" s="39" t="s">
-        <v>458</v>
+        <v>414</v>
       </c>
       <c r="J20" s="39" t="s">
-        <v>298</v>
+        <v>265</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>580</v>
+        <v>496</v>
       </c>
       <c r="L20" s="39" t="s">
-        <v>475</v>
+        <v>440</v>
       </c>
       <c r="M20" s="39" t="s">
-        <v>437</v>
+        <v>344</v>
+      </c>
+      <c r="AC20" s="39" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="21">
       <c r="C21" s="36" t="s">
-        <v>526</v>
+        <v>457</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>554</v>
-      </c>
-      <c r="E21" s="37" t="s">
-        <v>265</v>
+        <v>475</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>347</v>
+        <v>302</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>397</v>
+        <v>325</v>
       </c>
       <c r="I21" s="39" t="s">
-        <v>459</v>
+        <v>415</v>
       </c>
       <c r="J21" s="39" t="s">
-        <v>299</v>
+        <v>266</v>
       </c>
       <c r="K21" s="39" t="s">
-        <v>581</v>
+        <v>497</v>
       </c>
       <c r="L21" s="39" t="s">
-        <v>476</v>
+        <v>441</v>
       </c>
       <c r="M21" s="39" t="s">
-        <v>438</v>
+        <v>345</v>
+      </c>
+      <c r="AC21" s="39" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="22">
       <c r="C22" s="36" t="s">
-        <v>527</v>
+        <v>458</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>555</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>266</v>
+        <v>476</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>348</v>
+        <v>303</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>398</v>
+        <v>326</v>
       </c>
       <c r="I22" s="39" t="s">
-        <v>460</v>
+        <v>416</v>
       </c>
       <c r="J22" s="39" t="s">
-        <v>300</v>
+        <v>267</v>
       </c>
       <c r="K22" s="39" t="s">
-        <v>582</v>
-      </c>
-      <c r="L22" s="39" t="s">
-        <v>477</v>
+        <v>498</v>
+      </c>
+      <c r="M22" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="AC22" s="39" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="23">
       <c r="C23" s="36" t="s">
-        <v>528</v>
+        <v>459</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>556</v>
-      </c>
-      <c r="E23" s="37" t="s">
-        <v>267</v>
+        <v>477</v>
       </c>
       <c r="F23" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>417</v>
+      </c>
+      <c r="J23" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="K23" s="39" t="s">
+        <v>499</v>
+      </c>
+      <c r="M23" s="39" t="s">
+        <v>347</v>
+      </c>
+      <c r="AC23" s="39" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" s="36" t="s">
+        <v>478</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>305</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="I24" s="39" t="s">
+        <v>418</v>
+      </c>
+      <c r="J24" s="39" t="s">
+        <v>269</v>
+      </c>
+      <c r="K24" s="39" t="s">
+        <v>500</v>
+      </c>
+      <c r="M24" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="AC24" s="39" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="D25" s="36" t="s">
+        <v>479</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>306</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>329</v>
+      </c>
+      <c r="I25" s="39" t="s">
+        <v>419</v>
+      </c>
+      <c r="J25" s="39" t="s">
+        <v>270</v>
+      </c>
+      <c r="K25" s="39" t="s">
+        <v>501</v>
+      </c>
+      <c r="M25" s="39" t="s">
         <v>349</v>
       </c>
-      <c r="G23" s="38" t="s">
-        <v>399</v>
-      </c>
-      <c r="J23" s="39" t="s">
-        <v>301</v>
-      </c>
-      <c r="K23" s="39" t="s">
-        <v>583</v>
-      </c>
-      <c r="L23" s="39" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="C24" s="36" t="s">
-        <v>529</v>
-      </c>
-      <c r="D24" s="36" t="s">
-        <v>557</v>
-      </c>
-      <c r="E24" s="37" t="s">
-        <v>268</v>
-      </c>
-      <c r="F24" s="37" t="s">
+      <c r="AC25" s="39" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" s="36" t="s">
+        <v>480</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="I26" s="39" t="s">
+        <v>420</v>
+      </c>
+      <c r="J26" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="K26" s="39" t="s">
+        <v>502</v>
+      </c>
+      <c r="M26" s="39" t="s">
         <v>350</v>
       </c>
-      <c r="G24" s="38" t="s">
-        <v>400</v>
-      </c>
-      <c r="J24" s="39" t="s">
-        <v>302</v>
-      </c>
-      <c r="K24" s="39" t="s">
-        <v>584</v>
-      </c>
-      <c r="L24" s="39" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="C25" s="36" t="s">
-        <v>530</v>
-      </c>
-      <c r="D25" s="36" t="s">
-        <v>558</v>
-      </c>
-      <c r="E25" s="37" t="s">
-        <v>269</v>
-      </c>
-      <c r="F25" s="37" t="s">
+      <c r="AC26" s="39" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="D27" s="36" t="s">
+        <v>481</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>308</v>
+      </c>
+      <c r="I27" s="39" t="s">
+        <v>421</v>
+      </c>
+      <c r="J27" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="K27" s="39" t="s">
+        <v>503</v>
+      </c>
+      <c r="M27" s="39" t="s">
         <v>351</v>
       </c>
-      <c r="G25" s="38" t="s">
-        <v>401</v>
-      </c>
-      <c r="J25" s="39" t="s">
-        <v>303</v>
-      </c>
-      <c r="K25" s="39" t="s">
-        <v>585</v>
-      </c>
-      <c r="L25" s="39" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="C26" s="36" t="s">
-        <v>531</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>559</v>
-      </c>
-      <c r="E26" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="F26" s="37" t="s">
+      <c r="AC27" s="39" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="F28" s="37" t="s">
+        <v>309</v>
+      </c>
+      <c r="I28" s="39" t="s">
+        <v>422</v>
+      </c>
+      <c r="J28" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="K28" s="39" t="s">
+        <v>504</v>
+      </c>
+      <c r="M28" s="39" t="s">
         <v>352</v>
       </c>
-      <c r="G26" s="38" t="s">
-        <v>402</v>
-      </c>
-      <c r="J26" s="39" t="s">
-        <v>304</v>
-      </c>
-      <c r="K26" s="39" t="s">
-        <v>586</v>
-      </c>
-      <c r="L26" s="39" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="C27" s="36" t="s">
-        <v>532</v>
-      </c>
-      <c r="D27" s="36" t="s">
-        <v>560</v>
-      </c>
-      <c r="E27" s="37" t="s">
-        <v>271</v>
-      </c>
-      <c r="F27" s="37" t="s">
+      <c r="AC28" s="39" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="I29" s="39" t="s">
+        <v>423</v>
+      </c>
+      <c r="J29" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="K29" s="39" t="s">
+        <v>505</v>
+      </c>
+      <c r="M29" s="39" t="s">
         <v>353</v>
       </c>
-      <c r="G27" s="38" t="s">
-        <v>403</v>
-      </c>
-      <c r="J27" s="39" t="s">
-        <v>305</v>
-      </c>
-      <c r="K27" s="39" t="s">
-        <v>587</v>
-      </c>
-      <c r="L27" s="39" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="C28" s="36" t="s">
-        <v>533</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>561</v>
-      </c>
-      <c r="E28" s="37" t="s">
-        <v>272</v>
-      </c>
-      <c r="F28" s="37" t="s">
+      <c r="AC29" s="39" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="I30" s="39" t="s">
+        <v>424</v>
+      </c>
+      <c r="J30" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="M30" s="39" t="s">
         <v>354</v>
       </c>
-      <c r="G28" s="38" t="s">
-        <v>404</v>
-      </c>
-      <c r="J28" s="39" t="s">
-        <v>306</v>
-      </c>
-      <c r="K28" s="39" t="s">
-        <v>588</v>
-      </c>
-      <c r="L28" s="39" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" s="36" t="s">
-        <v>534</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>562</v>
-      </c>
-      <c r="E29" s="37" t="s">
-        <v>273</v>
-      </c>
-      <c r="F29" s="37" t="s">
+      <c r="AC30" s="39" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="I31" s="39" t="s">
+        <v>425</v>
+      </c>
+      <c r="J31" s="39" t="s">
+        <v>276</v>
+      </c>
+      <c r="M31" s="39" t="s">
         <v>355</v>
       </c>
-      <c r="G29" s="38" t="s">
-        <v>405</v>
-      </c>
-      <c r="J29" s="39" t="s">
-        <v>307</v>
-      </c>
-      <c r="K29" s="39" t="s">
-        <v>589</v>
-      </c>
-      <c r="L29" s="39" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" s="36" t="s">
-        <v>535</v>
-      </c>
-      <c r="D30" s="36" t="s">
-        <v>563</v>
-      </c>
-      <c r="E30" s="37" t="s">
-        <v>274</v>
-      </c>
-      <c r="F30" s="37" t="s">
+      <c r="AC31" s="39" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="J32" s="39" t="s">
+        <v>277</v>
+      </c>
+      <c r="M32" s="39" t="s">
         <v>356</v>
       </c>
-      <c r="G30" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="J30" s="39" t="s">
-        <v>308</v>
-      </c>
-      <c r="K30" s="39" t="s">
-        <v>590</v>
-      </c>
-      <c r="L30" s="39" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="C31" s="36" t="s">
-        <v>536</v>
-      </c>
-      <c r="D31" s="36" t="s">
-        <v>564</v>
-      </c>
-      <c r="E31" s="37" t="s">
-        <v>275</v>
-      </c>
-      <c r="F31" s="37" t="s">
+      <c r="AC32" s="39" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="J33" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="M33" s="39" t="s">
         <v>357</v>
       </c>
-      <c r="G31" s="38" t="s">
-        <v>407</v>
-      </c>
-      <c r="J31" s="39" t="s">
-        <v>309</v>
-      </c>
-      <c r="K31" s="39" t="s">
-        <v>591</v>
-      </c>
-      <c r="L31" s="39" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="C32" s="36" t="s">
-        <v>537</v>
-      </c>
-      <c r="D32" s="36" t="s">
-        <v>565</v>
-      </c>
-      <c r="E32" s="37" t="s">
-        <v>276</v>
-      </c>
-      <c r="F32" s="37" t="s">
+      <c r="AC33" s="39" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="J34" s="39" t="s">
+        <v>279</v>
+      </c>
+      <c r="M34" s="39" t="s">
         <v>358</v>
       </c>
-      <c r="G32" s="38" t="s">
-        <v>408</v>
-      </c>
-      <c r="J32" s="39" t="s">
-        <v>310</v>
-      </c>
-      <c r="K32" s="39" t="s">
-        <v>592</v>
-      </c>
-      <c r="L32" s="39" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="C33" s="36" t="s">
-        <v>538</v>
-      </c>
-      <c r="E33" s="37" t="s">
-        <v>277</v>
-      </c>
-      <c r="F33" s="37" t="s">
+      <c r="AC34" s="39" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="J35" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="M35" s="39" t="s">
         <v>359</v>
       </c>
-      <c r="G33" s="38" t="s">
-        <v>409</v>
-      </c>
-      <c r="J33" s="39" t="s">
-        <v>311</v>
-      </c>
-      <c r="K33" s="39" t="s">
-        <v>593</v>
-      </c>
-      <c r="L33" s="39" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="E34" s="37" t="s">
-        <v>278</v>
-      </c>
-      <c r="F34" s="37" t="s">
+    </row>
+    <row r="36">
+      <c r="J36" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="M36" s="39" t="s">
         <v>360</v>
       </c>
-      <c r="G34" s="38" t="s">
-        <v>410</v>
-      </c>
-      <c r="J34" s="39" t="s">
-        <v>312</v>
-      </c>
-      <c r="K34" s="39" t="s">
-        <v>594</v>
-      </c>
-      <c r="L34" s="39" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="E35" s="37" t="s">
-        <v>279</v>
-      </c>
-      <c r="F35" s="37" t="s">
+    </row>
+    <row r="37">
+      <c r="J37" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="M37" s="39" t="s">
         <v>361</v>
       </c>
-      <c r="G35" s="38" t="s">
-        <v>411</v>
-      </c>
-      <c r="J35" s="39" t="s">
-        <v>313</v>
-      </c>
-      <c r="K35" s="39" t="s">
-        <v>595</v>
-      </c>
-      <c r="L35" s="39" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="E36" s="37" t="s">
-        <v>280</v>
-      </c>
-      <c r="F36" s="37" t="s">
+    </row>
+    <row r="38">
+      <c r="J38" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="M38" s="39" t="s">
         <v>362</v>
       </c>
-      <c r="G36" s="38" t="s">
-        <v>412</v>
-      </c>
-      <c r="J36" s="39" t="s">
-        <v>314</v>
-      </c>
-      <c r="K36" s="39" t="s">
-        <v>596</v>
-      </c>
-      <c r="L36" s="39" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="E37" s="37" t="s">
-        <v>281</v>
-      </c>
-      <c r="F37" s="37" t="s">
+    </row>
+    <row r="39">
+      <c r="J39" s="39" t="s">
+        <v>284</v>
+      </c>
+      <c r="M39" s="39" t="s">
         <v>363</v>
       </c>
-      <c r="G37" s="38" t="s">
-        <v>413</v>
-      </c>
-      <c r="J37" s="39" t="s">
-        <v>315</v>
-      </c>
-      <c r="K37" s="39" t="s">
-        <v>597</v>
-      </c>
-      <c r="L37" s="39" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="E38" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="F38" s="37" t="s">
+    </row>
+    <row r="40">
+      <c r="J40" s="39" t="s">
+        <v>285</v>
+      </c>
+      <c r="M40" s="39" t="s">
         <v>364</v>
       </c>
-      <c r="G38" s="38" t="s">
-        <v>414</v>
-      </c>
-      <c r="J38" s="39" t="s">
-        <v>316</v>
-      </c>
-      <c r="K38" s="39" t="s">
-        <v>598</v>
-      </c>
-      <c r="L38" s="39" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="F39" s="37" t="s">
+    </row>
+    <row r="41">
+      <c r="M41" s="39" t="s">
         <v>365</v>
-      </c>
-      <c r="G39" s="38" t="s">
-        <v>415</v>
-      </c>
-      <c r="J39" s="39" t="s">
-        <v>317</v>
-      </c>
-      <c r="K39" s="39" t="s">
-        <v>599</v>
-      </c>
-      <c r="L39" s="39" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="F40" s="37" t="s">
-        <v>366</v>
-      </c>
-      <c r="G40" s="38" t="s">
-        <v>416</v>
-      </c>
-      <c r="J40" s="39" t="s">
-        <v>318</v>
-      </c>
-      <c r="K40" s="39" t="s">
-        <v>600</v>
-      </c>
-      <c r="L40" s="39" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="F41" s="37" t="s">
-        <v>367</v>
-      </c>
-      <c r="G41" s="38" t="s">
-        <v>417</v>
-      </c>
-      <c r="J41" s="39" t="s">
-        <v>319</v>
-      </c>
-      <c r="K41" s="39" t="s">
-        <v>601</v>
-      </c>
-      <c r="L41" s="39" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="F42" s="37" t="s">
-        <v>368</v>
-      </c>
-      <c r="G42" s="38" t="s">
-        <v>418</v>
-      </c>
-      <c r="J42" s="39" t="s">
-        <v>320</v>
-      </c>
-      <c r="K42" s="39" t="s">
-        <v>602</v>
-      </c>
-      <c r="L42" s="39" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="F43" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="G43" s="38" t="s">
-        <v>419</v>
-      </c>
-      <c r="J43" s="39" t="s">
-        <v>321</v>
-      </c>
-      <c r="K43" s="39" t="s">
-        <v>603</v>
-      </c>
-      <c r="L43" s="39" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="F44" s="37" t="s">
-        <v>370</v>
-      </c>
-      <c r="G44" s="38" t="s">
-        <v>420</v>
-      </c>
-      <c r="J44" s="39" t="s">
-        <v>322</v>
-      </c>
-      <c r="K44" s="39" t="s">
-        <v>604</v>
-      </c>
-      <c r="L44" s="39" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="F45" s="37" t="s">
-        <v>371</v>
-      </c>
-      <c r="G45" s="38" t="s">
-        <v>421</v>
-      </c>
-      <c r="J45" s="39" t="s">
-        <v>323</v>
-      </c>
-      <c r="K45" s="39" t="s">
-        <v>605</v>
-      </c>
-      <c r="L45" s="39" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="F46" s="37" t="s">
-        <v>372</v>
-      </c>
-      <c r="G46" s="38" t="s">
-        <v>422</v>
-      </c>
-      <c r="J46" s="39" t="s">
-        <v>324</v>
-      </c>
-      <c r="K46" s="39" t="s">
-        <v>606</v>
-      </c>
-      <c r="L46" s="39" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="F47" s="37" t="s">
-        <v>373</v>
-      </c>
-      <c r="J47" s="39" t="s">
-        <v>325</v>
-      </c>
-      <c r="K47" s="39" t="s">
-        <v>607</v>
-      </c>
-      <c r="L47" s="39" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="F48" s="37" t="s">
-        <v>374</v>
-      </c>
-      <c r="J48" s="39" t="s">
-        <v>326</v>
-      </c>
-      <c r="K48" s="39" t="s">
-        <v>608</v>
-      </c>
-      <c r="L48" s="39" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="F49" s="37" t="s">
-        <v>375</v>
-      </c>
-      <c r="J49" s="39" t="s">
-        <v>327</v>
-      </c>
-      <c r="L49" s="39" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="F50" s="37" t="s">
-        <v>376</v>
-      </c>
-      <c r="J50" s="39" t="s">
-        <v>328</v>
-      </c>
-      <c r="L50" s="39" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="F51" s="37" t="s">
-        <v>377</v>
-      </c>
-      <c r="J51" s="39" t="s">
-        <v>329</v>
-      </c>
-      <c r="L51" s="39" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="F52" s="37" t="s">
-        <v>378</v>
-      </c>
-      <c r="J52" s="39" t="s">
-        <v>330</v>
-      </c>
-      <c r="L52" s="39" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="F53" s="37" t="s">
-        <v>379</v>
-      </c>
-      <c r="L53" s="39" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="F54" s="37" t="s">
-        <v>380</v>
-      </c>
-      <c r="L54" s="39" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="L55" s="39" t="s">
-        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cellstyle resolve / class name refactor
</commit_message>
<xml_diff>
--- a/X-Domestic Standard Upload.xlsx
+++ b/X-Domestic Standard Upload.xlsx
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="599">
   <si>
     <t>#</t>
   </si>
@@ -1144,6 +1144,141 @@
     <t>col:0</t>
   </si>
   <si>
+    <t>col:1</t>
+  </si>
+  <si>
+    <t>col:2</t>
+  </si>
+  <si>
+    <t>col:3</t>
+  </si>
+  <si>
+    <t>col:4</t>
+  </si>
+  <si>
+    <t>col:5</t>
+  </si>
+  <si>
+    <t>col:6</t>
+  </si>
+  <si>
+    <t>col:7</t>
+  </si>
+  <si>
+    <t>col:8</t>
+  </si>
+  <si>
+    <t>col:9</t>
+  </si>
+  <si>
+    <t>col:10</t>
+  </si>
+  <si>
+    <t>col:11</t>
+  </si>
+  <si>
+    <t>col:12</t>
+  </si>
+  <si>
+    <t>col:13</t>
+  </si>
+  <si>
+    <t>col:14</t>
+  </si>
+  <si>
+    <t>col:15</t>
+  </si>
+  <si>
+    <t>col:16</t>
+  </si>
+  <si>
+    <t>col:17</t>
+  </si>
+  <si>
+    <t>col:18</t>
+  </si>
+  <si>
+    <t>col:19</t>
+  </si>
+  <si>
+    <t>col:20</t>
+  </si>
+  <si>
+    <t>col:21</t>
+  </si>
+  <si>
+    <t>col:22</t>
+  </si>
+  <si>
+    <t>col:23</t>
+  </si>
+  <si>
+    <t>col:24</t>
+  </si>
+  <si>
+    <t>col:25</t>
+  </si>
+  <si>
+    <t>col:26</t>
+  </si>
+  <si>
+    <t>col:27</t>
+  </si>
+  <si>
+    <t>col:28</t>
+  </si>
+  <si>
+    <t>col:29</t>
+  </si>
+  <si>
+    <t>col:30</t>
+  </si>
+  <si>
+    <t>col:31</t>
+  </si>
+  <si>
+    <t>col:32</t>
+  </si>
+  <si>
+    <t>col:33</t>
+  </si>
+  <si>
+    <t>col:34</t>
+  </si>
+  <si>
+    <t>col:35</t>
+  </si>
+  <si>
+    <t>col:36</t>
+  </si>
+  <si>
+    <t>col:37</t>
+  </si>
+  <si>
+    <t>col:38</t>
+  </si>
+  <si>
+    <t>col:39</t>
+  </si>
+  <si>
+    <t>col:40</t>
+  </si>
+  <si>
+    <t>col:41</t>
+  </si>
+  <si>
+    <t>col:42</t>
+  </si>
+  <si>
+    <t>col:43</t>
+  </si>
+  <si>
+    <t>col:44</t>
+  </si>
+  <si>
+    <t>col:45</t>
+  </si>
+  <si>
     <t>dep:0</t>
   </si>
   <si>
@@ -1186,72 +1321,6 @@
     <t>dep:13</t>
   </si>
   <si>
-    <t>dep:14</t>
-  </si>
-  <si>
-    <t>dep:15</t>
-  </si>
-  <si>
-    <t>dep:16</t>
-  </si>
-  <si>
-    <t>dep:17</t>
-  </si>
-  <si>
-    <t>dep:18</t>
-  </si>
-  <si>
-    <t>dep:19</t>
-  </si>
-  <si>
-    <t>dep:20</t>
-  </si>
-  <si>
-    <t>dep:21</t>
-  </si>
-  <si>
-    <t>dep:22</t>
-  </si>
-  <si>
-    <t>dep:23</t>
-  </si>
-  <si>
-    <t>dep:24</t>
-  </si>
-  <si>
-    <t>dep:25</t>
-  </si>
-  <si>
-    <t>dep:26</t>
-  </si>
-  <si>
-    <t>dep:27</t>
-  </si>
-  <si>
-    <t>dep:28</t>
-  </si>
-  <si>
-    <t>dep:29</t>
-  </si>
-  <si>
-    <t>dep:30</t>
-  </si>
-  <si>
-    <t>dep:31</t>
-  </si>
-  <si>
-    <t>dep:32</t>
-  </si>
-  <si>
-    <t>dep:33</t>
-  </si>
-  <si>
-    <t>dep:34</t>
-  </si>
-  <si>
-    <t>dep:35</t>
-  </si>
-  <si>
     <t>siz:0</t>
   </si>
   <si>
@@ -1309,18 +1378,6 @@
     <t>siz:18</t>
   </si>
   <si>
-    <t>siz:19</t>
-  </si>
-  <si>
-    <t>siz:20</t>
-  </si>
-  <si>
-    <t>siz:21</t>
-  </si>
-  <si>
-    <t>siz:22</t>
-  </si>
-  <si>
     <t>typ:0</t>
   </si>
   <si>
@@ -1381,6 +1438,30 @@
     <t>typ:19</t>
   </si>
   <si>
+    <t>typ:20</t>
+  </si>
+  <si>
+    <t>typ:21</t>
+  </si>
+  <si>
+    <t>typ:22</t>
+  </si>
+  <si>
+    <t>typ:23</t>
+  </si>
+  <si>
+    <t>typ:24</t>
+  </si>
+  <si>
+    <t>typ:25</t>
+  </si>
+  <si>
+    <t>typ:26</t>
+  </si>
+  <si>
+    <t>typ:27</t>
+  </si>
+  <si>
     <t>mat:0</t>
   </si>
   <si>
@@ -1489,6 +1570,30 @@
     <t>mat:35</t>
   </si>
   <si>
+    <t>mat:36</t>
+  </si>
+  <si>
+    <t>mat:37</t>
+  </si>
+  <si>
+    <t>mat:38</t>
+  </si>
+  <si>
+    <t>mat:39</t>
+  </si>
+  <si>
+    <t>mat:40</t>
+  </si>
+  <si>
+    <t>mat:41</t>
+  </si>
+  <si>
+    <t>mat:42</t>
+  </si>
+  <si>
+    <t>mat:43</t>
+  </si>
+  <si>
     <t>wei:0</t>
   </si>
   <si>
@@ -1579,6 +1684,42 @@
     <t>wei:29</t>
   </si>
   <si>
+    <t>wei:30</t>
+  </si>
+  <si>
+    <t>wei:31</t>
+  </si>
+  <si>
+    <t>wei:32</t>
+  </si>
+  <si>
+    <t>wei:33</t>
+  </si>
+  <si>
+    <t>wei:34</t>
+  </si>
+  <si>
+    <t>wei:35</t>
+  </si>
+  <si>
+    <t>wei:36</t>
+  </si>
+  <si>
+    <t>wei:37</t>
+  </si>
+  <si>
+    <t>wei:38</t>
+  </si>
+  <si>
+    <t>wei:39</t>
+  </si>
+  <si>
+    <t>wei:40</t>
+  </si>
+  <si>
+    <t>wei:41</t>
+  </si>
+  <si>
     <t>vpn:0</t>
   </si>
   <si>
@@ -1591,84 +1732,15 @@
     <t>vpn:3</t>
   </si>
   <si>
+    <t>vpn:4</t>
+  </si>
+  <si>
     <t>sup:0</t>
   </si>
   <si>
     <t>sup:1</t>
   </si>
   <si>
-    <t>sup:2</t>
-  </si>
-  <si>
-    <t>sup:3</t>
-  </si>
-  <si>
-    <t>sup:4</t>
-  </si>
-  <si>
-    <t>sup:5</t>
-  </si>
-  <si>
-    <t>sup:6</t>
-  </si>
-  <si>
-    <t>sup:7</t>
-  </si>
-  <si>
-    <t>sup:8</t>
-  </si>
-  <si>
-    <t>sup:9</t>
-  </si>
-  <si>
-    <t>sup:10</t>
-  </si>
-  <si>
-    <t>sup:11</t>
-  </si>
-  <si>
-    <t>sup:12</t>
-  </si>
-  <si>
-    <t>sup:13</t>
-  </si>
-  <si>
-    <t>sup:14</t>
-  </si>
-  <si>
-    <t>sup:15</t>
-  </si>
-  <si>
-    <t>sup:16</t>
-  </si>
-  <si>
-    <t>sup:17</t>
-  </si>
-  <si>
-    <t>sup:18</t>
-  </si>
-  <si>
-    <t>sup:19</t>
-  </si>
-  <si>
-    <t>sup:20</t>
-  </si>
-  <si>
-    <t>sup:21</t>
-  </si>
-  <si>
-    <t>sup:22</t>
-  </si>
-  <si>
-    <t>sup:23</t>
-  </si>
-  <si>
-    <t>sup:24</t>
-  </si>
-  <si>
-    <t>sup:25</t>
-  </si>
-  <si>
     <t>cat:0</t>
   </si>
   <si>
@@ -1717,6 +1789,36 @@
     <t>cat:15</t>
   </si>
   <si>
+    <t>cat:16</t>
+  </si>
+  <si>
+    <t>cat:17</t>
+  </si>
+  <si>
+    <t>cat:18</t>
+  </si>
+  <si>
+    <t>cat:19</t>
+  </si>
+  <si>
+    <t>cat:20</t>
+  </si>
+  <si>
+    <t>cat:21</t>
+  </si>
+  <si>
+    <t>cat:22</t>
+  </si>
+  <si>
+    <t>cat:23</t>
+  </si>
+  <si>
+    <t>cat:24</t>
+  </si>
+  <si>
+    <t>cat:25</t>
+  </si>
+  <si>
     <t>ven:0</t>
   </si>
   <si>
@@ -1771,6 +1873,51 @@
     <t>ven:17</t>
   </si>
   <si>
+    <t>ven:18</t>
+  </si>
+  <si>
+    <t>ven:19</t>
+  </si>
+  <si>
+    <t>ven:20</t>
+  </si>
+  <si>
+    <t>ven:21</t>
+  </si>
+  <si>
+    <t>ven:22</t>
+  </si>
+  <si>
+    <t>ven:23</t>
+  </si>
+  <si>
+    <t>ven:24</t>
+  </si>
+  <si>
+    <t>ven:25</t>
+  </si>
+  <si>
+    <t>ven:26</t>
+  </si>
+  <si>
+    <t>ven:27</t>
+  </si>
+  <si>
+    <t>ven:28</t>
+  </si>
+  <si>
+    <t>ven:29</t>
+  </si>
+  <si>
+    <t>ven:30</t>
+  </si>
+  <si>
+    <t>ven:31</t>
+  </si>
+  <si>
+    <t>ven:32</t>
+  </si>
+  <si>
     <t>lab:0</t>
   </si>
   <si>
@@ -1837,6 +1984,81 @@
     <t>lab:21</t>
   </si>
   <si>
+    <t>lab:22</t>
+  </si>
+  <si>
+    <t>lab:23</t>
+  </si>
+  <si>
+    <t>lab:24</t>
+  </si>
+  <si>
+    <t>lab:25</t>
+  </si>
+  <si>
+    <t>lab:26</t>
+  </si>
+  <si>
+    <t>lab:27</t>
+  </si>
+  <si>
+    <t>lab:28</t>
+  </si>
+  <si>
+    <t>lab:29</t>
+  </si>
+  <si>
+    <t>lab:30</t>
+  </si>
+  <si>
+    <t>lab:31</t>
+  </si>
+  <si>
+    <t>lab:32</t>
+  </si>
+  <si>
+    <t>lab:33</t>
+  </si>
+  <si>
+    <t>lab:34</t>
+  </si>
+  <si>
+    <t>lab:35</t>
+  </si>
+  <si>
+    <t>lab:36</t>
+  </si>
+  <si>
+    <t>lab:37</t>
+  </si>
+  <si>
+    <t>lab:38</t>
+  </si>
+  <si>
+    <t>lab:39</t>
+  </si>
+  <si>
+    <t>lab:40</t>
+  </si>
+  <si>
+    <t>lab:41</t>
+  </si>
+  <si>
+    <t>lab:42</t>
+  </si>
+  <si>
+    <t>lab:43</t>
+  </si>
+  <si>
+    <t>lab:44</t>
+  </si>
+  <si>
+    <t>lab:45</t>
+  </si>
+  <si>
+    <t>lab:46</t>
+  </si>
+  <si>
     <t>cla:0</t>
   </si>
   <si>
@@ -1909,6 +2131,42 @@
     <t>cla:23</t>
   </si>
   <si>
+    <t>cla:24</t>
+  </si>
+  <si>
+    <t>cla:25</t>
+  </si>
+  <si>
+    <t>cla:26</t>
+  </si>
+  <si>
+    <t>cla:27</t>
+  </si>
+  <si>
+    <t>cla:28</t>
+  </si>
+  <si>
+    <t>cla:29</t>
+  </si>
+  <si>
+    <t>cla:30</t>
+  </si>
+  <si>
+    <t>cla:31</t>
+  </si>
+  <si>
+    <t>cla:32</t>
+  </si>
+  <si>
+    <t>cla:33</t>
+  </si>
+  <si>
+    <t>cla:34</t>
+  </si>
+  <si>
+    <t>cla:35</t>
+  </si>
+  <si>
     <t>pon:0</t>
   </si>
   <si>
@@ -1928,9 +2186,6 @@
   </si>
   <si>
     <t>pon:6</t>
-  </si>
-  <si>
-    <t>pon:7</t>
   </si>
 </sst>
 </file>
@@ -6387,7 +6642,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A17F3EB-F212-417F-BA00-A3FB97B2BF77}">
-  <dimension ref="A1:CV41"/>
+  <dimension ref="A1:CV52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
@@ -7693,7 +7948,7 @@
       <c r="AA5" s="50"/>
       <c r="AB5" s="50"/>
       <c r="AC5" s="39" t="s">
-        <v>366</v>
+        <v>401</v>
       </c>
       <c r="AD5" s="50"/>
       <c r="AE5" s="50"/>
@@ -7769,857 +8024,1137 @@
     </row>
     <row r="6">
       <c r="B6" s="36" t="s">
-        <v>396</v>
+        <v>443</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>442</v>
+        <v>476</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>460</v>
+        <v>509</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>250</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>310</v>
+        <v>329</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>506</v>
+        <v>592</v>
       </c>
       <c r="I6" s="39" t="s">
-        <v>400</v>
+        <v>448</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>251</v>
+        <v>296</v>
       </c>
       <c r="K6" s="39" t="s">
-        <v>482</v>
+        <v>556</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>426</v>
+        <v>450</v>
       </c>
       <c r="M6" s="39" t="s">
-        <v>330</v>
+        <v>357</v>
       </c>
       <c r="AC6" s="39" t="s">
-        <v>367</v>
+        <v>402</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="36" t="s">
-        <v>397</v>
+        <v>444</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>443</v>
+        <v>477</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>461</v>
+        <v>510</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>251</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>288</v>
+        <v>311</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>507</v>
+        <v>593</v>
       </c>
       <c r="I7" s="39" t="s">
-        <v>401</v>
+        <v>449</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>252</v>
+        <v>297</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>483</v>
+        <v>557</v>
       </c>
       <c r="L7" s="39" t="s">
-        <v>427</v>
+        <v>451</v>
       </c>
       <c r="M7" s="39" t="s">
-        <v>331</v>
+        <v>358</v>
       </c>
       <c r="AC7" s="39" t="s">
-        <v>368</v>
+        <v>403</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="36" t="s">
-        <v>398</v>
+        <v>445</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>444</v>
+        <v>478</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>462</v>
+        <v>511</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>252</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>289</v>
+        <v>312</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>508</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>402</v>
+        <v>594</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>253</v>
+        <v>298</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>484</v>
+        <v>558</v>
       </c>
       <c r="L8" s="39" t="s">
-        <v>428</v>
+        <v>452</v>
       </c>
       <c r="M8" s="39" t="s">
-        <v>332</v>
+        <v>359</v>
       </c>
       <c r="AC8" s="39" t="s">
-        <v>369</v>
+        <v>404</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="36" t="s">
-        <v>399</v>
+        <v>446</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>445</v>
+        <v>479</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>463</v>
+        <v>512</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>253</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>509</v>
-      </c>
-      <c r="I9" s="39" t="s">
-        <v>403</v>
+        <v>595</v>
       </c>
       <c r="J9" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="K9" s="39" t="s">
+        <v>559</v>
+      </c>
+      <c r="L9" s="39" t="s">
+        <v>453</v>
+      </c>
+      <c r="M9" s="39" t="s">
+        <v>360</v>
+      </c>
+      <c r="AC9" s="39" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="36" t="s">
+        <v>447</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>480</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>513</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="K9" s="39" t="s">
-        <v>485</v>
-      </c>
-      <c r="L9" s="39" t="s">
-        <v>429</v>
-      </c>
-      <c r="M9" s="39" t="s">
+      <c r="F10" s="37" t="s">
+        <v>314</v>
+      </c>
+      <c r="G10" s="38" t="s">
         <v>333</v>
       </c>
-      <c r="AC9" s="39" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>464</v>
-      </c>
-      <c r="F10" s="37" t="s">
-        <v>291</v>
-      </c>
-      <c r="G10" s="38" t="s">
-        <v>314</v>
-      </c>
       <c r="H10" s="40" t="s">
-        <v>510</v>
-      </c>
-      <c r="I10" s="39" t="s">
-        <v>404</v>
+        <v>596</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>486</v>
+        <v>560</v>
       </c>
       <c r="L10" s="39" t="s">
-        <v>430</v>
+        <v>454</v>
       </c>
       <c r="M10" s="39" t="s">
-        <v>334</v>
+        <v>361</v>
       </c>
       <c r="AC10" s="39" t="s">
-        <v>371</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11">
       <c r="C11" s="36" t="s">
-        <v>447</v>
+        <v>481</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>465</v>
+        <v>514</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>255</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>292</v>
+        <v>315</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>511</v>
-      </c>
-      <c r="I11" s="39" t="s">
-        <v>405</v>
+        <v>597</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>256</v>
+        <v>301</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>487</v>
+        <v>561</v>
       </c>
       <c r="L11" s="39" t="s">
-        <v>431</v>
+        <v>455</v>
       </c>
       <c r="M11" s="39" t="s">
-        <v>335</v>
+        <v>362</v>
       </c>
       <c r="AC11" s="39" t="s">
-        <v>372</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12">
       <c r="C12" s="36" t="s">
-        <v>448</v>
+        <v>482</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>466</v>
+        <v>515</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>256</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>512</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>406</v>
+        <v>598</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>257</v>
+        <v>302</v>
       </c>
       <c r="K12" s="39" t="s">
-        <v>488</v>
+        <v>562</v>
       </c>
       <c r="L12" s="39" t="s">
-        <v>432</v>
+        <v>456</v>
       </c>
       <c r="M12" s="39" t="s">
-        <v>336</v>
+        <v>363</v>
       </c>
       <c r="AC12" s="39" t="s">
-        <v>373</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="36" t="s">
-        <v>449</v>
+        <v>483</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>467</v>
+        <v>516</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>257</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>294</v>
+        <v>317</v>
       </c>
       <c r="G13" s="38" t="s">
-        <v>317</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>513</v>
-      </c>
-      <c r="I13" s="39" t="s">
-        <v>407</v>
+        <v>336</v>
       </c>
       <c r="J13" s="39" t="s">
-        <v>258</v>
+        <v>303</v>
       </c>
       <c r="K13" s="39" t="s">
-        <v>489</v>
+        <v>563</v>
       </c>
       <c r="L13" s="39" t="s">
-        <v>433</v>
+        <v>457</v>
       </c>
       <c r="M13" s="39" t="s">
-        <v>337</v>
+        <v>364</v>
       </c>
       <c r="AC13" s="39" t="s">
-        <v>374</v>
+        <v>409</v>
       </c>
     </row>
     <row r="14">
       <c r="C14" s="36" t="s">
-        <v>450</v>
+        <v>484</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>468</v>
+        <v>517</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>258</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>318</v>
-      </c>
-      <c r="I14" s="39" t="s">
-        <v>408</v>
+        <v>337</v>
       </c>
       <c r="J14" s="39" t="s">
-        <v>259</v>
+        <v>304</v>
       </c>
       <c r="K14" s="39" t="s">
-        <v>490</v>
+        <v>564</v>
       </c>
       <c r="L14" s="39" t="s">
-        <v>434</v>
+        <v>458</v>
       </c>
       <c r="M14" s="39" t="s">
-        <v>338</v>
+        <v>365</v>
       </c>
       <c r="AC14" s="39" t="s">
-        <v>375</v>
+        <v>410</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="36" t="s">
-        <v>451</v>
+        <v>485</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>469</v>
+        <v>518</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>259</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>319</v>
-      </c>
-      <c r="I15" s="39" t="s">
-        <v>409</v>
+        <v>338</v>
       </c>
       <c r="J15" s="39" t="s">
-        <v>260</v>
+        <v>305</v>
       </c>
       <c r="K15" s="39" t="s">
-        <v>491</v>
+        <v>565</v>
       </c>
       <c r="L15" s="39" t="s">
-        <v>435</v>
+        <v>459</v>
       </c>
       <c r="M15" s="39" t="s">
-        <v>339</v>
+        <v>366</v>
       </c>
       <c r="AC15" s="39" t="s">
-        <v>376</v>
+        <v>411</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="36" t="s">
-        <v>452</v>
+        <v>486</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>470</v>
+        <v>519</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>260</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>297</v>
+        <v>320</v>
       </c>
       <c r="G16" s="38" t="s">
-        <v>320</v>
-      </c>
-      <c r="I16" s="39" t="s">
-        <v>410</v>
+        <v>339</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>261</v>
+        <v>306</v>
       </c>
       <c r="K16" s="39" t="s">
-        <v>492</v>
+        <v>566</v>
       </c>
       <c r="L16" s="39" t="s">
-        <v>436</v>
+        <v>460</v>
       </c>
       <c r="M16" s="39" t="s">
-        <v>340</v>
+        <v>367</v>
       </c>
       <c r="AC16" s="39" t="s">
-        <v>377</v>
+        <v>412</v>
       </c>
     </row>
     <row r="17">
       <c r="C17" s="36" t="s">
-        <v>453</v>
+        <v>487</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>471</v>
+        <v>520</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>261</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>298</v>
+        <v>321</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>321</v>
-      </c>
-      <c r="I17" s="39" t="s">
-        <v>411</v>
+        <v>340</v>
       </c>
       <c r="J17" s="39" t="s">
-        <v>262</v>
+        <v>307</v>
       </c>
       <c r="K17" s="39" t="s">
-        <v>493</v>
+        <v>567</v>
       </c>
       <c r="L17" s="39" t="s">
-        <v>437</v>
+        <v>461</v>
       </c>
       <c r="M17" s="39" t="s">
-        <v>341</v>
+        <v>368</v>
       </c>
       <c r="AC17" s="39" t="s">
-        <v>378</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" s="36" t="s">
-        <v>454</v>
+        <v>488</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>472</v>
+        <v>521</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>262</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="I18" s="39" t="s">
-        <v>412</v>
+        <v>341</v>
       </c>
       <c r="J18" s="39" t="s">
-        <v>263</v>
+        <v>308</v>
       </c>
       <c r="K18" s="39" t="s">
-        <v>494</v>
+        <v>568</v>
       </c>
       <c r="L18" s="39" t="s">
-        <v>438</v>
+        <v>462</v>
       </c>
       <c r="M18" s="39" t="s">
-        <v>342</v>
+        <v>369</v>
       </c>
       <c r="AC18" s="39" t="s">
-        <v>379</v>
+        <v>414</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" s="36" t="s">
-        <v>455</v>
+        <v>489</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>473</v>
+        <v>522</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>263</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="G19" s="38" t="s">
-        <v>323</v>
-      </c>
-      <c r="I19" s="39" t="s">
-        <v>413</v>
+        <v>342</v>
       </c>
       <c r="J19" s="39" t="s">
-        <v>264</v>
+        <v>309</v>
       </c>
       <c r="K19" s="39" t="s">
-        <v>495</v>
+        <v>569</v>
       </c>
       <c r="L19" s="39" t="s">
-        <v>439</v>
+        <v>463</v>
       </c>
       <c r="M19" s="39" t="s">
-        <v>343</v>
+        <v>370</v>
       </c>
       <c r="AC19" s="39" t="s">
-        <v>380</v>
+        <v>415</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" s="36" t="s">
-        <v>456</v>
+        <v>490</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>474</v>
+        <v>523</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>264</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>324</v>
-      </c>
-      <c r="I20" s="39" t="s">
-        <v>414</v>
-      </c>
-      <c r="J20" s="39" t="s">
-        <v>265</v>
+        <v>343</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>496</v>
+        <v>570</v>
       </c>
       <c r="L20" s="39" t="s">
-        <v>440</v>
+        <v>464</v>
       </c>
       <c r="M20" s="39" t="s">
-        <v>344</v>
+        <v>371</v>
       </c>
       <c r="AC20" s="39" t="s">
-        <v>381</v>
+        <v>416</v>
       </c>
     </row>
     <row r="21">
       <c r="C21" s="36" t="s">
-        <v>457</v>
+        <v>491</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>475</v>
+        <v>524</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>265</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>325</v>
-      </c>
-      <c r="I21" s="39" t="s">
-        <v>415</v>
-      </c>
-      <c r="J21" s="39" t="s">
-        <v>266</v>
+        <v>344</v>
       </c>
       <c r="K21" s="39" t="s">
-        <v>497</v>
+        <v>571</v>
       </c>
       <c r="L21" s="39" t="s">
-        <v>441</v>
+        <v>465</v>
       </c>
       <c r="M21" s="39" t="s">
-        <v>345</v>
+        <v>372</v>
       </c>
       <c r="AC21" s="39" t="s">
-        <v>382</v>
+        <v>417</v>
       </c>
     </row>
     <row r="22">
       <c r="C22" s="36" t="s">
-        <v>458</v>
+        <v>492</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>476</v>
+        <v>525</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>266</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>326</v>
-      </c>
-      <c r="I22" s="39" t="s">
-        <v>416</v>
-      </c>
-      <c r="J22" s="39" t="s">
-        <v>267</v>
+        <v>345</v>
       </c>
       <c r="K22" s="39" t="s">
-        <v>498</v>
+        <v>572</v>
+      </c>
+      <c r="L22" s="39" t="s">
+        <v>466</v>
       </c>
       <c r="M22" s="39" t="s">
-        <v>346</v>
+        <v>373</v>
       </c>
       <c r="AC22" s="39" t="s">
-        <v>383</v>
+        <v>418</v>
       </c>
     </row>
     <row r="23">
       <c r="C23" s="36" t="s">
-        <v>459</v>
+        <v>493</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>477</v>
+        <v>526</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>267</v>
       </c>
       <c r="F23" s="37" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>327</v>
-      </c>
-      <c r="I23" s="39" t="s">
-        <v>417</v>
-      </c>
-      <c r="J23" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="K23" s="39" t="s">
+        <v>573</v>
+      </c>
+      <c r="L23" s="39" t="s">
+        <v>467</v>
+      </c>
+      <c r="M23" s="39" t="s">
+        <v>374</v>
+      </c>
+      <c r="AC23" s="39" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="36" t="s">
+        <v>494</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>527</v>
+      </c>
+      <c r="E24" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="K23" s="39" t="s">
+      <c r="F24" s="37" t="s">
+        <v>328</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="K24" s="39" t="s">
+        <v>574</v>
+      </c>
+      <c r="L24" s="39" t="s">
+        <v>468</v>
+      </c>
+      <c r="M24" s="39" t="s">
+        <v>375</v>
+      </c>
+      <c r="AC24" s="39" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="36" t="s">
+        <v>495</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>528</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="K25" s="39" t="s">
+        <v>575</v>
+      </c>
+      <c r="L25" s="39" t="s">
+        <v>469</v>
+      </c>
+      <c r="M25" s="39" t="s">
+        <v>376</v>
+      </c>
+      <c r="AC25" s="39" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" s="36" t="s">
+        <v>496</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>529</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="K26" s="39" t="s">
+        <v>576</v>
+      </c>
+      <c r="L26" s="39" t="s">
+        <v>470</v>
+      </c>
+      <c r="M26" s="39" t="s">
+        <v>377</v>
+      </c>
+      <c r="AC26" s="39" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" s="36" t="s">
+        <v>497</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>530</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="K27" s="39" t="s">
+        <v>577</v>
+      </c>
+      <c r="L27" s="39" t="s">
+        <v>471</v>
+      </c>
+      <c r="M27" s="39" t="s">
+        <v>378</v>
+      </c>
+      <c r="AC27" s="39" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" s="36" t="s">
+        <v>498</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>531</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="G28" s="38" t="s">
+        <v>351</v>
+      </c>
+      <c r="K28" s="39" t="s">
+        <v>578</v>
+      </c>
+      <c r="L28" s="39" t="s">
+        <v>472</v>
+      </c>
+      <c r="M28" s="39" t="s">
+        <v>379</v>
+      </c>
+      <c r="AC28" s="39" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="36" t="s">
         <v>499</v>
       </c>
-      <c r="M23" s="39" t="s">
-        <v>347</v>
-      </c>
-      <c r="AC23" s="39" t="s">
+      <c r="D29" s="36" t="s">
+        <v>532</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>352</v>
+      </c>
+      <c r="K29" s="39" t="s">
+        <v>579</v>
+      </c>
+      <c r="L29" s="39" t="s">
+        <v>473</v>
+      </c>
+      <c r="M29" s="39" t="s">
+        <v>380</v>
+      </c>
+      <c r="AC29" s="39" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" s="36" t="s">
+        <v>500</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>533</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="G30" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="K30" s="39" t="s">
+        <v>580</v>
+      </c>
+      <c r="L30" s="39" t="s">
+        <v>474</v>
+      </c>
+      <c r="M30" s="39" t="s">
+        <v>381</v>
+      </c>
+      <c r="AC30" s="39" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="36" t="s">
+        <v>501</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>534</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="G31" s="38" t="s">
+        <v>354</v>
+      </c>
+      <c r="K31" s="39" t="s">
+        <v>581</v>
+      </c>
+      <c r="L31" s="39" t="s">
+        <v>475</v>
+      </c>
+      <c r="M31" s="39" t="s">
+        <v>382</v>
+      </c>
+      <c r="AC31" s="39" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" s="36" t="s">
+        <v>502</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>535</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>276</v>
+      </c>
+      <c r="G32" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="K32" s="39" t="s">
+        <v>582</v>
+      </c>
+      <c r="M32" s="39" t="s">
+        <v>383</v>
+      </c>
+      <c r="AC32" s="39" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" s="36" t="s">
+        <v>503</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>536</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>356</v>
+      </c>
+      <c r="K33" s="39" t="s">
+        <v>583</v>
+      </c>
+      <c r="M33" s="39" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="D24" s="36" t="s">
-        <v>478</v>
-      </c>
-      <c r="F24" s="37" t="s">
-        <v>305</v>
-      </c>
-      <c r="G24" s="38" t="s">
-        <v>328</v>
-      </c>
-      <c r="I24" s="39" t="s">
-        <v>418</v>
-      </c>
-      <c r="J24" s="39" t="s">
-        <v>269</v>
-      </c>
-      <c r="K24" s="39" t="s">
-        <v>500</v>
-      </c>
-      <c r="M24" s="39" t="s">
-        <v>348</v>
-      </c>
-      <c r="AC24" s="39" t="s">
+      <c r="AC33" s="39" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" s="36" t="s">
+        <v>504</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>537</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>278</v>
+      </c>
+      <c r="K34" s="39" t="s">
+        <v>584</v>
+      </c>
+      <c r="M34" s="39" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="D25" s="36" t="s">
-        <v>479</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>306</v>
-      </c>
-      <c r="G25" s="38" t="s">
-        <v>329</v>
-      </c>
-      <c r="I25" s="39" t="s">
-        <v>419</v>
-      </c>
-      <c r="J25" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="K25" s="39" t="s">
-        <v>501</v>
-      </c>
-      <c r="M25" s="39" t="s">
-        <v>349</v>
-      </c>
-      <c r="AC25" s="39" t="s">
+      <c r="AC34" s="39" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" s="36" t="s">
+        <v>505</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>538</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="K35" s="39" t="s">
+        <v>585</v>
+      </c>
+      <c r="M35" s="39" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="D26" s="36" t="s">
-        <v>480</v>
-      </c>
-      <c r="F26" s="37" t="s">
-        <v>307</v>
-      </c>
-      <c r="I26" s="39" t="s">
-        <v>420</v>
-      </c>
-      <c r="J26" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="K26" s="39" t="s">
-        <v>502</v>
-      </c>
-      <c r="M26" s="39" t="s">
-        <v>350</v>
-      </c>
-      <c r="AC26" s="39" t="s">
+      <c r="AC35" s="39" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="C36" s="36" t="s">
+        <v>506</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>539</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="K36" s="39" t="s">
+        <v>586</v>
+      </c>
+      <c r="M36" s="39" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="D27" s="36" t="s">
-        <v>481</v>
-      </c>
-      <c r="F27" s="37" t="s">
-        <v>308</v>
-      </c>
-      <c r="I27" s="39" t="s">
-        <v>421</v>
-      </c>
-      <c r="J27" s="39" t="s">
-        <v>272</v>
-      </c>
-      <c r="K27" s="39" t="s">
-        <v>503</v>
-      </c>
-      <c r="M27" s="39" t="s">
-        <v>351</v>
-      </c>
-      <c r="AC27" s="39" t="s">
+      <c r="AC36" s="39" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" s="36" t="s">
+        <v>507</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>540</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="K37" s="39" t="s">
+        <v>587</v>
+      </c>
+      <c r="M37" s="39" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="F28" s="37" t="s">
-        <v>309</v>
-      </c>
-      <c r="I28" s="39" t="s">
-        <v>422</v>
-      </c>
-      <c r="J28" s="39" t="s">
-        <v>273</v>
-      </c>
-      <c r="K28" s="39" t="s">
-        <v>504</v>
-      </c>
-      <c r="M28" s="39" t="s">
-        <v>352</v>
-      </c>
-      <c r="AC28" s="39" t="s">
+      <c r="AC37" s="39" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="C38" s="36" t="s">
+        <v>508</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>541</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="K38" s="39" t="s">
+        <v>588</v>
+      </c>
+      <c r="M38" s="39" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="I29" s="39" t="s">
-        <v>423</v>
-      </c>
-      <c r="J29" s="39" t="s">
-        <v>274</v>
-      </c>
-      <c r="K29" s="39" t="s">
-        <v>505</v>
-      </c>
-      <c r="M29" s="39" t="s">
-        <v>353</v>
-      </c>
-      <c r="AC29" s="39" t="s">
+      <c r="AC38" s="39" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" s="36" t="s">
+        <v>542</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="K39" s="39" t="s">
+        <v>589</v>
+      </c>
+      <c r="M39" s="39" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="I30" s="39" t="s">
-        <v>424</v>
-      </c>
-      <c r="J30" s="39" t="s">
-        <v>275</v>
-      </c>
-      <c r="M30" s="39" t="s">
-        <v>354</v>
-      </c>
-      <c r="AC30" s="39" t="s">
+      <c r="AC39" s="39" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" s="36" t="s">
+        <v>543</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="K40" s="39" t="s">
+        <v>590</v>
+      </c>
+      <c r="M40" s="39" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="I31" s="39" t="s">
-        <v>425</v>
-      </c>
-      <c r="J31" s="39" t="s">
-        <v>276</v>
-      </c>
-      <c r="M31" s="39" t="s">
-        <v>355</v>
-      </c>
-      <c r="AC31" s="39" t="s">
+      <c r="AC40" s="39" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" s="36" t="s">
+        <v>544</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="K41" s="39" t="s">
+        <v>591</v>
+      </c>
+      <c r="M41" s="39" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="J32" s="39" t="s">
-        <v>277</v>
-      </c>
-      <c r="M32" s="39" t="s">
-        <v>356</v>
-      </c>
-      <c r="AC32" s="39" t="s">
+      <c r="AC41" s="39" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" s="36" t="s">
+        <v>545</v>
+      </c>
+      <c r="E42" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="M42" s="39" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="J33" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="M33" s="39" t="s">
-        <v>357</v>
-      </c>
-      <c r="AC33" s="39" t="s">
+      <c r="AC42" s="39" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="D43" s="36" t="s">
+        <v>546</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>287</v>
+      </c>
+      <c r="M43" s="39" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="J34" s="39" t="s">
-        <v>279</v>
-      </c>
-      <c r="M34" s="39" t="s">
-        <v>358</v>
-      </c>
-      <c r="AC34" s="39" t="s">
+      <c r="AC43" s="39" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="D44" s="36" t="s">
+        <v>547</v>
+      </c>
+      <c r="E44" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="M44" s="39" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="J35" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="M35" s="39" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="J36" s="39" t="s">
-        <v>281</v>
-      </c>
-      <c r="M36" s="39" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="J37" s="39" t="s">
-        <v>282</v>
-      </c>
-      <c r="M37" s="39" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="J38" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="M38" s="39" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="J39" s="39" t="s">
-        <v>284</v>
-      </c>
-      <c r="M39" s="39" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="J40" s="39" t="s">
-        <v>285</v>
-      </c>
-      <c r="M40" s="39" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="M41" s="39" t="s">
-        <v>365</v>
+      <c r="AC44" s="39" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="D45" s="36" t="s">
+        <v>548</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>289</v>
+      </c>
+      <c r="M45" s="39" t="s">
+        <v>396</v>
+      </c>
+      <c r="AC45" s="39" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="D46" s="36" t="s">
+        <v>549</v>
+      </c>
+      <c r="E46" s="37" t="s">
+        <v>290</v>
+      </c>
+      <c r="M46" s="39" t="s">
+        <v>397</v>
+      </c>
+      <c r="AC46" s="39" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="D47" s="36" t="s">
+        <v>550</v>
+      </c>
+      <c r="E47" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="M47" s="39" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="D48" s="36" t="s">
+        <v>551</v>
+      </c>
+      <c r="E48" s="37" t="s">
+        <v>292</v>
+      </c>
+      <c r="M48" s="39" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="D49" s="36" t="s">
+        <v>552</v>
+      </c>
+      <c r="E49" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="M49" s="39" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="D50" s="36" t="s">
+        <v>553</v>
+      </c>
+      <c r="E50" s="37" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="D51" s="36" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="D52" s="36" t="s">
+        <v>555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
write names in range, lookups..
</commit_message>
<xml_diff>
--- a/X-Domestic Standard Upload.xlsx
+++ b/X-Domestic Standard Upload.xlsx
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="548">
   <si>
     <t>#</t>
   </si>
@@ -1240,45 +1240,6 @@
     <t>col:32</t>
   </si>
   <si>
-    <t>col:33</t>
-  </si>
-  <si>
-    <t>col:34</t>
-  </si>
-  <si>
-    <t>col:35</t>
-  </si>
-  <si>
-    <t>col:36</t>
-  </si>
-  <si>
-    <t>col:37</t>
-  </si>
-  <si>
-    <t>col:38</t>
-  </si>
-  <si>
-    <t>col:39</t>
-  </si>
-  <si>
-    <t>col:40</t>
-  </si>
-  <si>
-    <t>col:41</t>
-  </si>
-  <si>
-    <t>col:42</t>
-  </si>
-  <si>
-    <t>col:43</t>
-  </si>
-  <si>
-    <t>col:44</t>
-  </si>
-  <si>
-    <t>col:45</t>
-  </si>
-  <si>
     <t>dep:0</t>
   </si>
   <si>
@@ -1291,36 +1252,6 @@
     <t>dep:3</t>
   </si>
   <si>
-    <t>dep:4</t>
-  </si>
-  <si>
-    <t>dep:5</t>
-  </si>
-  <si>
-    <t>dep:6</t>
-  </si>
-  <si>
-    <t>dep:7</t>
-  </si>
-  <si>
-    <t>dep:8</t>
-  </si>
-  <si>
-    <t>dep:9</t>
-  </si>
-  <si>
-    <t>dep:10</t>
-  </si>
-  <si>
-    <t>dep:11</t>
-  </si>
-  <si>
-    <t>dep:12</t>
-  </si>
-  <si>
-    <t>dep:13</t>
-  </si>
-  <si>
     <t>siz:0</t>
   </si>
   <si>
@@ -1354,30 +1285,6 @@
     <t>siz:10</t>
   </si>
   <si>
-    <t>siz:11</t>
-  </si>
-  <si>
-    <t>siz:12</t>
-  </si>
-  <si>
-    <t>siz:13</t>
-  </si>
-  <si>
-    <t>siz:14</t>
-  </si>
-  <si>
-    <t>siz:15</t>
-  </si>
-  <si>
-    <t>siz:16</t>
-  </si>
-  <si>
-    <t>siz:17</t>
-  </si>
-  <si>
-    <t>siz:18</t>
-  </si>
-  <si>
     <t>typ:0</t>
   </si>
   <si>
@@ -1462,6 +1369,54 @@
     <t>typ:27</t>
   </si>
   <si>
+    <t>typ:28</t>
+  </si>
+  <si>
+    <t>typ:29</t>
+  </si>
+  <si>
+    <t>typ:30</t>
+  </si>
+  <si>
+    <t>typ:31</t>
+  </si>
+  <si>
+    <t>typ:32</t>
+  </si>
+  <si>
+    <t>typ:33</t>
+  </si>
+  <si>
+    <t>typ:34</t>
+  </si>
+  <si>
+    <t>typ:35</t>
+  </si>
+  <si>
+    <t>typ:36</t>
+  </si>
+  <si>
+    <t>typ:37</t>
+  </si>
+  <si>
+    <t>typ:38</t>
+  </si>
+  <si>
+    <t>typ:39</t>
+  </si>
+  <si>
+    <t>typ:40</t>
+  </si>
+  <si>
+    <t>typ:41</t>
+  </si>
+  <si>
+    <t>typ:42</t>
+  </si>
+  <si>
+    <t>typ:43</t>
+  </si>
+  <si>
     <t>mat:0</t>
   </si>
   <si>
@@ -1585,15 +1540,6 @@
     <t>mat:40</t>
   </si>
   <si>
-    <t>mat:41</t>
-  </si>
-  <si>
-    <t>mat:42</t>
-  </si>
-  <si>
-    <t>mat:43</t>
-  </si>
-  <si>
     <t>wei:0</t>
   </si>
   <si>
@@ -1735,12 +1681,51 @@
     <t>vpn:4</t>
   </si>
   <si>
+    <t>vpn:5</t>
+  </si>
+  <si>
+    <t>vpn:6</t>
+  </si>
+  <si>
+    <t>vpn:7</t>
+  </si>
+  <si>
+    <t>vpn:8</t>
+  </si>
+  <si>
+    <t>vpn:9</t>
+  </si>
+  <si>
+    <t>vpn:10</t>
+  </si>
+  <si>
+    <t>vpn:11</t>
+  </si>
+  <si>
+    <t>vpn:12</t>
+  </si>
+  <si>
+    <t>vpn:13</t>
+  </si>
+  <si>
+    <t>vpn:14</t>
+  </si>
+  <si>
+    <t>vpn:15</t>
+  </si>
+  <si>
+    <t>vpn:16</t>
+  </si>
+  <si>
     <t>sup:0</t>
   </si>
   <si>
     <t>sup:1</t>
   </si>
   <si>
+    <t>sup:2</t>
+  </si>
+  <si>
     <t>cat:0</t>
   </si>
   <si>
@@ -1819,6 +1804,21 @@
     <t>cat:25</t>
   </si>
   <si>
+    <t>cat:26</t>
+  </si>
+  <si>
+    <t>cat:27</t>
+  </si>
+  <si>
+    <t>cat:28</t>
+  </si>
+  <si>
+    <t>cat:29</t>
+  </si>
+  <si>
+    <t>cat:30</t>
+  </si>
+  <si>
     <t>ven:0</t>
   </si>
   <si>
@@ -1837,87 +1837,6 @@
     <t>ven:5</t>
   </si>
   <si>
-    <t>ven:6</t>
-  </si>
-  <si>
-    <t>ven:7</t>
-  </si>
-  <si>
-    <t>ven:8</t>
-  </si>
-  <si>
-    <t>ven:9</t>
-  </si>
-  <si>
-    <t>ven:10</t>
-  </si>
-  <si>
-    <t>ven:11</t>
-  </si>
-  <si>
-    <t>ven:12</t>
-  </si>
-  <si>
-    <t>ven:13</t>
-  </si>
-  <si>
-    <t>ven:14</t>
-  </si>
-  <si>
-    <t>ven:15</t>
-  </si>
-  <si>
-    <t>ven:16</t>
-  </si>
-  <si>
-    <t>ven:17</t>
-  </si>
-  <si>
-    <t>ven:18</t>
-  </si>
-  <si>
-    <t>ven:19</t>
-  </si>
-  <si>
-    <t>ven:20</t>
-  </si>
-  <si>
-    <t>ven:21</t>
-  </si>
-  <si>
-    <t>ven:22</t>
-  </si>
-  <si>
-    <t>ven:23</t>
-  </si>
-  <si>
-    <t>ven:24</t>
-  </si>
-  <si>
-    <t>ven:25</t>
-  </si>
-  <si>
-    <t>ven:26</t>
-  </si>
-  <si>
-    <t>ven:27</t>
-  </si>
-  <si>
-    <t>ven:28</t>
-  </si>
-  <si>
-    <t>ven:29</t>
-  </si>
-  <si>
-    <t>ven:30</t>
-  </si>
-  <si>
-    <t>ven:31</t>
-  </si>
-  <si>
-    <t>ven:32</t>
-  </si>
-  <si>
     <t>lab:0</t>
   </si>
   <si>
@@ -2008,57 +1927,6 @@
     <t>lab:29</t>
   </si>
   <si>
-    <t>lab:30</t>
-  </si>
-  <si>
-    <t>lab:31</t>
-  </si>
-  <si>
-    <t>lab:32</t>
-  </si>
-  <si>
-    <t>lab:33</t>
-  </si>
-  <si>
-    <t>lab:34</t>
-  </si>
-  <si>
-    <t>lab:35</t>
-  </si>
-  <si>
-    <t>lab:36</t>
-  </si>
-  <si>
-    <t>lab:37</t>
-  </si>
-  <si>
-    <t>lab:38</t>
-  </si>
-  <si>
-    <t>lab:39</t>
-  </si>
-  <si>
-    <t>lab:40</t>
-  </si>
-  <si>
-    <t>lab:41</t>
-  </si>
-  <si>
-    <t>lab:42</t>
-  </si>
-  <si>
-    <t>lab:43</t>
-  </si>
-  <si>
-    <t>lab:44</t>
-  </si>
-  <si>
-    <t>lab:45</t>
-  </si>
-  <si>
-    <t>lab:46</t>
-  </si>
-  <si>
     <t>cla:0</t>
   </si>
   <si>
@@ -2098,75 +1966,6 @@
     <t>cla:12</t>
   </si>
   <si>
-    <t>cla:13</t>
-  </si>
-  <si>
-    <t>cla:14</t>
-  </si>
-  <si>
-    <t>cla:15</t>
-  </si>
-  <si>
-    <t>cla:16</t>
-  </si>
-  <si>
-    <t>cla:17</t>
-  </si>
-  <si>
-    <t>cla:18</t>
-  </si>
-  <si>
-    <t>cla:19</t>
-  </si>
-  <si>
-    <t>cla:20</t>
-  </si>
-  <si>
-    <t>cla:21</t>
-  </si>
-  <si>
-    <t>cla:22</t>
-  </si>
-  <si>
-    <t>cla:23</t>
-  </si>
-  <si>
-    <t>cla:24</t>
-  </si>
-  <si>
-    <t>cla:25</t>
-  </si>
-  <si>
-    <t>cla:26</t>
-  </si>
-  <si>
-    <t>cla:27</t>
-  </si>
-  <si>
-    <t>cla:28</t>
-  </si>
-  <si>
-    <t>cla:29</t>
-  </si>
-  <si>
-    <t>cla:30</t>
-  </si>
-  <si>
-    <t>cla:31</t>
-  </si>
-  <si>
-    <t>cla:32</t>
-  </si>
-  <si>
-    <t>cla:33</t>
-  </si>
-  <si>
-    <t>cla:34</t>
-  </si>
-  <si>
-    <t>cla:35</t>
-  </si>
-  <si>
     <t>pon:0</t>
   </si>
   <si>
@@ -2186,6 +1985,54 @@
   </si>
   <si>
     <t>pon:6</t>
+  </si>
+  <si>
+    <t>pon:7</t>
+  </si>
+  <si>
+    <t>pon:8</t>
+  </si>
+  <si>
+    <t>pon:9</t>
+  </si>
+  <si>
+    <t>pon:10</t>
+  </si>
+  <si>
+    <t>pon:11</t>
+  </si>
+  <si>
+    <t>pon:12</t>
+  </si>
+  <si>
+    <t>pon:13</t>
+  </si>
+  <si>
+    <t>pon:14</t>
+  </si>
+  <si>
+    <t>pon:15</t>
+  </si>
+  <si>
+    <t>pon:16</t>
+  </si>
+  <si>
+    <t>pon:17</t>
+  </si>
+  <si>
+    <t>pon:18</t>
+  </si>
+  <si>
+    <t>pon:19</t>
+  </si>
+  <si>
+    <t>pon:20</t>
+  </si>
+  <si>
+    <t>pon:21</t>
+  </si>
+  <si>
+    <t>pon:22</t>
   </si>
 </sst>
 </file>
@@ -6642,7 +6489,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A17F3EB-F212-417F-BA00-A3FB97B2BF77}">
-  <dimension ref="A1:CV52"/>
+  <dimension ref="A1:CV49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
@@ -7948,7 +7795,7 @@
       <c r="AA5" s="50"/>
       <c r="AB5" s="50"/>
       <c r="AC5" s="39" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="AD5" s="50"/>
       <c r="AE5" s="50"/>
@@ -8024,1137 +7871,978 @@
     </row>
     <row r="6">
       <c r="B6" s="36" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="C6" s="36" t="s">
         <v>476</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>509</v>
+        <v>482</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>250</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>329</v>
+        <v>298</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>592</v>
+        <v>525</v>
       </c>
       <c r="I6" s="39" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="K6" s="39" t="s">
-        <v>556</v>
+        <v>512</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="M6" s="39" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="AC6" s="39" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="36" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="C7" s="36" t="s">
         <v>477</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>251</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>311</v>
+        <v>288</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>330</v>
+        <v>299</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>593</v>
+        <v>526</v>
       </c>
       <c r="I7" s="39" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>557</v>
+        <v>513</v>
       </c>
       <c r="L7" s="39" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="M7" s="39" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="AC7" s="39" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="36" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="C8" s="36" t="s">
         <v>478</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>511</v>
+        <v>484</v>
       </c>
       <c r="E8" s="37" t="s">
         <v>252</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>331</v>
+        <v>300</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>594</v>
+        <v>527</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>444</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>558</v>
+        <v>514</v>
       </c>
       <c r="L8" s="39" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="M8" s="39" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="AC8" s="39" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="36" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>479</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>512</v>
+        <v>485</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>253</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>313</v>
+        <v>290</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>332</v>
+        <v>301</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>595</v>
+        <v>528</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="K9" s="39" t="s">
-        <v>559</v>
+        <v>515</v>
       </c>
       <c r="L9" s="39" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="M9" s="39" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="AC9" s="39" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="36" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="C10" s="36" t="s">
         <v>480</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>513</v>
+        <v>486</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>254</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>333</v>
+        <v>302</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>596</v>
-      </c>
-      <c r="J10" s="39" t="s">
-        <v>300</v>
+        <v>529</v>
       </c>
       <c r="K10" s="39" t="s">
-        <v>560</v>
+        <v>516</v>
       </c>
       <c r="L10" s="39" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="M10" s="39" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="AC10" s="39" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11">
+      <c r="B11" s="36" t="s">
+        <v>430</v>
+      </c>
       <c r="C11" s="36" t="s">
         <v>481</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>255</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>334</v>
+        <v>303</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>597</v>
-      </c>
-      <c r="J11" s="39" t="s">
-        <v>301</v>
+        <v>530</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>561</v>
+        <v>517</v>
       </c>
       <c r="L11" s="39" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="M11" s="39" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="AC11" s="39" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12">
-      <c r="C12" s="36" t="s">
-        <v>482</v>
+      <c r="B12" s="36" t="s">
+        <v>431</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>256</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>335</v>
+        <v>304</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>598</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>302</v>
+        <v>531</v>
       </c>
       <c r="K12" s="39" t="s">
-        <v>562</v>
+        <v>518</v>
       </c>
       <c r="L12" s="39" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="M12" s="39" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="AC12" s="39" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13">
-      <c r="C13" s="36" t="s">
-        <v>483</v>
+      <c r="B13" s="36" t="s">
+        <v>432</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>516</v>
+        <v>489</v>
       </c>
       <c r="E13" s="37" t="s">
         <v>257</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
       <c r="G13" s="38" t="s">
-        <v>336</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>303</v>
+        <v>305</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>532</v>
       </c>
       <c r="K13" s="39" t="s">
-        <v>563</v>
+        <v>519</v>
       </c>
       <c r="L13" s="39" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="M13" s="39" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="AC13" s="39" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="36" t="s">
-        <v>484</v>
+      <c r="B14" s="36" t="s">
+        <v>433</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="E14" s="37" t="s">
         <v>258</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>337</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>304</v>
+        <v>306</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>533</v>
       </c>
       <c r="K14" s="39" t="s">
-        <v>564</v>
+        <v>520</v>
       </c>
       <c r="L14" s="39" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="M14" s="39" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="AC14" s="39" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15">
-      <c r="C15" s="36" t="s">
-        <v>485</v>
+      <c r="B15" s="36" t="s">
+        <v>434</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>518</v>
+        <v>491</v>
       </c>
       <c r="E15" s="37" t="s">
         <v>259</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>338</v>
-      </c>
-      <c r="J15" s="39" t="s">
-        <v>305</v>
+        <v>307</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>534</v>
       </c>
       <c r="K15" s="39" t="s">
-        <v>565</v>
+        <v>521</v>
       </c>
       <c r="L15" s="39" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="M15" s="39" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="AC15" s="39" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16">
-      <c r="C16" s="36" t="s">
-        <v>486</v>
+      <c r="B16" s="36" t="s">
+        <v>435</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="E16" s="37" t="s">
         <v>260</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="G16" s="38" t="s">
-        <v>339</v>
-      </c>
-      <c r="J16" s="39" t="s">
-        <v>306</v>
+        <v>308</v>
+      </c>
+      <c r="H16" s="40" t="s">
+        <v>535</v>
       </c>
       <c r="K16" s="39" t="s">
-        <v>566</v>
+        <v>522</v>
       </c>
       <c r="L16" s="39" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="M16" s="39" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="AC16" s="39" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
     </row>
     <row r="17">
-      <c r="C17" s="36" t="s">
-        <v>487</v>
+      <c r="B17" s="36" t="s">
+        <v>436</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>520</v>
+        <v>493</v>
       </c>
       <c r="E17" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="F17" s="37" t="s">
-        <v>321</v>
-      </c>
       <c r="G17" s="38" t="s">
-        <v>340</v>
-      </c>
-      <c r="J17" s="39" t="s">
-        <v>307</v>
+        <v>309</v>
+      </c>
+      <c r="H17" s="40" t="s">
+        <v>536</v>
       </c>
       <c r="K17" s="39" t="s">
-        <v>567</v>
+        <v>523</v>
       </c>
       <c r="L17" s="39" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="M17" s="39" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="AC17" s="39" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18">
-      <c r="C18" s="36" t="s">
-        <v>488</v>
+      <c r="B18" s="36" t="s">
+        <v>437</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>521</v>
+        <v>494</v>
       </c>
       <c r="E18" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="F18" s="37" t="s">
-        <v>322</v>
-      </c>
       <c r="G18" s="38" t="s">
-        <v>341</v>
-      </c>
-      <c r="J18" s="39" t="s">
-        <v>308</v>
+        <v>310</v>
+      </c>
+      <c r="H18" s="40" t="s">
+        <v>537</v>
       </c>
       <c r="K18" s="39" t="s">
-        <v>568</v>
+        <v>524</v>
       </c>
       <c r="L18" s="39" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="M18" s="39" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="AC18" s="39" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
     </row>
     <row r="19">
-      <c r="C19" s="36" t="s">
-        <v>489</v>
+      <c r="B19" s="36" t="s">
+        <v>438</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="E19" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="F19" s="37" t="s">
-        <v>323</v>
-      </c>
       <c r="G19" s="38" t="s">
-        <v>342</v>
-      </c>
-      <c r="J19" s="39" t="s">
-        <v>309</v>
-      </c>
-      <c r="K19" s="39" t="s">
-        <v>569</v>
+        <v>311</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>538</v>
       </c>
       <c r="L19" s="39" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="M19" s="39" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="AC19" s="39" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
     </row>
     <row r="20">
-      <c r="C20" s="36" t="s">
-        <v>490</v>
+      <c r="B20" s="36" t="s">
+        <v>439</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>523</v>
+        <v>496</v>
       </c>
       <c r="E20" s="37" t="s">
         <v>264</v>
       </c>
-      <c r="F20" s="37" t="s">
-        <v>324</v>
-      </c>
       <c r="G20" s="38" t="s">
-        <v>343</v>
-      </c>
-      <c r="K20" s="39" t="s">
-        <v>570</v>
+        <v>312</v>
+      </c>
+      <c r="H20" s="40" t="s">
+        <v>539</v>
       </c>
       <c r="L20" s="39" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="M20" s="39" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="AC20" s="39" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="36" t="s">
-        <v>491</v>
+      <c r="B21" s="36" t="s">
+        <v>440</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="E21" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="F21" s="37" t="s">
-        <v>325</v>
-      </c>
       <c r="G21" s="38" t="s">
-        <v>344</v>
-      </c>
-      <c r="K21" s="39" t="s">
-        <v>571</v>
+        <v>313</v>
+      </c>
+      <c r="H21" s="40" t="s">
+        <v>540</v>
       </c>
       <c r="L21" s="39" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="M21" s="39" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="AC21" s="39" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22">
-      <c r="C22" s="36" t="s">
-        <v>492</v>
+      <c r="B22" s="36" t="s">
+        <v>441</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>525</v>
+        <v>498</v>
       </c>
       <c r="E22" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="F22" s="37" t="s">
-        <v>326</v>
-      </c>
       <c r="G22" s="38" t="s">
-        <v>345</v>
-      </c>
-      <c r="K22" s="39" t="s">
-        <v>572</v>
+        <v>314</v>
+      </c>
+      <c r="H22" s="40" t="s">
+        <v>541</v>
       </c>
       <c r="L22" s="39" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="M22" s="39" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="AC22" s="39" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
     </row>
     <row r="23">
-      <c r="C23" s="36" t="s">
-        <v>493</v>
-      </c>
       <c r="D23" s="36" t="s">
-        <v>526</v>
+        <v>499</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>267</v>
       </c>
-      <c r="F23" s="37" t="s">
-        <v>327</v>
-      </c>
       <c r="G23" s="38" t="s">
-        <v>346</v>
-      </c>
-      <c r="K23" s="39" t="s">
-        <v>573</v>
+        <v>315</v>
+      </c>
+      <c r="H23" s="40" t="s">
+        <v>542</v>
       </c>
       <c r="L23" s="39" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="M23" s="39" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="AC23" s="39" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24">
-      <c r="C24" s="36" t="s">
-        <v>494</v>
-      </c>
       <c r="D24" s="36" t="s">
-        <v>527</v>
+        <v>500</v>
       </c>
       <c r="E24" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="F24" s="37" t="s">
-        <v>328</v>
-      </c>
       <c r="G24" s="38" t="s">
-        <v>347</v>
-      </c>
-      <c r="K24" s="39" t="s">
-        <v>574</v>
+        <v>316</v>
+      </c>
+      <c r="H24" s="40" t="s">
+        <v>543</v>
       </c>
       <c r="L24" s="39" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="M24" s="39" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="AC24" s="39" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
     </row>
     <row r="25">
-      <c r="C25" s="36" t="s">
-        <v>495</v>
-      </c>
       <c r="D25" s="36" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="E25" s="37" t="s">
         <v>269</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>348</v>
-      </c>
-      <c r="K25" s="39" t="s">
-        <v>575</v>
+        <v>317</v>
+      </c>
+      <c r="H25" s="40" t="s">
+        <v>544</v>
       </c>
       <c r="L25" s="39" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="M25" s="39" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="AC25" s="39" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
     </row>
     <row r="26">
-      <c r="C26" s="36" t="s">
-        <v>496</v>
-      </c>
       <c r="D26" s="36" t="s">
-        <v>529</v>
+        <v>502</v>
       </c>
       <c r="E26" s="37" t="s">
         <v>270</v>
       </c>
       <c r="G26" s="38" t="s">
-        <v>349</v>
-      </c>
-      <c r="K26" s="39" t="s">
-        <v>576</v>
+        <v>318</v>
+      </c>
+      <c r="H26" s="40" t="s">
+        <v>545</v>
       </c>
       <c r="L26" s="39" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="M26" s="39" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="AC26" s="39" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
     </row>
     <row r="27">
-      <c r="C27" s="36" t="s">
-        <v>497</v>
-      </c>
       <c r="D27" s="36" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="E27" s="37" t="s">
         <v>271</v>
       </c>
       <c r="G27" s="38" t="s">
-        <v>350</v>
-      </c>
-      <c r="K27" s="39" t="s">
-        <v>577</v>
+        <v>319</v>
+      </c>
+      <c r="H27" s="40" t="s">
+        <v>546</v>
       </c>
       <c r="L27" s="39" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="M27" s="39" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="AC27" s="39" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
     </row>
     <row r="28">
-      <c r="C28" s="36" t="s">
-        <v>498</v>
-      </c>
       <c r="D28" s="36" t="s">
-        <v>531</v>
+        <v>504</v>
       </c>
       <c r="E28" s="37" t="s">
         <v>272</v>
       </c>
       <c r="G28" s="38" t="s">
-        <v>351</v>
-      </c>
-      <c r="K28" s="39" t="s">
-        <v>578</v>
+        <v>320</v>
+      </c>
+      <c r="H28" s="40" t="s">
+        <v>547</v>
       </c>
       <c r="L28" s="39" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="M28" s="39" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="AC28" s="39" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="36" t="s">
-        <v>499</v>
-      </c>
       <c r="D29" s="36" t="s">
-        <v>532</v>
+        <v>505</v>
       </c>
       <c r="E29" s="37" t="s">
         <v>273</v>
       </c>
       <c r="G29" s="38" t="s">
-        <v>352</v>
-      </c>
-      <c r="K29" s="39" t="s">
-        <v>579</v>
+        <v>321</v>
       </c>
       <c r="L29" s="39" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="M29" s="39" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
       <c r="AC29" s="39" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="36" t="s">
-        <v>500</v>
-      </c>
       <c r="D30" s="36" t="s">
-        <v>533</v>
+        <v>506</v>
       </c>
       <c r="E30" s="37" t="s">
         <v>274</v>
       </c>
       <c r="G30" s="38" t="s">
-        <v>353</v>
-      </c>
-      <c r="K30" s="39" t="s">
-        <v>580</v>
+        <v>322</v>
       </c>
       <c r="L30" s="39" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="M30" s="39" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="AC30" s="39" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
     </row>
     <row r="31">
-      <c r="C31" s="36" t="s">
-        <v>501</v>
-      </c>
       <c r="D31" s="36" t="s">
-        <v>534</v>
+        <v>507</v>
       </c>
       <c r="E31" s="37" t="s">
         <v>275</v>
       </c>
       <c r="G31" s="38" t="s">
-        <v>354</v>
-      </c>
-      <c r="K31" s="39" t="s">
-        <v>581</v>
+        <v>323</v>
       </c>
       <c r="L31" s="39" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="M31" s="39" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="AC31" s="39" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
     </row>
     <row r="32">
-      <c r="C32" s="36" t="s">
-        <v>502</v>
-      </c>
       <c r="D32" s="36" t="s">
-        <v>535</v>
+        <v>508</v>
       </c>
       <c r="E32" s="37" t="s">
         <v>276</v>
       </c>
       <c r="G32" s="38" t="s">
-        <v>355</v>
-      </c>
-      <c r="K32" s="39" t="s">
-        <v>582</v>
+        <v>324</v>
+      </c>
+      <c r="L32" s="39" t="s">
+        <v>471</v>
       </c>
       <c r="M32" s="39" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="AC32" s="39" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
     </row>
     <row r="33">
-      <c r="C33" s="36" t="s">
-        <v>503</v>
-      </c>
       <c r="D33" s="36" t="s">
-        <v>536</v>
+        <v>509</v>
       </c>
       <c r="E33" s="37" t="s">
         <v>277</v>
       </c>
       <c r="G33" s="38" t="s">
-        <v>356</v>
-      </c>
-      <c r="K33" s="39" t="s">
-        <v>583</v>
+        <v>325</v>
+      </c>
+      <c r="L33" s="39" t="s">
+        <v>472</v>
       </c>
       <c r="M33" s="39" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="AC33" s="39" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
     </row>
     <row r="34">
-      <c r="C34" s="36" t="s">
-        <v>504</v>
-      </c>
       <c r="D34" s="36" t="s">
-        <v>537</v>
+        <v>510</v>
       </c>
       <c r="E34" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="K34" s="39" t="s">
-        <v>584</v>
+      <c r="G34" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="L34" s="39" t="s">
+        <v>473</v>
       </c>
       <c r="M34" s="39" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="AC34" s="39" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
     </row>
     <row r="35">
-      <c r="C35" s="36" t="s">
-        <v>505</v>
-      </c>
       <c r="D35" s="36" t="s">
-        <v>538</v>
+        <v>511</v>
       </c>
       <c r="E35" s="37" t="s">
         <v>279</v>
       </c>
-      <c r="K35" s="39" t="s">
-        <v>585</v>
+      <c r="G35" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="L35" s="39" t="s">
+        <v>474</v>
       </c>
       <c r="M35" s="39" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="AC35" s="39" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
     </row>
     <row r="36">
-      <c r="C36" s="36" t="s">
-        <v>506</v>
-      </c>
-      <c r="D36" s="36" t="s">
-        <v>539</v>
-      </c>
       <c r="E36" s="37" t="s">
         <v>280</v>
       </c>
-      <c r="K36" s="39" t="s">
-        <v>586</v>
+      <c r="G36" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="L36" s="39" t="s">
+        <v>475</v>
       </c>
       <c r="M36" s="39" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="AC36" s="39" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
     </row>
     <row r="37">
-      <c r="C37" s="36" t="s">
-        <v>507</v>
-      </c>
-      <c r="D37" s="36" t="s">
-        <v>540</v>
-      </c>
       <c r="E37" s="37" t="s">
         <v>281</v>
       </c>
-      <c r="K37" s="39" t="s">
-        <v>587</v>
+      <c r="G37" s="38" t="s">
+        <v>329</v>
       </c>
       <c r="M37" s="39" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="AC37" s="39" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
     </row>
     <row r="38">
-      <c r="C38" s="36" t="s">
-        <v>508</v>
-      </c>
-      <c r="D38" s="36" t="s">
-        <v>541</v>
-      </c>
-      <c r="E38" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="K38" s="39" t="s">
-        <v>588</v>
+      <c r="G38" s="38" t="s">
+        <v>330</v>
       </c>
       <c r="M38" s="39" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="AC38" s="39" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
     </row>
     <row r="39">
-      <c r="D39" s="36" t="s">
-        <v>542</v>
-      </c>
-      <c r="E39" s="37" t="s">
-        <v>283</v>
-      </c>
-      <c r="K39" s="39" t="s">
-        <v>589</v>
+      <c r="G39" s="38" t="s">
+        <v>331</v>
       </c>
       <c r="M39" s="39" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="AC39" s="39" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
     </row>
     <row r="40">
-      <c r="D40" s="36" t="s">
-        <v>543</v>
-      </c>
-      <c r="E40" s="37" t="s">
-        <v>284</v>
-      </c>
-      <c r="K40" s="39" t="s">
-        <v>590</v>
+      <c r="G40" s="38" t="s">
+        <v>332</v>
       </c>
       <c r="M40" s="39" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="AC40" s="39" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
     </row>
     <row r="41">
-      <c r="D41" s="36" t="s">
-        <v>544</v>
-      </c>
-      <c r="E41" s="37" t="s">
-        <v>285</v>
-      </c>
-      <c r="K41" s="39" t="s">
-        <v>591</v>
+      <c r="G41" s="38" t="s">
+        <v>333</v>
       </c>
       <c r="M41" s="39" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="AC41" s="39" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
     </row>
     <row r="42">
-      <c r="D42" s="36" t="s">
-        <v>545</v>
-      </c>
-      <c r="E42" s="37" t="s">
-        <v>286</v>
+      <c r="G42" s="38" t="s">
+        <v>334</v>
       </c>
       <c r="M42" s="39" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="AC42" s="39" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
     </row>
     <row r="43">
-      <c r="D43" s="36" t="s">
-        <v>546</v>
-      </c>
-      <c r="E43" s="37" t="s">
-        <v>287</v>
+      <c r="G43" s="38" t="s">
+        <v>335</v>
       </c>
       <c r="M43" s="39" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="AC43" s="39" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
     </row>
     <row r="44">
-      <c r="D44" s="36" t="s">
-        <v>547</v>
-      </c>
-      <c r="E44" s="37" t="s">
-        <v>288</v>
+      <c r="G44" s="38" t="s">
+        <v>336</v>
       </c>
       <c r="M44" s="39" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="AC44" s="39" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
     </row>
     <row r="45">
-      <c r="D45" s="36" t="s">
-        <v>548</v>
-      </c>
-      <c r="E45" s="37" t="s">
-        <v>289</v>
+      <c r="G45" s="38" t="s">
+        <v>337</v>
       </c>
       <c r="M45" s="39" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="AC45" s="39" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
     </row>
     <row r="46">
-      <c r="D46" s="36" t="s">
-        <v>549</v>
-      </c>
-      <c r="E46" s="37" t="s">
-        <v>290</v>
+      <c r="G46" s="38" t="s">
+        <v>338</v>
       </c>
       <c r="M46" s="39" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="AC46" s="39" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
     </row>
     <row r="47">
-      <c r="D47" s="36" t="s">
-        <v>550</v>
-      </c>
-      <c r="E47" s="37" t="s">
-        <v>291</v>
-      </c>
-      <c r="M47" s="39" t="s">
-        <v>398</v>
+      <c r="G47" s="38" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="48">
-      <c r="D48" s="36" t="s">
-        <v>551</v>
-      </c>
-      <c r="E48" s="37" t="s">
-        <v>292</v>
-      </c>
-      <c r="M48" s="39" t="s">
-        <v>399</v>
+      <c r="G48" s="38" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="49">
-      <c r="D49" s="36" t="s">
-        <v>552</v>
-      </c>
-      <c r="E49" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="M49" s="39" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="D50" s="36" t="s">
-        <v>553</v>
-      </c>
-      <c r="E50" s="37" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="D51" s="36" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="D52" s="36" t="s">
-        <v>555</v>
+      <c r="G49" s="38" t="s">
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>